<commit_message>
doc: atualizar planejamento de sprint
</commit_message>
<xml_diff>
--- a/Artefatos/sprints/Planejamento_sprints.xlsx
+++ b/Artefatos/sprints/Planejamento_sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\repositories\plf-es-2023-2-ti3-6653100-fabrica-do-saber\Artefatos\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96081C18-A71B-4F02-899A-03A9B9AD35A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9922CF-AF07-47FB-B047-AEEEB2406E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,35 +1320,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1358,19 +1339,56 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1387,15 +1405,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1404,15 +1413,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3239,166 +3239,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="76" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="77"/>
-      <c r="H10" s="78"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="76" t="s">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="78"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="76" t="s">
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="78"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69"/>
       <c r="K12" s="47"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="76" t="s">
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="77"/>
-      <c r="H13" s="78"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="76" t="s">
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="78"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="76" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="77"/>
-      <c r="H15" s="78"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="18"/>
@@ -3500,16 +3500,16 @@
     <row r="99" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="50"/>
-      <c r="B100" s="80"/>
-      <c r="C100" s="65"/>
-      <c r="D100" s="81" t="s">
+      <c r="B100" s="70"/>
+      <c r="C100" s="62"/>
+      <c r="D100" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="E100" s="65"/>
-      <c r="F100" s="81" t="s">
+      <c r="E100" s="62"/>
+      <c r="F100" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="G100" s="65"/>
+      <c r="G100" s="62"/>
       <c r="H100" s="51" t="s">
         <v>18</v>
       </c>
@@ -3531,12 +3531,12 @@
     </row>
     <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
-      <c r="B101" s="83"/>
-      <c r="C101" s="65"/>
-      <c r="D101" s="82" t="s">
+      <c r="B101" s="61"/>
+      <c r="C101" s="62"/>
+      <c r="D101" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="65"/>
+      <c r="E101" s="62"/>
       <c r="F101" s="53" t="s">
         <v>24</v>
       </c>
@@ -3569,12 +3569,12 @@
     </row>
     <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
-      <c r="B102" s="83"/>
-      <c r="C102" s="65"/>
-      <c r="D102" s="82" t="s">
+      <c r="B102" s="61"/>
+      <c r="C102" s="62"/>
+      <c r="D102" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="E102" s="65"/>
+      <c r="E102" s="62"/>
       <c r="F102" s="53" t="s">
         <v>29</v>
       </c>
@@ -3608,12 +3608,12 @@
     </row>
     <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="50"/>
-      <c r="B103" s="83"/>
-      <c r="C103" s="65"/>
-      <c r="D103" s="82" t="s">
+      <c r="B103" s="61"/>
+      <c r="C103" s="62"/>
+      <c r="D103" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="65"/>
+      <c r="E103" s="62"/>
       <c r="F103" s="53"/>
       <c r="G103" s="54" t="s">
         <v>34</v>
@@ -3645,12 +3645,12 @@
     </row>
     <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="50"/>
-      <c r="B104" s="83"/>
-      <c r="C104" s="65"/>
-      <c r="D104" s="82" t="s">
+      <c r="B104" s="61"/>
+      <c r="C104" s="62"/>
+      <c r="D104" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="65"/>
+      <c r="E104" s="62"/>
       <c r="F104" s="53"/>
       <c r="G104" s="54" t="s">
         <v>36</v>
@@ -3680,12 +3680,12 @@
     </row>
     <row r="105" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="50"/>
-      <c r="B105" s="83"/>
-      <c r="C105" s="65"/>
-      <c r="D105" s="82" t="s">
+      <c r="B105" s="61"/>
+      <c r="C105" s="62"/>
+      <c r="D105" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E105" s="65"/>
+      <c r="E105" s="62"/>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="s">
         <v>39</v>
@@ -3710,8 +3710,8 @@
     </row>
     <row r="106" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="50"/>
-      <c r="B106" s="83"/>
-      <c r="C106" s="65"/>
+      <c r="B106" s="61"/>
+      <c r="C106" s="62"/>
       <c r="F106" s="53"/>
       <c r="G106" s="54"/>
       <c r="H106" s="53"/>
@@ -3722,8 +3722,8 @@
     </row>
     <row r="107" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="50"/>
-      <c r="B107" s="83"/>
-      <c r="C107" s="65"/>
+      <c r="B107" s="61"/>
+      <c r="C107" s="62"/>
       <c r="D107" s="55"/>
       <c r="E107" s="53"/>
       <c r="F107" s="53"/>
@@ -4691,12 +4691,24 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B100:C100"/>
     <mergeCell ref="D100:E100"/>
@@ -4708,24 +4720,12 @@
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D105:E105"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="F10:F15" xr:uid="{49EDF03A-7EFB-435C-A992-40D98DE85B41}">
@@ -4768,59 +4768,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -4832,16 +4832,16 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="93" t="str">
+      <c r="B7" s="96" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -4853,15 +4853,15 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
@@ -4873,11 +4873,11 @@
       <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="73"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
       <c r="H10" s="6" t="s">
         <v>45</v>
       </c>
@@ -4892,9 +4892,9 @@
       <c r="D11" s="14">
         <v>45190</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="73"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4908,9 +4908,9 @@
         <f t="shared" ref="D12" si="0">C12+13</f>
         <v>45204</v>
       </c>
-      <c r="E12" s="85"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4924,9 +4924,9 @@
       <c r="D13" s="14">
         <v>45225</v>
       </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="73"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="65"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4939,9 +4939,9 @@
       <c r="D14" s="14">
         <v>45246</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4980,13 +4980,13 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="22" t="s">
         <v>47</v>
       </c>
@@ -4995,11 +4995,11 @@
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="88"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="73"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="25" t="s">
         <v>48</v>
       </c>
@@ -5009,11 +5009,11 @@
       <c r="B20" s="27">
         <v>0</v>
       </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="73"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="28"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -5030,13 +5030,13 @@
       <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="90" t="s">
+      <c r="C21" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="92"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="90"/>
       <c r="H21" s="12" t="s">
         <v>52</v>
       </c>
@@ -5046,13 +5046,13 @@
       <c r="B22" s="27">
         <v>2</v>
       </c>
-      <c r="C22" s="90" t="s">
+      <c r="C22" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="92"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="12" t="s">
         <v>49</v>
       </c>
@@ -5061,13 +5061,13 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="90" t="s">
+      <c r="C23" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="92"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="90"/>
       <c r="H23" s="12" t="s">
         <v>49</v>
       </c>
@@ -5076,13 +5076,13 @@
       <c r="B24" s="27">
         <v>4</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="98"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="87"/>
       <c r="H24" s="12" t="s">
         <v>49</v>
       </c>
@@ -5091,13 +5091,13 @@
       <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="96" t="s">
+      <c r="C25" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="98"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="87"/>
       <c r="H25" s="12" t="s">
         <v>49</v>
       </c>
@@ -5106,13 +5106,13 @@
       <c r="B26" s="27">
         <v>6</v>
       </c>
-      <c r="C26" s="96" t="s">
+      <c r="C26" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="98"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
       <c r="H26" s="12" t="s">
         <v>49</v>
       </c>
@@ -5121,13 +5121,13 @@
       <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="96" t="s">
+      <c r="C27" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="98"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="87"/>
       <c r="H27" s="12" t="s">
         <v>49</v>
       </c>
@@ -5136,13 +5136,13 @@
       <c r="B28" s="27">
         <v>8</v>
       </c>
-      <c r="C28" s="96" t="s">
+      <c r="C28" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="98"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="87"/>
       <c r="H28" s="12" t="s">
         <v>49</v>
       </c>
@@ -5151,13 +5151,13 @@
       <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="C29" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="98"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="87"/>
       <c r="H29" s="12" t="s">
         <v>49</v>
       </c>
@@ -5166,13 +5166,13 @@
       <c r="B30" s="27">
         <v>10</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C30" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="97"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="98"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="87"/>
       <c r="H30" s="12" t="s">
         <v>49</v>
       </c>
@@ -5181,13 +5181,13 @@
       <c r="B31" s="9">
         <v>11</v>
       </c>
-      <c r="C31" s="96" t="s">
+      <c r="C31" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="98"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="87"/>
       <c r="H31" s="12" t="s">
         <v>49</v>
       </c>
@@ -5196,13 +5196,13 @@
       <c r="B32" s="27">
         <v>12</v>
       </c>
-      <c r="C32" s="96" t="s">
+      <c r="C32" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="98"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="87"/>
       <c r="H32" s="12" t="s">
         <v>52</v>
       </c>
@@ -5211,13 +5211,13 @@
       <c r="B33" s="9">
         <v>13</v>
       </c>
-      <c r="C33" s="90" t="s">
+      <c r="C33" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="92"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="90"/>
       <c r="H33" s="12" t="s">
         <v>52</v>
       </c>
@@ -5226,11 +5226,11 @@
       <c r="B34" s="27">
         <v>14</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="97"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="87"/>
       <c r="H34" s="12" t="s">
         <v>49</v>
       </c>
@@ -5239,11 +5239,11 @@
       <c r="B35" s="9">
         <v>15</v>
       </c>
-      <c r="C35" s="96"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="98"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
       <c r="H35" s="12" t="s">
         <v>49</v>
       </c>
@@ -5252,11 +5252,11 @@
       <c r="B36" s="27">
         <v>16</v>
       </c>
-      <c r="C36" s="96"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="73"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="65"/>
       <c r="H36" s="12" t="s">
         <v>49</v>
       </c>
@@ -5265,11 +5265,11 @@
       <c r="B37" s="9">
         <v>17</v>
       </c>
-      <c r="C37" s="96"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="65"/>
       <c r="H37" s="12" t="s">
         <v>49</v>
       </c>
@@ -5278,11 +5278,11 @@
       <c r="B38" s="27">
         <v>18</v>
       </c>
-      <c r="C38" s="96"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="73"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="12" t="s">
         <v>49</v>
       </c>
@@ -5291,11 +5291,11 @@
       <c r="B39" s="9">
         <v>19</v>
       </c>
-      <c r="C39" s="96"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="73"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="65"/>
       <c r="H39" s="12" t="s">
         <v>49</v>
       </c>
@@ -5304,11 +5304,11 @@
       <c r="B40" s="27">
         <v>20</v>
       </c>
-      <c r="C40" s="96"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="73"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="65"/>
       <c r="H40" s="12" t="s">
         <v>49</v>
       </c>
@@ -5317,11 +5317,11 @@
       <c r="B41" s="9">
         <v>21</v>
       </c>
-      <c r="C41" s="96"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="73"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="12" t="s">
         <v>49</v>
       </c>
@@ -5330,11 +5330,11 @@
       <c r="B42" s="27">
         <v>22</v>
       </c>
-      <c r="C42" s="96"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="73"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="65"/>
       <c r="H42" s="12" t="s">
         <v>49</v>
       </c>
@@ -5343,11 +5343,11 @@
       <c r="B43" s="9">
         <v>23</v>
       </c>
-      <c r="C43" s="96"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="73"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="65"/>
       <c r="H43" s="12" t="s">
         <v>49</v>
       </c>
@@ -5356,11 +5356,11 @@
       <c r="B44" s="27">
         <v>24</v>
       </c>
-      <c r="C44" s="96"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="73"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
       <c r="H44" s="12" t="s">
         <v>49</v>
       </c>
@@ -5369,11 +5369,11 @@
       <c r="B45" s="9">
         <v>25</v>
       </c>
-      <c r="C45" s="96"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="73"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="65"/>
       <c r="H45" s="12" t="s">
         <v>49</v>
       </c>
@@ -5382,11 +5382,11 @@
       <c r="B46" s="27">
         <v>26</v>
       </c>
-      <c r="C46" s="96"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="73"/>
+      <c r="C46" s="85"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="65"/>
       <c r="H46" s="12" t="s">
         <v>49</v>
       </c>
@@ -5395,11 +5395,11 @@
       <c r="B47" s="9">
         <v>27</v>
       </c>
-      <c r="C47" s="96"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="73"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="65"/>
       <c r="H47" s="12" t="s">
         <v>49</v>
       </c>
@@ -5408,11 +5408,11 @@
       <c r="B48" s="27">
         <v>28</v>
       </c>
-      <c r="C48" s="96"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="72"/>
-      <c r="G48" s="73"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="65"/>
       <c r="H48" s="12" t="s">
         <v>49</v>
       </c>
@@ -5421,11 +5421,11 @@
       <c r="B49" s="9">
         <v>29</v>
       </c>
-      <c r="C49" s="96"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="73"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="65"/>
       <c r="H49" s="12" t="s">
         <v>49</v>
       </c>
@@ -5434,11 +5434,11 @@
       <c r="B50" s="27">
         <v>30</v>
       </c>
-      <c r="C50" s="96"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="72"/>
-      <c r="G50" s="73"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="65"/>
       <c r="H50" s="12" t="s">
         <v>49</v>
       </c>
@@ -5447,11 +5447,11 @@
       <c r="B51" s="9">
         <v>31</v>
       </c>
-      <c r="C51" s="96"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="73"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="65"/>
       <c r="H51" s="12" t="s">
         <v>49</v>
       </c>
@@ -5460,11 +5460,11 @@
       <c r="B52" s="27">
         <v>32</v>
       </c>
-      <c r="C52" s="96"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="73"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="65"/>
       <c r="H52" s="12" t="s">
         <v>49</v>
       </c>
@@ -5473,11 +5473,11 @@
       <c r="B53" s="9">
         <v>33</v>
       </c>
-      <c r="C53" s="96"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="73"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="65"/>
       <c r="H53" s="12" t="s">
         <v>49</v>
       </c>
@@ -5486,11 +5486,11 @@
       <c r="B54" s="27">
         <v>34</v>
       </c>
-      <c r="C54" s="96"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="73"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="65"/>
       <c r="H54" s="12" t="s">
         <v>49</v>
       </c>
@@ -5499,11 +5499,11 @@
       <c r="B55" s="9">
         <v>35</v>
       </c>
-      <c r="C55" s="96"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="72"/>
-      <c r="F55" s="72"/>
-      <c r="G55" s="73"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="64"/>
+      <c r="E55" s="64"/>
+      <c r="F55" s="64"/>
+      <c r="G55" s="65"/>
       <c r="H55" s="12" t="s">
         <v>49</v>
       </c>
@@ -5512,11 +5512,11 @@
       <c r="B56" s="27">
         <v>36</v>
       </c>
-      <c r="C56" s="96"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="73"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="65"/>
       <c r="H56" s="12" t="s">
         <v>49</v>
       </c>
@@ -5525,11 +5525,11 @@
       <c r="B57" s="9">
         <v>37</v>
       </c>
-      <c r="C57" s="96"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="73"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="65"/>
       <c r="H57" s="12" t="s">
         <v>49</v>
       </c>
@@ -5538,11 +5538,11 @@
       <c r="B58" s="27">
         <v>38</v>
       </c>
-      <c r="C58" s="96"/>
-      <c r="D58" s="72"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
-      <c r="G58" s="73"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="65"/>
       <c r="H58" s="12" t="s">
         <v>49</v>
       </c>
@@ -5551,11 +5551,11 @@
       <c r="B59" s="9">
         <v>39</v>
       </c>
-      <c r="C59" s="96"/>
-      <c r="D59" s="72"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="73"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="65"/>
       <c r="H59" s="12" t="s">
         <v>49</v>
       </c>
@@ -5564,11 +5564,11 @@
       <c r="B60" s="27">
         <v>40</v>
       </c>
-      <c r="C60" s="96"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="73"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="65"/>
       <c r="H60" s="12" t="s">
         <v>49</v>
       </c>
@@ -5577,11 +5577,11 @@
       <c r="B61" s="9">
         <v>41</v>
       </c>
-      <c r="C61" s="96"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72"/>
-      <c r="F61" s="72"/>
-      <c r="G61" s="73"/>
+      <c r="C61" s="85"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="65"/>
       <c r="H61" s="12" t="s">
         <v>49</v>
       </c>
@@ -5590,11 +5590,11 @@
       <c r="B62" s="27">
         <v>42</v>
       </c>
-      <c r="C62" s="96"/>
-      <c r="D62" s="72"/>
-      <c r="E62" s="72"/>
-      <c r="F62" s="72"/>
-      <c r="G62" s="73"/>
+      <c r="C62" s="85"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="65"/>
       <c r="H62" s="12" t="s">
         <v>49</v>
       </c>
@@ -5603,11 +5603,11 @@
       <c r="B63" s="9">
         <v>43</v>
       </c>
-      <c r="C63" s="96"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="73"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="65"/>
       <c r="H63" s="12" t="s">
         <v>49</v>
       </c>
@@ -5616,11 +5616,11 @@
       <c r="B64" s="27">
         <v>44</v>
       </c>
-      <c r="C64" s="96"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="73"/>
+      <c r="C64" s="85"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="65"/>
       <c r="H64" s="12" t="s">
         <v>49</v>
       </c>
@@ -5629,11 +5629,11 @@
       <c r="B65" s="9">
         <v>45</v>
       </c>
-      <c r="C65" s="96"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="73"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="65"/>
       <c r="H65" s="12" t="s">
         <v>49</v>
       </c>
@@ -5642,11 +5642,11 @@
       <c r="B66" s="27">
         <v>46</v>
       </c>
-      <c r="C66" s="96"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="73"/>
+      <c r="C66" s="85"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="65"/>
       <c r="H66" s="12" t="s">
         <v>49</v>
       </c>
@@ -5655,11 +5655,11 @@
       <c r="B67" s="9">
         <v>47</v>
       </c>
-      <c r="C67" s="96"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="73"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
       <c r="H67" s="12" t="s">
         <v>49</v>
       </c>
@@ -5668,11 +5668,11 @@
       <c r="B68" s="27">
         <v>48</v>
       </c>
-      <c r="C68" s="96"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="73"/>
+      <c r="C68" s="85"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="65"/>
       <c r="H68" s="12" t="s">
         <v>49</v>
       </c>
@@ -5681,11 +5681,11 @@
       <c r="B69" s="9">
         <v>49</v>
       </c>
-      <c r="C69" s="96"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="72"/>
-      <c r="G69" s="73"/>
+      <c r="C69" s="85"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="65"/>
       <c r="H69" s="12" t="s">
         <v>49</v>
       </c>
@@ -5694,11 +5694,11 @@
       <c r="B70" s="27">
         <v>50</v>
       </c>
-      <c r="C70" s="96"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="72"/>
-      <c r="G70" s="73"/>
+      <c r="C70" s="85"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="65"/>
       <c r="H70" s="12" t="s">
         <v>49</v>
       </c>
@@ -5707,11 +5707,11 @@
       <c r="B71" s="9">
         <v>51</v>
       </c>
-      <c r="C71" s="96"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="72"/>
-      <c r="F71" s="72"/>
-      <c r="G71" s="73"/>
+      <c r="C71" s="85"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
       <c r="H71" s="12" t="s">
         <v>49</v>
       </c>
@@ -5720,11 +5720,11 @@
       <c r="B72" s="27">
         <v>52</v>
       </c>
-      <c r="C72" s="96"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="73"/>
+      <c r="C72" s="85"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="65"/>
       <c r="H72" s="12" t="s">
         <v>49</v>
       </c>
@@ -5733,11 +5733,11 @@
       <c r="B73" s="9">
         <v>53</v>
       </c>
-      <c r="C73" s="96"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="73"/>
+      <c r="C73" s="85"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
       <c r="H73" s="12" t="s">
         <v>49</v>
       </c>
@@ -5746,11 +5746,11 @@
       <c r="B74" s="27">
         <v>54</v>
       </c>
-      <c r="C74" s="96"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="72"/>
-      <c r="G74" s="73"/>
+      <c r="C74" s="85"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
       <c r="H74" s="12" t="s">
         <v>49</v>
       </c>
@@ -5759,11 +5759,11 @@
       <c r="B75" s="9">
         <v>55</v>
       </c>
-      <c r="C75" s="96"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="72"/>
-      <c r="G75" s="73"/>
+      <c r="C75" s="85"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
       <c r="H75" s="12" t="s">
         <v>49</v>
       </c>
@@ -5772,11 +5772,11 @@
       <c r="B76" s="27">
         <v>56</v>
       </c>
-      <c r="C76" s="96"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="72"/>
-      <c r="G76" s="73"/>
+      <c r="C76" s="85"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
       <c r="H76" s="12" t="s">
         <v>49</v>
       </c>
@@ -5785,11 +5785,11 @@
       <c r="B77" s="9">
         <v>57</v>
       </c>
-      <c r="C77" s="96"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="72"/>
-      <c r="G77" s="73"/>
+      <c r="C77" s="85"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
       <c r="H77" s="12" t="s">
         <v>49</v>
       </c>
@@ -5798,11 +5798,11 @@
       <c r="B78" s="27">
         <v>58</v>
       </c>
-      <c r="C78" s="96"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="C78" s="85"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
       <c r="H78" s="12" t="s">
         <v>49</v>
       </c>
@@ -5811,11 +5811,11 @@
       <c r="B79" s="9">
         <v>59</v>
       </c>
-      <c r="C79" s="96"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="72"/>
-      <c r="F79" s="72"/>
-      <c r="G79" s="73"/>
+      <c r="C79" s="85"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="65"/>
       <c r="H79" s="12" t="s">
         <v>49</v>
       </c>
@@ -5824,11 +5824,11 @@
       <c r="B80" s="27">
         <v>60</v>
       </c>
-      <c r="C80" s="96"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="72"/>
-      <c r="F80" s="72"/>
-      <c r="G80" s="73"/>
+      <c r="C80" s="85"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="65"/>
       <c r="H80" s="12" t="s">
         <v>49</v>
       </c>
@@ -5837,11 +5837,11 @@
       <c r="B81" s="9">
         <v>61</v>
       </c>
-      <c r="C81" s="96"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
-      <c r="F81" s="72"/>
-      <c r="G81" s="73"/>
+      <c r="C81" s="85"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="65"/>
       <c r="H81" s="12" t="s">
         <v>49</v>
       </c>
@@ -5850,11 +5850,11 @@
       <c r="B82" s="27">
         <v>62</v>
       </c>
-      <c r="C82" s="96"/>
-      <c r="D82" s="72"/>
-      <c r="E82" s="72"/>
-      <c r="F82" s="72"/>
-      <c r="G82" s="73"/>
+      <c r="C82" s="85"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="65"/>
       <c r="H82" s="12" t="s">
         <v>49</v>
       </c>
@@ -5863,11 +5863,11 @@
       <c r="B83" s="9">
         <v>63</v>
       </c>
-      <c r="C83" s="96"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
-      <c r="F83" s="72"/>
-      <c r="G83" s="73"/>
+      <c r="C83" s="85"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="65"/>
       <c r="H83" s="12" t="s">
         <v>49</v>
       </c>
@@ -5876,11 +5876,11 @@
       <c r="B84" s="27">
         <v>64</v>
       </c>
-      <c r="C84" s="96"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="72"/>
-      <c r="F84" s="72"/>
-      <c r="G84" s="73"/>
+      <c r="C84" s="85"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="65"/>
       <c r="H84" s="12" t="s">
         <v>49</v>
       </c>
@@ -5889,11 +5889,11 @@
       <c r="B85" s="9">
         <v>65</v>
       </c>
-      <c r="C85" s="96"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="72"/>
-      <c r="F85" s="72"/>
-      <c r="G85" s="73"/>
+      <c r="C85" s="85"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="65"/>
       <c r="H85" s="12" t="s">
         <v>49</v>
       </c>
@@ -5902,11 +5902,11 @@
       <c r="B86" s="27">
         <v>66</v>
       </c>
-      <c r="C86" s="96"/>
-      <c r="D86" s="72"/>
-      <c r="E86" s="72"/>
-      <c r="F86" s="72"/>
-      <c r="G86" s="73"/>
+      <c r="C86" s="85"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
+      <c r="F86" s="64"/>
+      <c r="G86" s="65"/>
       <c r="H86" s="12" t="s">
         <v>49</v>
       </c>
@@ -5915,11 +5915,11 @@
       <c r="B87" s="9">
         <v>67</v>
       </c>
-      <c r="C87" s="96"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="72"/>
-      <c r="F87" s="72"/>
-      <c r="G87" s="73"/>
+      <c r="C87" s="85"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="65"/>
       <c r="H87" s="12" t="s">
         <v>49</v>
       </c>
@@ -5928,11 +5928,11 @@
       <c r="B88" s="27">
         <v>68</v>
       </c>
-      <c r="C88" s="96"/>
-      <c r="D88" s="72"/>
-      <c r="E88" s="72"/>
-      <c r="F88" s="72"/>
-      <c r="G88" s="73"/>
+      <c r="C88" s="85"/>
+      <c r="D88" s="64"/>
+      <c r="E88" s="64"/>
+      <c r="F88" s="64"/>
+      <c r="G88" s="65"/>
       <c r="H88" s="12" t="s">
         <v>49</v>
       </c>
@@ -5941,11 +5941,11 @@
       <c r="B89" s="9">
         <v>69</v>
       </c>
-      <c r="C89" s="96"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="72"/>
-      <c r="F89" s="72"/>
-      <c r="G89" s="73"/>
+      <c r="C89" s="85"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="64"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="65"/>
       <c r="H89" s="12" t="s">
         <v>49</v>
       </c>
@@ -5954,11 +5954,11 @@
       <c r="B90" s="27">
         <v>70</v>
       </c>
-      <c r="C90" s="96"/>
-      <c r="D90" s="72"/>
-      <c r="E90" s="72"/>
-      <c r="F90" s="72"/>
-      <c r="G90" s="73"/>
+      <c r="C90" s="85"/>
+      <c r="D90" s="64"/>
+      <c r="E90" s="64"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="65"/>
       <c r="H90" s="12" t="s">
         <v>49</v>
       </c>
@@ -5967,11 +5967,11 @@
       <c r="B91" s="9">
         <v>71</v>
       </c>
-      <c r="C91" s="96"/>
-      <c r="D91" s="72"/>
-      <c r="E91" s="72"/>
-      <c r="F91" s="72"/>
-      <c r="G91" s="73"/>
+      <c r="C91" s="85"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="65"/>
       <c r="H91" s="12" t="s">
         <v>49</v>
       </c>
@@ -5980,11 +5980,11 @@
       <c r="B92" s="27">
         <v>72</v>
       </c>
-      <c r="C92" s="96"/>
-      <c r="D92" s="72"/>
-      <c r="E92" s="72"/>
-      <c r="F92" s="72"/>
-      <c r="G92" s="73"/>
+      <c r="C92" s="85"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
+      <c r="F92" s="64"/>
+      <c r="G92" s="65"/>
       <c r="H92" s="12" t="s">
         <v>49</v>
       </c>
@@ -5993,11 +5993,11 @@
       <c r="B93" s="9">
         <v>73</v>
       </c>
-      <c r="C93" s="96"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="72"/>
-      <c r="F93" s="72"/>
-      <c r="G93" s="73"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="65"/>
       <c r="H93" s="12" t="s">
         <v>49</v>
       </c>
@@ -6006,11 +6006,11 @@
       <c r="B94" s="27">
         <v>74</v>
       </c>
-      <c r="C94" s="96"/>
-      <c r="D94" s="72"/>
-      <c r="E94" s="72"/>
-      <c r="F94" s="72"/>
-      <c r="G94" s="73"/>
+      <c r="C94" s="85"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="64"/>
+      <c r="G94" s="65"/>
       <c r="H94" s="12" t="s">
         <v>49</v>
       </c>
@@ -6019,11 +6019,11 @@
       <c r="B95" s="9">
         <v>75</v>
       </c>
-      <c r="C95" s="96"/>
-      <c r="D95" s="72"/>
-      <c r="E95" s="72"/>
-      <c r="F95" s="72"/>
-      <c r="G95" s="73"/>
+      <c r="C95" s="85"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="65"/>
       <c r="H95" s="12" t="s">
         <v>49</v>
       </c>
@@ -6032,11 +6032,11 @@
       <c r="B96" s="27">
         <v>76</v>
       </c>
-      <c r="C96" s="96"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="72"/>
-      <c r="F96" s="72"/>
-      <c r="G96" s="73"/>
+      <c r="C96" s="85"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="64"/>
+      <c r="F96" s="64"/>
+      <c r="G96" s="65"/>
       <c r="H96" s="12" t="s">
         <v>49</v>
       </c>
@@ -6045,11 +6045,11 @@
       <c r="B97" s="9">
         <v>77</v>
       </c>
-      <c r="C97" s="96"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="72"/>
-      <c r="F97" s="72"/>
-      <c r="G97" s="73"/>
+      <c r="C97" s="85"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="65"/>
       <c r="H97" s="12" t="s">
         <v>49</v>
       </c>
@@ -6058,11 +6058,11 @@
       <c r="B98" s="27">
         <v>78</v>
       </c>
-      <c r="C98" s="96"/>
-      <c r="D98" s="72"/>
-      <c r="E98" s="72"/>
-      <c r="F98" s="72"/>
-      <c r="G98" s="73"/>
+      <c r="C98" s="85"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="64"/>
+      <c r="G98" s="65"/>
       <c r="H98" s="12" t="s">
         <v>49</v>
       </c>
@@ -6071,11 +6071,11 @@
       <c r="B99" s="9">
         <v>79</v>
       </c>
-      <c r="C99" s="96"/>
-      <c r="D99" s="72"/>
-      <c r="E99" s="72"/>
-      <c r="F99" s="72"/>
-      <c r="G99" s="73"/>
+      <c r="C99" s="85"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="64"/>
+      <c r="G99" s="65"/>
       <c r="H99" s="12" t="s">
         <v>49</v>
       </c>
@@ -6084,11 +6084,11 @@
       <c r="B100" s="27">
         <v>80</v>
       </c>
-      <c r="C100" s="96"/>
-      <c r="D100" s="72"/>
-      <c r="E100" s="72"/>
-      <c r="F100" s="72"/>
-      <c r="G100" s="73"/>
+      <c r="C100" s="85"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="64"/>
+      <c r="G100" s="65"/>
       <c r="H100" s="12" t="s">
         <v>49</v>
       </c>
@@ -6097,11 +6097,11 @@
       <c r="B101" s="9">
         <v>81</v>
       </c>
-      <c r="C101" s="96"/>
-      <c r="D101" s="72"/>
-      <c r="E101" s="72"/>
-      <c r="F101" s="72"/>
-      <c r="G101" s="73"/>
+      <c r="C101" s="85"/>
+      <c r="D101" s="64"/>
+      <c r="E101" s="64"/>
+      <c r="F101" s="64"/>
+      <c r="G101" s="65"/>
       <c r="H101" s="12" t="s">
         <v>49</v>
       </c>
@@ -6110,11 +6110,11 @@
       <c r="B102" s="27">
         <v>82</v>
       </c>
-      <c r="C102" s="96"/>
-      <c r="D102" s="72"/>
-      <c r="E102" s="72"/>
-      <c r="F102" s="72"/>
-      <c r="G102" s="73"/>
+      <c r="C102" s="85"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
+      <c r="G102" s="65"/>
       <c r="H102" s="12" t="s">
         <v>49</v>
       </c>
@@ -6123,11 +6123,11 @@
       <c r="B103" s="9">
         <v>83</v>
       </c>
-      <c r="C103" s="96"/>
-      <c r="D103" s="72"/>
-      <c r="E103" s="72"/>
-      <c r="F103" s="72"/>
-      <c r="G103" s="73"/>
+      <c r="C103" s="85"/>
+      <c r="D103" s="64"/>
+      <c r="E103" s="64"/>
+      <c r="F103" s="64"/>
+      <c r="G103" s="65"/>
       <c r="H103" s="12" t="s">
         <v>49</v>
       </c>
@@ -6136,11 +6136,11 @@
       <c r="B104" s="27">
         <v>84</v>
       </c>
-      <c r="C104" s="96"/>
-      <c r="D104" s="72"/>
-      <c r="E104" s="72"/>
-      <c r="F104" s="72"/>
-      <c r="G104" s="73"/>
+      <c r="C104" s="85"/>
+      <c r="D104" s="64"/>
+      <c r="E104" s="64"/>
+      <c r="F104" s="64"/>
+      <c r="G104" s="65"/>
       <c r="H104" s="12" t="s">
         <v>49</v>
       </c>
@@ -6149,11 +6149,11 @@
       <c r="B105" s="9">
         <v>85</v>
       </c>
-      <c r="C105" s="96"/>
-      <c r="D105" s="72"/>
-      <c r="E105" s="72"/>
-      <c r="F105" s="72"/>
-      <c r="G105" s="73"/>
+      <c r="C105" s="85"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="64"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="65"/>
       <c r="H105" s="12" t="s">
         <v>49</v>
       </c>
@@ -6162,11 +6162,11 @@
       <c r="B106" s="27">
         <v>86</v>
       </c>
-      <c r="C106" s="96"/>
-      <c r="D106" s="72"/>
-      <c r="E106" s="72"/>
-      <c r="F106" s="72"/>
-      <c r="G106" s="73"/>
+      <c r="C106" s="85"/>
+      <c r="D106" s="64"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="64"/>
+      <c r="G106" s="65"/>
       <c r="H106" s="12" t="s">
         <v>49</v>
       </c>
@@ -6175,11 +6175,11 @@
       <c r="B107" s="9">
         <v>87</v>
       </c>
-      <c r="C107" s="96"/>
-      <c r="D107" s="72"/>
-      <c r="E107" s="72"/>
-      <c r="F107" s="72"/>
-      <c r="G107" s="73"/>
+      <c r="C107" s="85"/>
+      <c r="D107" s="64"/>
+      <c r="E107" s="64"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="65"/>
       <c r="H107" s="12" t="s">
         <v>49</v>
       </c>
@@ -6188,11 +6188,11 @@
       <c r="B108" s="27">
         <v>88</v>
       </c>
-      <c r="C108" s="96"/>
-      <c r="D108" s="72"/>
-      <c r="E108" s="72"/>
-      <c r="F108" s="72"/>
-      <c r="G108" s="73"/>
+      <c r="C108" s="85"/>
+      <c r="D108" s="64"/>
+      <c r="E108" s="64"/>
+      <c r="F108" s="64"/>
+      <c r="G108" s="65"/>
       <c r="H108" s="12" t="s">
         <v>49</v>
       </c>
@@ -6201,11 +6201,11 @@
       <c r="B109" s="9">
         <v>89</v>
       </c>
-      <c r="C109" s="96"/>
-      <c r="D109" s="72"/>
-      <c r="E109" s="72"/>
-      <c r="F109" s="72"/>
-      <c r="G109" s="73"/>
+      <c r="C109" s="85"/>
+      <c r="D109" s="64"/>
+      <c r="E109" s="64"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="65"/>
       <c r="H109" s="12" t="s">
         <v>49</v>
       </c>
@@ -6214,11 +6214,11 @@
       <c r="B110" s="27">
         <v>90</v>
       </c>
-      <c r="C110" s="96"/>
-      <c r="D110" s="72"/>
-      <c r="E110" s="72"/>
-      <c r="F110" s="72"/>
-      <c r="G110" s="73"/>
+      <c r="C110" s="85"/>
+      <c r="D110" s="64"/>
+      <c r="E110" s="64"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="65"/>
       <c r="H110" s="12" t="s">
         <v>49</v>
       </c>
@@ -6227,11 +6227,11 @@
       <c r="B111" s="9">
         <v>91</v>
       </c>
-      <c r="C111" s="96"/>
-      <c r="D111" s="72"/>
-      <c r="E111" s="72"/>
-      <c r="F111" s="72"/>
-      <c r="G111" s="73"/>
+      <c r="C111" s="85"/>
+      <c r="D111" s="64"/>
+      <c r="E111" s="64"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="65"/>
       <c r="H111" s="12" t="s">
         <v>49</v>
       </c>
@@ -6240,11 +6240,11 @@
       <c r="B112" s="27">
         <v>92</v>
       </c>
-      <c r="C112" s="96"/>
-      <c r="D112" s="72"/>
-      <c r="E112" s="72"/>
-      <c r="F112" s="72"/>
-      <c r="G112" s="73"/>
+      <c r="C112" s="85"/>
+      <c r="D112" s="64"/>
+      <c r="E112" s="64"/>
+      <c r="F112" s="64"/>
+      <c r="G112" s="65"/>
       <c r="H112" s="12" t="s">
         <v>49</v>
       </c>
@@ -6253,11 +6253,11 @@
       <c r="B113" s="9">
         <v>93</v>
       </c>
-      <c r="C113" s="96"/>
-      <c r="D113" s="72"/>
-      <c r="E113" s="72"/>
-      <c r="F113" s="72"/>
-      <c r="G113" s="73"/>
+      <c r="C113" s="85"/>
+      <c r="D113" s="64"/>
+      <c r="E113" s="64"/>
+      <c r="F113" s="64"/>
+      <c r="G113" s="65"/>
       <c r="H113" s="12" t="s">
         <v>49</v>
       </c>
@@ -6266,11 +6266,11 @@
       <c r="B114" s="27">
         <v>94</v>
       </c>
-      <c r="C114" s="96"/>
-      <c r="D114" s="72"/>
-      <c r="E114" s="72"/>
-      <c r="F114" s="72"/>
-      <c r="G114" s="73"/>
+      <c r="C114" s="85"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="64"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="65"/>
       <c r="H114" s="12" t="s">
         <v>49</v>
       </c>
@@ -6279,11 +6279,11 @@
       <c r="B115" s="9">
         <v>95</v>
       </c>
-      <c r="C115" s="96"/>
-      <c r="D115" s="72"/>
-      <c r="E115" s="72"/>
-      <c r="F115" s="72"/>
-      <c r="G115" s="73"/>
+      <c r="C115" s="85"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="64"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="65"/>
       <c r="H115" s="12" t="s">
         <v>49</v>
       </c>
@@ -6292,11 +6292,11 @@
       <c r="B116" s="27">
         <v>96</v>
       </c>
-      <c r="C116" s="96"/>
-      <c r="D116" s="72"/>
-      <c r="E116" s="72"/>
-      <c r="F116" s="72"/>
-      <c r="G116" s="73"/>
+      <c r="C116" s="85"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="64"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="65"/>
       <c r="H116" s="12" t="s">
         <v>49</v>
       </c>
@@ -6305,11 +6305,11 @@
       <c r="B117" s="9">
         <v>97</v>
       </c>
-      <c r="C117" s="96"/>
-      <c r="D117" s="72"/>
-      <c r="E117" s="72"/>
-      <c r="F117" s="72"/>
-      <c r="G117" s="73"/>
+      <c r="C117" s="85"/>
+      <c r="D117" s="64"/>
+      <c r="E117" s="64"/>
+      <c r="F117" s="64"/>
+      <c r="G117" s="65"/>
       <c r="H117" s="12" t="s">
         <v>49</v>
       </c>
@@ -6318,11 +6318,11 @@
       <c r="B118" s="27">
         <v>98</v>
       </c>
-      <c r="C118" s="96"/>
-      <c r="D118" s="72"/>
-      <c r="E118" s="72"/>
-      <c r="F118" s="72"/>
-      <c r="G118" s="73"/>
+      <c r="C118" s="85"/>
+      <c r="D118" s="64"/>
+      <c r="E118" s="64"/>
+      <c r="F118" s="64"/>
+      <c r="G118" s="65"/>
       <c r="H118" s="12" t="s">
         <v>49</v>
       </c>
@@ -6331,11 +6331,11 @@
       <c r="B119" s="9">
         <v>99</v>
       </c>
-      <c r="C119" s="96"/>
-      <c r="D119" s="72"/>
-      <c r="E119" s="72"/>
-      <c r="F119" s="72"/>
-      <c r="G119" s="73"/>
+      <c r="C119" s="85"/>
+      <c r="D119" s="64"/>
+      <c r="E119" s="64"/>
+      <c r="F119" s="64"/>
+      <c r="G119" s="65"/>
       <c r="H119" s="12" t="s">
         <v>49</v>
       </c>
@@ -6344,11 +6344,11 @@
       <c r="B120" s="27">
         <v>100</v>
       </c>
-      <c r="C120" s="96"/>
-      <c r="D120" s="72"/>
-      <c r="E120" s="72"/>
-      <c r="F120" s="72"/>
-      <c r="G120" s="73"/>
+      <c r="C120" s="85"/>
+      <c r="D120" s="64"/>
+      <c r="E120" s="64"/>
+      <c r="F120" s="64"/>
+      <c r="G120" s="65"/>
       <c r="H120" s="12" t="s">
         <v>49</v>
       </c>
@@ -8027,53 +8027,50 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
@@ -8098,50 +8095,53 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C95:G95"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H120" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8191,85 +8191,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2">
         <f>Requisitos!C11</f>
         <v>45170</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K65" si="0">K1+1</f>
         <v>45171</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45172</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45173</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45174</v>
@@ -8283,18 +8283,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="str">
+      <c r="B7" s="75" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45176</v>
@@ -8311,13 +8311,13 @@
       <c r="B9" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="57" t="s">
         <v>55</v>
       </c>
@@ -9691,13 +9691,13 @@
       <c r="B63" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="72"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="73"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="65"/>
       <c r="K63" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -9707,11 +9707,11 @@
       <c r="B64" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="73"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="65"/>
       <c r="H64" s="7" t="s">
         <v>67</v>
       </c>
@@ -9728,11 +9728,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="73"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="65"/>
       <c r="H65" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B10,H$11:H$60)</f>
         <v>0</v>
@@ -9751,11 +9751,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="73"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="65"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -9774,11 +9774,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="73"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -9797,11 +9797,11 @@
         <f>'Dados do Projeto'!B13</f>
         <v>Maria Eduarda Amaral</v>
       </c>
-      <c r="C68" s="72"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="73"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="65"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -9820,11 +9820,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="72"/>
-      <c r="G69" s="73"/>
+      <c r="C69" s="64"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="65"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -9843,11 +9843,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="72"/>
-      <c r="G70" s="73"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="65"/>
       <c r="H70" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -10975,8 +10975,8 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10996,85 +10996,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2">
         <f>Requisitos!C12</f>
         <v>45191</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45192</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45193</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45194</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45195</v>
@@ -11088,18 +11088,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="str">
+      <c r="B7" s="75" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45197</v>
@@ -11116,13 +11116,13 @@
       <c r="B9" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="57" t="s">
         <v>55</v>
       </c>
@@ -11539,10 +11539,10 @@
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H23" s="13">
         <v>0</v>
@@ -11567,10 +11567,10 @@
         <v>3</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H24" s="13">
         <v>0</v>
@@ -12483,7 +12483,7 @@
       <c r="F71" s="30"/>
       <c r="G71" s="30">
         <f>COUNTIFS(G11:G60, "Concluído",D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J71" s="5"/>
     </row>
@@ -12491,23 +12491,23 @@
       <c r="B72" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="73"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="73"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
       <c r="H73" s="7" t="s">
         <v>67</v>
       </c>
@@ -12520,11 +12520,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="72"/>
-      <c r="G74" s="73"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -12539,11 +12539,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="72"/>
-      <c r="G75" s="73"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -12558,11 +12558,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="72"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="72"/>
-      <c r="G76" s="73"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -12577,11 +12577,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="72"/>
-      <c r="G77" s="73"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -12596,11 +12596,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -13851,85 +13851,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2">
         <f>Requisitos!C13</f>
         <v>45205</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>45206</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45207</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45208</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45209</v>
@@ -13943,18 +13943,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="str">
+      <c r="B7" s="75" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45211</v>
@@ -13971,13 +13971,13 @@
       <c r="B9" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="57" t="s">
         <v>55</v>
       </c>
@@ -15117,23 +15117,23 @@
       <c r="B72" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="73"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="73"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
       <c r="H73" s="7" t="s">
         <v>67</v>
       </c>
@@ -15146,11 +15146,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="72"/>
-      <c r="G74" s="73"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -15165,11 +15165,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="72"/>
-      <c r="G75" s="73"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -15184,11 +15184,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="72"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="72"/>
-      <c r="G76" s="73"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -15203,11 +15203,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="72"/>
-      <c r="G77" s="73"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -15222,11 +15222,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -16250,12 +16250,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B9:I9"/>
@@ -16264,6 +16258,12 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F20:F25">
     <cfRule type="expression" dxfId="89" priority="1">
@@ -16450,85 +16450,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2">
         <f>Requisitos!C14</f>
         <v>45226</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>45227</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45228</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45229</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45230</v>
@@ -16542,18 +16542,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="str">
+      <c r="B7" s="75" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -16570,13 +16570,13 @@
       <c r="B9" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="57" t="s">
         <v>55</v>
       </c>
@@ -17716,23 +17716,23 @@
       <c r="B72" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="73"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="73"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
       <c r="H73" s="7" t="s">
         <v>67</v>
       </c>
@@ -17745,11 +17745,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="72"/>
-      <c r="G74" s="73"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -17764,11 +17764,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="72"/>
-      <c r="G75" s="73"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -17783,11 +17783,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="72"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="72"/>
-      <c r="G76" s="73"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -17802,11 +17802,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="72"/>
-      <c r="G77" s="73"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -17821,11 +17821,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -18849,12 +18849,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B9:I9"/>
@@ -18863,6 +18857,12 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F20:F25">
     <cfRule type="expression" dxfId="63" priority="1">
@@ -19048,85 +19048,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2">
         <f>Requisitos!C15</f>
         <v>45247</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45248</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45249</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45250</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45251</v>
@@ -19139,18 +19139,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="str">
+      <c r="B7" s="75" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45253</v>
@@ -19166,13 +19166,13 @@
       <c r="B9" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="58" t="s">
         <v>55</v>
       </c>
@@ -20136,23 +20136,23 @@
       <c r="B63" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="72"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="73"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="65"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="73"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="65"/>
       <c r="H64" s="7" t="s">
         <v>67</v>
       </c>
@@ -20165,11 +20165,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="73"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="65"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -20184,11 +20184,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="73"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="65"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -20203,11 +20203,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="73"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -20222,11 +20222,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C68" s="72"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="73"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="65"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -20241,11 +20241,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="72"/>
-      <c r="G69" s="73"/>
+      <c r="C69" s="64"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="65"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -21208,12 +21208,6 @@
   </sheetData>
   <autoFilter ref="B10:J60" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B9:I9"/>
@@ -21222,6 +21216,12 @@
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F17">
     <cfRule type="containsBlanks" dxfId="37" priority="1">

</xml_diff>

<commit_message>
doc: update planejamento_sprints #69
</commit_message>
<xml_diff>
--- a/Artefatos/sprints/Planejamento_sprints.xlsx
+++ b/Artefatos/sprints/Planejamento_sprints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositorios_github\plf-es-2023-2-ti3-6653100-fabrica-do-saber\Artefatos\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EEF05C-5262-4B09-A995-E7F5DFD48C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756140CC-EDDB-4A66-A4C7-212145E3FA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1068,14 +1068,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1259,7 +1265,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1403,35 +1409,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1441,19 +1428,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1470,15 +1485,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1489,22 +1495,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1515,33 +1524,36 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="123">
@@ -2668,7 +2680,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:style val="18"/>
   <c:chart>
@@ -3286,166 +3298,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="76" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="78" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="78" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="80"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="78" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
       <c r="K12" s="47"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="78" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="79"/>
-      <c r="H13" s="80"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="71"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="78" t="s">
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="79"/>
-      <c r="H14" s="80"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="78" t="s">
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="79"/>
-      <c r="H15" s="80"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="18"/>
@@ -3547,16 +3559,16 @@
     <row r="99" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="50"/>
-      <c r="B100" s="82"/>
-      <c r="C100" s="67"/>
-      <c r="D100" s="83" t="s">
+      <c r="B100" s="72"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="E100" s="67"/>
-      <c r="F100" s="83" t="s">
+      <c r="E100" s="64"/>
+      <c r="F100" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="G100" s="67"/>
+      <c r="G100" s="64"/>
       <c r="H100" s="51" t="s">
         <v>18</v>
       </c>
@@ -3578,12 +3590,12 @@
     </row>
     <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
-      <c r="B101" s="85"/>
-      <c r="C101" s="67"/>
-      <c r="D101" s="84" t="s">
+      <c r="B101" s="63"/>
+      <c r="C101" s="64"/>
+      <c r="D101" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="67"/>
+      <c r="E101" s="64"/>
       <c r="F101" s="53" t="s">
         <v>24</v>
       </c>
@@ -3616,12 +3628,12 @@
     </row>
     <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
-      <c r="B102" s="85"/>
-      <c r="C102" s="67"/>
-      <c r="D102" s="84" t="s">
+      <c r="B102" s="63"/>
+      <c r="C102" s="64"/>
+      <c r="D102" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="E102" s="67"/>
+      <c r="E102" s="64"/>
       <c r="F102" s="53" t="s">
         <v>29</v>
       </c>
@@ -3655,12 +3667,12 @@
     </row>
     <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="50"/>
-      <c r="B103" s="85"/>
-      <c r="C103" s="67"/>
-      <c r="D103" s="84" t="s">
+      <c r="B103" s="63"/>
+      <c r="C103" s="64"/>
+      <c r="D103" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="67"/>
+      <c r="E103" s="64"/>
       <c r="F103" s="53"/>
       <c r="G103" s="54" t="s">
         <v>34</v>
@@ -3692,12 +3704,12 @@
     </row>
     <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="50"/>
-      <c r="B104" s="85"/>
-      <c r="C104" s="67"/>
-      <c r="D104" s="84" t="s">
+      <c r="B104" s="63"/>
+      <c r="C104" s="64"/>
+      <c r="D104" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="67"/>
+      <c r="E104" s="64"/>
       <c r="F104" s="53"/>
       <c r="G104" s="54" t="s">
         <v>36</v>
@@ -3727,12 +3739,12 @@
     </row>
     <row r="105" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="50"/>
-      <c r="B105" s="85"/>
-      <c r="C105" s="67"/>
-      <c r="D105" s="84" t="s">
+      <c r="B105" s="63"/>
+      <c r="C105" s="64"/>
+      <c r="D105" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="E105" s="67"/>
+      <c r="E105" s="64"/>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="s">
         <v>39</v>
@@ -3757,8 +3769,8 @@
     </row>
     <row r="106" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="50"/>
-      <c r="B106" s="85"/>
-      <c r="C106" s="67"/>
+      <c r="B106" s="63"/>
+      <c r="C106" s="64"/>
       <c r="F106" s="53"/>
       <c r="G106" s="54"/>
       <c r="H106" s="53"/>
@@ -3769,8 +3781,8 @@
     </row>
     <row r="107" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="50"/>
-      <c r="B107" s="85"/>
-      <c r="C107" s="67"/>
+      <c r="B107" s="63"/>
+      <c r="C107" s="64"/>
       <c r="D107" s="55"/>
       <c r="E107" s="53"/>
       <c r="F107" s="53"/>
@@ -4738,12 +4750,24 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B100:C100"/>
     <mergeCell ref="D100:E100"/>
@@ -4755,24 +4779,12 @@
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D105:E105"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="F10:F15" xr:uid="{49EDF03A-7EFB-435C-A992-40D98DE85B41}">
@@ -4797,8 +4809,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:G32"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H28" sqref="C28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4815,59 +4827,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -4883,12 +4895,12 @@
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -4903,12 +4915,12 @@
       <c r="B9" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
@@ -4923,8 +4935,8 @@
       <c r="E10" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="6" t="s">
         <v>45</v>
       </c>
@@ -4939,9 +4951,9 @@
       <c r="D11" s="14">
         <v>45190</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4955,9 +4967,9 @@
         <f t="shared" ref="D12" si="0">C12+13</f>
         <v>45204</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4971,9 +4983,9 @@
       <c r="D13" s="14">
         <v>45225</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4986,9 +4998,9 @@
       <c r="D14" s="14">
         <v>45246</v>
       </c>
-      <c r="E14" s="88"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5027,13 +5039,13 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
-      <c r="C18" s="89" t="s">
+      <c r="C18" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
       <c r="H18" s="22" t="s">
         <v>47</v>
       </c>
@@ -5042,11 +5054,11 @@
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="90"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="25" t="s">
         <v>48</v>
       </c>
@@ -5056,11 +5068,11 @@
       <c r="B20" s="27">
         <v>0</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="28"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -5077,14 +5089,14 @@
       <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="12" t="s">
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="104" t="s">
         <v>50</v>
       </c>
       <c r="J21" s="48"/>
@@ -5093,14 +5105,14 @@
       <c r="B22" s="27">
         <v>2</v>
       </c>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="12" t="s">
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="104" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5108,14 +5120,14 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="12" t="s">
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="104" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5123,14 +5135,14 @@
       <c r="B24" s="27">
         <v>4</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="100"/>
-      <c r="H24" s="12" t="s">
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5138,13 +5150,13 @@
       <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="103"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="89"/>
       <c r="H25" s="12" t="s">
         <v>54</v>
       </c>
@@ -5153,13 +5165,13 @@
       <c r="B26" s="27">
         <v>6</v>
       </c>
-      <c r="C26" s="101" t="s">
+      <c r="C26" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="102"/>
-      <c r="G26" s="103"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="89"/>
       <c r="H26" s="12" t="s">
         <v>54</v>
       </c>
@@ -5168,29 +5180,29 @@
       <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="12" t="s">
-        <v>58</v>
+      <c r="D27" s="102"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="27">
         <v>8</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="C28" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="12" t="s">
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5198,14 +5210,14 @@
       <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="105"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="12" t="s">
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5213,14 +5225,14 @@
       <c r="B30" s="27">
         <v>10</v>
       </c>
-      <c r="C30" s="101" t="s">
+      <c r="C30" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="102"/>
-      <c r="E30" s="102"/>
-      <c r="F30" s="102"/>
-      <c r="G30" s="103"/>
-      <c r="H30" s="12" t="s">
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5228,14 +5240,14 @@
       <c r="B31" s="9">
         <v>11</v>
       </c>
-      <c r="C31" s="101" t="s">
+      <c r="C31" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="102"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="12" t="s">
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="107"/>
+      <c r="H31" s="108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5243,13 +5255,13 @@
       <c r="B32" s="27">
         <v>12</v>
       </c>
-      <c r="C32" s="101" t="s">
+      <c r="C32" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="103"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="89"/>
       <c r="H32" s="12" t="s">
         <v>58</v>
       </c>
@@ -5258,14 +5270,14 @@
       <c r="B33" s="9">
         <v>13</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="12" t="s">
+      <c r="D33" s="102"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="104" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5273,11 +5285,11 @@
       <c r="B34" s="27">
         <v>14</v>
       </c>
-      <c r="C34" s="101"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="103"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="89"/>
       <c r="H34" s="12" t="s">
         <v>54</v>
       </c>
@@ -5286,11 +5298,11 @@
       <c r="B35" s="9">
         <v>15</v>
       </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="103"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="89"/>
       <c r="H35" s="12" t="s">
         <v>54</v>
       </c>
@@ -5299,11 +5311,11 @@
       <c r="B36" s="27">
         <v>16</v>
       </c>
-      <c r="C36" s="101"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="75"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="12" t="s">
         <v>54</v>
       </c>
@@ -5312,11 +5324,11 @@
       <c r="B37" s="9">
         <v>17</v>
       </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="75"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="67"/>
       <c r="H37" s="12" t="s">
         <v>54</v>
       </c>
@@ -5325,11 +5337,11 @@
       <c r="B38" s="27">
         <v>18</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="75"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="67"/>
       <c r="H38" s="12" t="s">
         <v>54</v>
       </c>
@@ -5338,11 +5350,11 @@
       <c r="B39" s="9">
         <v>19</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="75"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="67"/>
       <c r="H39" s="12" t="s">
         <v>54</v>
       </c>
@@ -5351,11 +5363,11 @@
       <c r="B40" s="27">
         <v>20</v>
       </c>
-      <c r="C40" s="101"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="75"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="67"/>
       <c r="H40" s="12" t="s">
         <v>54</v>
       </c>
@@ -5364,11 +5376,11 @@
       <c r="B41" s="9">
         <v>21</v>
       </c>
-      <c r="C41" s="101"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="75"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="67"/>
       <c r="H41" s="12" t="s">
         <v>54</v>
       </c>
@@ -5377,11 +5389,11 @@
       <c r="B42" s="27">
         <v>22</v>
       </c>
-      <c r="C42" s="101"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="75"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="67"/>
       <c r="H42" s="12" t="s">
         <v>54</v>
       </c>
@@ -5390,11 +5402,11 @@
       <c r="B43" s="9">
         <v>23</v>
       </c>
-      <c r="C43" s="101"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="75"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="67"/>
       <c r="H43" s="12" t="s">
         <v>54</v>
       </c>
@@ -5403,11 +5415,11 @@
       <c r="B44" s="27">
         <v>24</v>
       </c>
-      <c r="C44" s="101"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="75"/>
+      <c r="C44" s="87"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="67"/>
       <c r="H44" s="12" t="s">
         <v>54</v>
       </c>
@@ -5416,11 +5428,11 @@
       <c r="B45" s="9">
         <v>25</v>
       </c>
-      <c r="C45" s="101"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="75"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="67"/>
       <c r="H45" s="12" t="s">
         <v>54</v>
       </c>
@@ -5429,11 +5441,11 @@
       <c r="B46" s="27">
         <v>26</v>
       </c>
-      <c r="C46" s="101"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="75"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
+      <c r="G46" s="67"/>
       <c r="H46" s="12" t="s">
         <v>54</v>
       </c>
@@ -5442,11 +5454,11 @@
       <c r="B47" s="9">
         <v>27</v>
       </c>
-      <c r="C47" s="101"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="75"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="67"/>
       <c r="H47" s="12" t="s">
         <v>54</v>
       </c>
@@ -5455,11 +5467,11 @@
       <c r="B48" s="27">
         <v>28</v>
       </c>
-      <c r="C48" s="101"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="75"/>
+      <c r="C48" s="87"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="67"/>
       <c r="H48" s="12" t="s">
         <v>54</v>
       </c>
@@ -5468,11 +5480,11 @@
       <c r="B49" s="9">
         <v>29</v>
       </c>
-      <c r="C49" s="101"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="75"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="67"/>
       <c r="H49" s="12" t="s">
         <v>54</v>
       </c>
@@ -5481,11 +5493,11 @@
       <c r="B50" s="27">
         <v>30</v>
       </c>
-      <c r="C50" s="101"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="75"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="67"/>
       <c r="H50" s="12" t="s">
         <v>54</v>
       </c>
@@ -5494,11 +5506,11 @@
       <c r="B51" s="9">
         <v>31</v>
       </c>
-      <c r="C51" s="101"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="75"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="66"/>
+      <c r="G51" s="67"/>
       <c r="H51" s="12" t="s">
         <v>54</v>
       </c>
@@ -5507,11 +5519,11 @@
       <c r="B52" s="27">
         <v>32</v>
       </c>
-      <c r="C52" s="101"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="75"/>
+      <c r="C52" s="87"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="66"/>
+      <c r="G52" s="67"/>
       <c r="H52" s="12" t="s">
         <v>54</v>
       </c>
@@ -5520,11 +5532,11 @@
       <c r="B53" s="9">
         <v>33</v>
       </c>
-      <c r="C53" s="101"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
-      <c r="F53" s="74"/>
-      <c r="G53" s="75"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="67"/>
       <c r="H53" s="12" t="s">
         <v>54</v>
       </c>
@@ -5533,11 +5545,11 @@
       <c r="B54" s="27">
         <v>34</v>
       </c>
-      <c r="C54" s="101"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="75"/>
+      <c r="C54" s="87"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="67"/>
       <c r="H54" s="12" t="s">
         <v>54</v>
       </c>
@@ -5546,11 +5558,11 @@
       <c r="B55" s="9">
         <v>35</v>
       </c>
-      <c r="C55" s="101"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="75"/>
+      <c r="C55" s="87"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="66"/>
+      <c r="G55" s="67"/>
       <c r="H55" s="12" t="s">
         <v>54</v>
       </c>
@@ -5559,11 +5571,11 @@
       <c r="B56" s="27">
         <v>36</v>
       </c>
-      <c r="C56" s="101"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="75"/>
+      <c r="C56" s="87"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="67"/>
       <c r="H56" s="12" t="s">
         <v>54</v>
       </c>
@@ -5572,11 +5584,11 @@
       <c r="B57" s="9">
         <v>37</v>
       </c>
-      <c r="C57" s="101"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="75"/>
+      <c r="C57" s="87"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="66"/>
+      <c r="G57" s="67"/>
       <c r="H57" s="12" t="s">
         <v>54</v>
       </c>
@@ -5585,11 +5597,11 @@
       <c r="B58" s="27">
         <v>38</v>
       </c>
-      <c r="C58" s="101"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="75"/>
+      <c r="C58" s="87"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="67"/>
       <c r="H58" s="12" t="s">
         <v>54</v>
       </c>
@@ -5598,11 +5610,11 @@
       <c r="B59" s="9">
         <v>39</v>
       </c>
-      <c r="C59" s="101"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="75"/>
+      <c r="C59" s="87"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="66"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="67"/>
       <c r="H59" s="12" t="s">
         <v>54</v>
       </c>
@@ -5611,11 +5623,11 @@
       <c r="B60" s="27">
         <v>40</v>
       </c>
-      <c r="C60" s="101"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
-      <c r="F60" s="74"/>
-      <c r="G60" s="75"/>
+      <c r="C60" s="87"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="67"/>
       <c r="H60" s="12" t="s">
         <v>54</v>
       </c>
@@ -5624,11 +5636,11 @@
       <c r="B61" s="9">
         <v>41</v>
       </c>
-      <c r="C61" s="101"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="75"/>
+      <c r="C61" s="87"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="67"/>
       <c r="H61" s="12" t="s">
         <v>54</v>
       </c>
@@ -5637,11 +5649,11 @@
       <c r="B62" s="27">
         <v>42</v>
       </c>
-      <c r="C62" s="101"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="75"/>
+      <c r="C62" s="87"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="66"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="67"/>
       <c r="H62" s="12" t="s">
         <v>54</v>
       </c>
@@ -5650,11 +5662,11 @@
       <c r="B63" s="9">
         <v>43</v>
       </c>
-      <c r="C63" s="101"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="75"/>
+      <c r="C63" s="87"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="67"/>
       <c r="H63" s="12" t="s">
         <v>54</v>
       </c>
@@ -5663,11 +5675,11 @@
       <c r="B64" s="27">
         <v>44</v>
       </c>
-      <c r="C64" s="101"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="75"/>
+      <c r="C64" s="87"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="67"/>
       <c r="H64" s="12" t="s">
         <v>54</v>
       </c>
@@ -5676,11 +5688,11 @@
       <c r="B65" s="9">
         <v>45</v>
       </c>
-      <c r="C65" s="101"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="75"/>
+      <c r="C65" s="87"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="67"/>
       <c r="H65" s="12" t="s">
         <v>54</v>
       </c>
@@ -5689,11 +5701,11 @@
       <c r="B66" s="27">
         <v>46</v>
       </c>
-      <c r="C66" s="101"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
+      <c r="C66" s="87"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="66"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="67"/>
       <c r="H66" s="12" t="s">
         <v>54</v>
       </c>
@@ -5702,11 +5714,11 @@
       <c r="B67" s="9">
         <v>47</v>
       </c>
-      <c r="C67" s="101"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="75"/>
+      <c r="C67" s="87"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="66"/>
+      <c r="G67" s="67"/>
       <c r="H67" s="12" t="s">
         <v>54</v>
       </c>
@@ -5715,11 +5727,11 @@
       <c r="B68" s="27">
         <v>48</v>
       </c>
-      <c r="C68" s="101"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
+      <c r="C68" s="87"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="67"/>
       <c r="H68" s="12" t="s">
         <v>54</v>
       </c>
@@ -5728,11 +5740,11 @@
       <c r="B69" s="9">
         <v>49</v>
       </c>
-      <c r="C69" s="101"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
+      <c r="C69" s="87"/>
+      <c r="D69" s="66"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="67"/>
       <c r="H69" s="12" t="s">
         <v>54</v>
       </c>
@@ -5741,11 +5753,11 @@
       <c r="B70" s="27">
         <v>50</v>
       </c>
-      <c r="C70" s="101"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="75"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="67"/>
       <c r="H70" s="12" t="s">
         <v>54</v>
       </c>
@@ -5754,11 +5766,11 @@
       <c r="B71" s="9">
         <v>51</v>
       </c>
-      <c r="C71" s="101"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="75"/>
+      <c r="C71" s="87"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="67"/>
       <c r="H71" s="12" t="s">
         <v>54</v>
       </c>
@@ -5767,11 +5779,11 @@
       <c r="B72" s="27">
         <v>52</v>
       </c>
-      <c r="C72" s="101"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="75"/>
+      <c r="C72" s="87"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="67"/>
       <c r="H72" s="12" t="s">
         <v>54</v>
       </c>
@@ -5780,11 +5792,11 @@
       <c r="B73" s="9">
         <v>53</v>
       </c>
-      <c r="C73" s="101"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
+      <c r="C73" s="87"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="67"/>
       <c r="H73" s="12" t="s">
         <v>54</v>
       </c>
@@ -5793,11 +5805,11 @@
       <c r="B74" s="27">
         <v>54</v>
       </c>
-      <c r="C74" s="101"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="67"/>
       <c r="H74" s="12" t="s">
         <v>54</v>
       </c>
@@ -5806,11 +5818,11 @@
       <c r="B75" s="9">
         <v>55</v>
       </c>
-      <c r="C75" s="101"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
+      <c r="C75" s="87"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="67"/>
       <c r="H75" s="12" t="s">
         <v>54</v>
       </c>
@@ -5819,11 +5831,11 @@
       <c r="B76" s="27">
         <v>56</v>
       </c>
-      <c r="C76" s="101"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
+      <c r="C76" s="87"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="67"/>
       <c r="H76" s="12" t="s">
         <v>54</v>
       </c>
@@ -5832,11 +5844,11 @@
       <c r="B77" s="9">
         <v>57</v>
       </c>
-      <c r="C77" s="101"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
       <c r="H77" s="12" t="s">
         <v>54</v>
       </c>
@@ -5845,11 +5857,11 @@
       <c r="B78" s="27">
         <v>58</v>
       </c>
-      <c r="C78" s="101"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
+      <c r="C78" s="87"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="67"/>
       <c r="H78" s="12" t="s">
         <v>54</v>
       </c>
@@ -5858,11 +5870,11 @@
       <c r="B79" s="9">
         <v>59</v>
       </c>
-      <c r="C79" s="101"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="75"/>
+      <c r="C79" s="87"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="67"/>
       <c r="H79" s="12" t="s">
         <v>54</v>
       </c>
@@ -5871,11 +5883,11 @@
       <c r="B80" s="27">
         <v>60</v>
       </c>
-      <c r="C80" s="101"/>
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="74"/>
-      <c r="G80" s="75"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="67"/>
       <c r="H80" s="12" t="s">
         <v>54</v>
       </c>
@@ -5884,11 +5896,11 @@
       <c r="B81" s="9">
         <v>61</v>
       </c>
-      <c r="C81" s="101"/>
-      <c r="D81" s="74"/>
-      <c r="E81" s="74"/>
-      <c r="F81" s="74"/>
-      <c r="G81" s="75"/>
+      <c r="C81" s="87"/>
+      <c r="D81" s="66"/>
+      <c r="E81" s="66"/>
+      <c r="F81" s="66"/>
+      <c r="G81" s="67"/>
       <c r="H81" s="12" t="s">
         <v>54</v>
       </c>
@@ -5897,11 +5909,11 @@
       <c r="B82" s="27">
         <v>62</v>
       </c>
-      <c r="C82" s="101"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="75"/>
+      <c r="C82" s="87"/>
+      <c r="D82" s="66"/>
+      <c r="E82" s="66"/>
+      <c r="F82" s="66"/>
+      <c r="G82" s="67"/>
       <c r="H82" s="12" t="s">
         <v>54</v>
       </c>
@@ -5910,11 +5922,11 @@
       <c r="B83" s="9">
         <v>63</v>
       </c>
-      <c r="C83" s="101"/>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="74"/>
-      <c r="G83" s="75"/>
+      <c r="C83" s="87"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="66"/>
+      <c r="F83" s="66"/>
+      <c r="G83" s="67"/>
       <c r="H83" s="12" t="s">
         <v>54</v>
       </c>
@@ -5923,11 +5935,11 @@
       <c r="B84" s="27">
         <v>64</v>
       </c>
-      <c r="C84" s="101"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="75"/>
+      <c r="C84" s="87"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="67"/>
       <c r="H84" s="12" t="s">
         <v>54</v>
       </c>
@@ -5936,11 +5948,11 @@
       <c r="B85" s="9">
         <v>65</v>
       </c>
-      <c r="C85" s="101"/>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
-      <c r="F85" s="74"/>
-      <c r="G85" s="75"/>
+      <c r="C85" s="87"/>
+      <c r="D85" s="66"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="67"/>
       <c r="H85" s="12" t="s">
         <v>54</v>
       </c>
@@ -5949,11 +5961,11 @@
       <c r="B86" s="27">
         <v>66</v>
       </c>
-      <c r="C86" s="101"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="75"/>
+      <c r="C86" s="87"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="66"/>
+      <c r="F86" s="66"/>
+      <c r="G86" s="67"/>
       <c r="H86" s="12" t="s">
         <v>54</v>
       </c>
@@ -5962,11 +5974,11 @@
       <c r="B87" s="9">
         <v>67</v>
       </c>
-      <c r="C87" s="101"/>
-      <c r="D87" s="74"/>
-      <c r="E87" s="74"/>
-      <c r="F87" s="74"/>
-      <c r="G87" s="75"/>
+      <c r="C87" s="87"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="66"/>
+      <c r="F87" s="66"/>
+      <c r="G87" s="67"/>
       <c r="H87" s="12" t="s">
         <v>54</v>
       </c>
@@ -5975,11 +5987,11 @@
       <c r="B88" s="27">
         <v>68</v>
       </c>
-      <c r="C88" s="101"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="74"/>
-      <c r="F88" s="74"/>
-      <c r="G88" s="75"/>
+      <c r="C88" s="87"/>
+      <c r="D88" s="66"/>
+      <c r="E88" s="66"/>
+      <c r="F88" s="66"/>
+      <c r="G88" s="67"/>
       <c r="H88" s="12" t="s">
         <v>54</v>
       </c>
@@ -5988,11 +6000,11 @@
       <c r="B89" s="9">
         <v>69</v>
       </c>
-      <c r="C89" s="101"/>
-      <c r="D89" s="74"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="74"/>
-      <c r="G89" s="75"/>
+      <c r="C89" s="87"/>
+      <c r="D89" s="66"/>
+      <c r="E89" s="66"/>
+      <c r="F89" s="66"/>
+      <c r="G89" s="67"/>
       <c r="H89" s="12" t="s">
         <v>54</v>
       </c>
@@ -6001,11 +6013,11 @@
       <c r="B90" s="27">
         <v>70</v>
       </c>
-      <c r="C90" s="101"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
-      <c r="G90" s="75"/>
+      <c r="C90" s="87"/>
+      <c r="D90" s="66"/>
+      <c r="E90" s="66"/>
+      <c r="F90" s="66"/>
+      <c r="G90" s="67"/>
       <c r="H90" s="12" t="s">
         <v>54</v>
       </c>
@@ -6014,11 +6026,11 @@
       <c r="B91" s="9">
         <v>71</v>
       </c>
-      <c r="C91" s="101"/>
-      <c r="D91" s="74"/>
-      <c r="E91" s="74"/>
-      <c r="F91" s="74"/>
-      <c r="G91" s="75"/>
+      <c r="C91" s="87"/>
+      <c r="D91" s="66"/>
+      <c r="E91" s="66"/>
+      <c r="F91" s="66"/>
+      <c r="G91" s="67"/>
       <c r="H91" s="12" t="s">
         <v>54</v>
       </c>
@@ -6027,11 +6039,11 @@
       <c r="B92" s="27">
         <v>72</v>
       </c>
-      <c r="C92" s="101"/>
-      <c r="D92" s="74"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="74"/>
-      <c r="G92" s="75"/>
+      <c r="C92" s="87"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="66"/>
+      <c r="F92" s="66"/>
+      <c r="G92" s="67"/>
       <c r="H92" s="12" t="s">
         <v>54</v>
       </c>
@@ -6040,11 +6052,11 @@
       <c r="B93" s="9">
         <v>73</v>
       </c>
-      <c r="C93" s="101"/>
-      <c r="D93" s="74"/>
-      <c r="E93" s="74"/>
-      <c r="F93" s="74"/>
-      <c r="G93" s="75"/>
+      <c r="C93" s="87"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="66"/>
+      <c r="F93" s="66"/>
+      <c r="G93" s="67"/>
       <c r="H93" s="12" t="s">
         <v>54</v>
       </c>
@@ -6053,11 +6065,11 @@
       <c r="B94" s="27">
         <v>74</v>
       </c>
-      <c r="C94" s="101"/>
-      <c r="D94" s="74"/>
-      <c r="E94" s="74"/>
-      <c r="F94" s="74"/>
-      <c r="G94" s="75"/>
+      <c r="C94" s="87"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="66"/>
+      <c r="F94" s="66"/>
+      <c r="G94" s="67"/>
       <c r="H94" s="12" t="s">
         <v>54</v>
       </c>
@@ -6066,11 +6078,11 @@
       <c r="B95" s="9">
         <v>75</v>
       </c>
-      <c r="C95" s="101"/>
-      <c r="D95" s="74"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="74"/>
-      <c r="G95" s="75"/>
+      <c r="C95" s="87"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="66"/>
+      <c r="F95" s="66"/>
+      <c r="G95" s="67"/>
       <c r="H95" s="12" t="s">
         <v>54</v>
       </c>
@@ -6079,11 +6091,11 @@
       <c r="B96" s="27">
         <v>76</v>
       </c>
-      <c r="C96" s="101"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="75"/>
+      <c r="C96" s="87"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="66"/>
+      <c r="F96" s="66"/>
+      <c r="G96" s="67"/>
       <c r="H96" s="12" t="s">
         <v>54</v>
       </c>
@@ -6092,11 +6104,11 @@
       <c r="B97" s="9">
         <v>77</v>
       </c>
-      <c r="C97" s="101"/>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="75"/>
+      <c r="C97" s="87"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="66"/>
+      <c r="F97" s="66"/>
+      <c r="G97" s="67"/>
       <c r="H97" s="12" t="s">
         <v>54</v>
       </c>
@@ -6105,11 +6117,11 @@
       <c r="B98" s="27">
         <v>78</v>
       </c>
-      <c r="C98" s="101"/>
-      <c r="D98" s="74"/>
-      <c r="E98" s="74"/>
-      <c r="F98" s="74"/>
-      <c r="G98" s="75"/>
+      <c r="C98" s="87"/>
+      <c r="D98" s="66"/>
+      <c r="E98" s="66"/>
+      <c r="F98" s="66"/>
+      <c r="G98" s="67"/>
       <c r="H98" s="12" t="s">
         <v>54</v>
       </c>
@@ -6118,11 +6130,11 @@
       <c r="B99" s="9">
         <v>79</v>
       </c>
-      <c r="C99" s="101"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="74"/>
-      <c r="G99" s="75"/>
+      <c r="C99" s="87"/>
+      <c r="D99" s="66"/>
+      <c r="E99" s="66"/>
+      <c r="F99" s="66"/>
+      <c r="G99" s="67"/>
       <c r="H99" s="12" t="s">
         <v>54</v>
       </c>
@@ -6131,11 +6143,11 @@
       <c r="B100" s="27">
         <v>80</v>
       </c>
-      <c r="C100" s="101"/>
-      <c r="D100" s="74"/>
-      <c r="E100" s="74"/>
-      <c r="F100" s="74"/>
-      <c r="G100" s="75"/>
+      <c r="C100" s="87"/>
+      <c r="D100" s="66"/>
+      <c r="E100" s="66"/>
+      <c r="F100" s="66"/>
+      <c r="G100" s="67"/>
       <c r="H100" s="12" t="s">
         <v>54</v>
       </c>
@@ -6144,11 +6156,11 @@
       <c r="B101" s="9">
         <v>81</v>
       </c>
-      <c r="C101" s="101"/>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="75"/>
+      <c r="C101" s="87"/>
+      <c r="D101" s="66"/>
+      <c r="E101" s="66"/>
+      <c r="F101" s="66"/>
+      <c r="G101" s="67"/>
       <c r="H101" s="12" t="s">
         <v>54</v>
       </c>
@@ -6157,11 +6169,11 @@
       <c r="B102" s="27">
         <v>82</v>
       </c>
-      <c r="C102" s="101"/>
-      <c r="D102" s="74"/>
-      <c r="E102" s="74"/>
-      <c r="F102" s="74"/>
-      <c r="G102" s="75"/>
+      <c r="C102" s="87"/>
+      <c r="D102" s="66"/>
+      <c r="E102" s="66"/>
+      <c r="F102" s="66"/>
+      <c r="G102" s="67"/>
       <c r="H102" s="12" t="s">
         <v>54</v>
       </c>
@@ -6170,11 +6182,11 @@
       <c r="B103" s="9">
         <v>83</v>
       </c>
-      <c r="C103" s="101"/>
-      <c r="D103" s="74"/>
-      <c r="E103" s="74"/>
-      <c r="F103" s="74"/>
-      <c r="G103" s="75"/>
+      <c r="C103" s="87"/>
+      <c r="D103" s="66"/>
+      <c r="E103" s="66"/>
+      <c r="F103" s="66"/>
+      <c r="G103" s="67"/>
       <c r="H103" s="12" t="s">
         <v>54</v>
       </c>
@@ -6183,11 +6195,11 @@
       <c r="B104" s="27">
         <v>84</v>
       </c>
-      <c r="C104" s="101"/>
-      <c r="D104" s="74"/>
-      <c r="E104" s="74"/>
-      <c r="F104" s="74"/>
-      <c r="G104" s="75"/>
+      <c r="C104" s="87"/>
+      <c r="D104" s="66"/>
+      <c r="E104" s="66"/>
+      <c r="F104" s="66"/>
+      <c r="G104" s="67"/>
       <c r="H104" s="12" t="s">
         <v>54</v>
       </c>
@@ -6196,11 +6208,11 @@
       <c r="B105" s="9">
         <v>85</v>
       </c>
-      <c r="C105" s="101"/>
-      <c r="D105" s="74"/>
-      <c r="E105" s="74"/>
-      <c r="F105" s="74"/>
-      <c r="G105" s="75"/>
+      <c r="C105" s="87"/>
+      <c r="D105" s="66"/>
+      <c r="E105" s="66"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="67"/>
       <c r="H105" s="12" t="s">
         <v>54</v>
       </c>
@@ -6209,11 +6221,11 @@
       <c r="B106" s="27">
         <v>86</v>
       </c>
-      <c r="C106" s="101"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="75"/>
+      <c r="C106" s="87"/>
+      <c r="D106" s="66"/>
+      <c r="E106" s="66"/>
+      <c r="F106" s="66"/>
+      <c r="G106" s="67"/>
       <c r="H106" s="12" t="s">
         <v>54</v>
       </c>
@@ -6222,11 +6234,11 @@
       <c r="B107" s="9">
         <v>87</v>
       </c>
-      <c r="C107" s="101"/>
-      <c r="D107" s="74"/>
-      <c r="E107" s="74"/>
-      <c r="F107" s="74"/>
-      <c r="G107" s="75"/>
+      <c r="C107" s="87"/>
+      <c r="D107" s="66"/>
+      <c r="E107" s="66"/>
+      <c r="F107" s="66"/>
+      <c r="G107" s="67"/>
       <c r="H107" s="12" t="s">
         <v>54</v>
       </c>
@@ -6235,11 +6247,11 @@
       <c r="B108" s="27">
         <v>88</v>
       </c>
-      <c r="C108" s="101"/>
-      <c r="D108" s="74"/>
-      <c r="E108" s="74"/>
-      <c r="F108" s="74"/>
-      <c r="G108" s="75"/>
+      <c r="C108" s="87"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="66"/>
+      <c r="F108" s="66"/>
+      <c r="G108" s="67"/>
       <c r="H108" s="12" t="s">
         <v>54</v>
       </c>
@@ -6248,11 +6260,11 @@
       <c r="B109" s="9">
         <v>89</v>
       </c>
-      <c r="C109" s="101"/>
-      <c r="D109" s="74"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
-      <c r="G109" s="75"/>
+      <c r="C109" s="87"/>
+      <c r="D109" s="66"/>
+      <c r="E109" s="66"/>
+      <c r="F109" s="66"/>
+      <c r="G109" s="67"/>
       <c r="H109" s="12" t="s">
         <v>54</v>
       </c>
@@ -6261,11 +6273,11 @@
       <c r="B110" s="27">
         <v>90</v>
       </c>
-      <c r="C110" s="101"/>
-      <c r="D110" s="74"/>
-      <c r="E110" s="74"/>
-      <c r="F110" s="74"/>
-      <c r="G110" s="75"/>
+      <c r="C110" s="87"/>
+      <c r="D110" s="66"/>
+      <c r="E110" s="66"/>
+      <c r="F110" s="66"/>
+      <c r="G110" s="67"/>
       <c r="H110" s="12" t="s">
         <v>54</v>
       </c>
@@ -6274,11 +6286,11 @@
       <c r="B111" s="9">
         <v>91</v>
       </c>
-      <c r="C111" s="101"/>
-      <c r="D111" s="74"/>
-      <c r="E111" s="74"/>
-      <c r="F111" s="74"/>
-      <c r="G111" s="75"/>
+      <c r="C111" s="87"/>
+      <c r="D111" s="66"/>
+      <c r="E111" s="66"/>
+      <c r="F111" s="66"/>
+      <c r="G111" s="67"/>
       <c r="H111" s="12" t="s">
         <v>54</v>
       </c>
@@ -6287,11 +6299,11 @@
       <c r="B112" s="27">
         <v>92</v>
       </c>
-      <c r="C112" s="101"/>
-      <c r="D112" s="74"/>
-      <c r="E112" s="74"/>
-      <c r="F112" s="74"/>
-      <c r="G112" s="75"/>
+      <c r="C112" s="87"/>
+      <c r="D112" s="66"/>
+      <c r="E112" s="66"/>
+      <c r="F112" s="66"/>
+      <c r="G112" s="67"/>
       <c r="H112" s="12" t="s">
         <v>54</v>
       </c>
@@ -6300,11 +6312,11 @@
       <c r="B113" s="9">
         <v>93</v>
       </c>
-      <c r="C113" s="101"/>
-      <c r="D113" s="74"/>
-      <c r="E113" s="74"/>
-      <c r="F113" s="74"/>
-      <c r="G113" s="75"/>
+      <c r="C113" s="87"/>
+      <c r="D113" s="66"/>
+      <c r="E113" s="66"/>
+      <c r="F113" s="66"/>
+      <c r="G113" s="67"/>
       <c r="H113" s="12" t="s">
         <v>54</v>
       </c>
@@ -6313,11 +6325,11 @@
       <c r="B114" s="27">
         <v>94</v>
       </c>
-      <c r="C114" s="101"/>
-      <c r="D114" s="74"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
-      <c r="G114" s="75"/>
+      <c r="C114" s="87"/>
+      <c r="D114" s="66"/>
+      <c r="E114" s="66"/>
+      <c r="F114" s="66"/>
+      <c r="G114" s="67"/>
       <c r="H114" s="12" t="s">
         <v>54</v>
       </c>
@@ -6326,11 +6338,11 @@
       <c r="B115" s="9">
         <v>95</v>
       </c>
-      <c r="C115" s="101"/>
-      <c r="D115" s="74"/>
-      <c r="E115" s="74"/>
-      <c r="F115" s="74"/>
-      <c r="G115" s="75"/>
+      <c r="C115" s="87"/>
+      <c r="D115" s="66"/>
+      <c r="E115" s="66"/>
+      <c r="F115" s="66"/>
+      <c r="G115" s="67"/>
       <c r="H115" s="12" t="s">
         <v>54</v>
       </c>
@@ -6339,11 +6351,11 @@
       <c r="B116" s="27">
         <v>96</v>
       </c>
-      <c r="C116" s="101"/>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
-      <c r="G116" s="75"/>
+      <c r="C116" s="87"/>
+      <c r="D116" s="66"/>
+      <c r="E116" s="66"/>
+      <c r="F116" s="66"/>
+      <c r="G116" s="67"/>
       <c r="H116" s="12" t="s">
         <v>54</v>
       </c>
@@ -6352,11 +6364,11 @@
       <c r="B117" s="9">
         <v>97</v>
       </c>
-      <c r="C117" s="101"/>
-      <c r="D117" s="74"/>
-      <c r="E117" s="74"/>
-      <c r="F117" s="74"/>
-      <c r="G117" s="75"/>
+      <c r="C117" s="87"/>
+      <c r="D117" s="66"/>
+      <c r="E117" s="66"/>
+      <c r="F117" s="66"/>
+      <c r="G117" s="67"/>
       <c r="H117" s="12" t="s">
         <v>54</v>
       </c>
@@ -6365,11 +6377,11 @@
       <c r="B118" s="27">
         <v>98</v>
       </c>
-      <c r="C118" s="101"/>
-      <c r="D118" s="74"/>
-      <c r="E118" s="74"/>
-      <c r="F118" s="74"/>
-      <c r="G118" s="75"/>
+      <c r="C118" s="87"/>
+      <c r="D118" s="66"/>
+      <c r="E118" s="66"/>
+      <c r="F118" s="66"/>
+      <c r="G118" s="67"/>
       <c r="H118" s="12" t="s">
         <v>54</v>
       </c>
@@ -6378,11 +6390,11 @@
       <c r="B119" s="9">
         <v>99</v>
       </c>
-      <c r="C119" s="101"/>
-      <c r="D119" s="74"/>
-      <c r="E119" s="74"/>
-      <c r="F119" s="74"/>
-      <c r="G119" s="75"/>
+      <c r="C119" s="87"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="67"/>
       <c r="H119" s="12" t="s">
         <v>54</v>
       </c>
@@ -6391,11 +6403,11 @@
       <c r="B120" s="27">
         <v>100</v>
       </c>
-      <c r="C120" s="101"/>
-      <c r="D120" s="74"/>
-      <c r="E120" s="74"/>
-      <c r="F120" s="74"/>
-      <c r="G120" s="75"/>
+      <c r="C120" s="87"/>
+      <c r="D120" s="66"/>
+      <c r="E120" s="66"/>
+      <c r="F120" s="66"/>
+      <c r="G120" s="67"/>
       <c r="H120" s="12" t="s">
         <v>54</v>
       </c>
@@ -8074,53 +8086,50 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
@@ -8145,52 +8154,55 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C95:G95"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H120" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$B$212:$B$214</formula1>
     </dataValidation>
@@ -8238,85 +8250,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="2">
         <f>Requisitos!C11</f>
         <v>45170</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K65" si="0">K1+1</f>
         <v>45171</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45172</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45173</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45174</v>
@@ -8330,18 +8342,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="77" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45176</v>
@@ -8355,16 +8367,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="57" t="s">
         <v>67</v>
       </c>
@@ -9735,30 +9747,30 @@
       </c>
     </row>
     <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="108" t="s">
+      <c r="B63" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="75"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="67"/>
       <c r="K63" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
       </c>
     </row>
     <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="109" t="s">
+      <c r="B64" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="74"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="75"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="67"/>
       <c r="H64" s="7" t="s">
         <v>101</v>
       </c>
@@ -9771,15 +9783,15 @@
       </c>
     </row>
     <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="107" t="str">
+      <c r="B65" s="98" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="74"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="75"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="67"/>
       <c r="H65" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B10,H$11:H$60)</f>
         <v>0</v>
@@ -9794,15 +9806,15 @@
       </c>
     </row>
     <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="107" t="str">
+      <c r="B66" s="98" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="66"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="67"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -9817,15 +9829,15 @@
       </c>
     </row>
     <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="107" t="str">
+      <c r="B67" s="98" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="75"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="66"/>
+      <c r="G67" s="67"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -9840,15 +9852,15 @@
       </c>
     </row>
     <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="107" t="str">
+      <c r="B68" s="98" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v>Maria Eduarda Amaral</v>
       </c>
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="67"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -9863,15 +9875,15 @@
       </c>
     </row>
     <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="107" t="str">
+      <c r="B69" s="98" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C69" s="74"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="66"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="67"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -9886,15 +9898,15 @@
       </c>
     </row>
     <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="107" t="str">
+      <c r="B70" s="98" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="75"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="67"/>
       <c r="H70" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -11022,7 +11034,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -11043,85 +11055,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="2">
         <f>Requisitos!C12</f>
         <v>45191</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45192</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45193</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45194</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45195</v>
@@ -11135,18 +11147,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="77" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45197</v>
@@ -11160,16 +11172,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="57" t="s">
         <v>67</v>
       </c>
@@ -12535,26 +12547,26 @@
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="108" t="s">
+      <c r="B72" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="74"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="75"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="67"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="109" t="s">
+      <c r="B73" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="67"/>
       <c r="H73" s="7" t="s">
         <v>101</v>
       </c>
@@ -12563,15 +12575,15 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="107" t="str">
+      <c r="B74" s="98" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="67"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -12582,15 +12594,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="107" t="str">
+      <c r="B75" s="98" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="67"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -12601,15 +12613,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="107" t="str">
+      <c r="B76" s="98" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="67"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -12620,15 +12632,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="107" t="str">
+      <c r="B77" s="98" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="74"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -12639,15 +12651,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="107" t="str">
+      <c r="B78" s="98" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="67"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -13878,7 +13890,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13898,85 +13910,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="2">
         <f>Requisitos!C13</f>
         <v>45205</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K22" si="0">K1+1</f>
         <v>45206</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45207</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45208</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45209</v>
@@ -13990,18 +14002,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="77" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45211</v>
@@ -14015,16 +14027,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="57" t="s">
         <v>67</v>
       </c>
@@ -14218,7 +14230,7 @@
         <v>11</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H15" s="13">
         <v>0</v>
@@ -14249,7 +14261,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
@@ -14273,7 +14285,7 @@
         <v>14</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H17" s="13">
         <v>0</v>
@@ -14304,7 +14316,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H18" s="13">
         <v>0</v>
@@ -14335,7 +14347,7 @@
         <v>14</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H19" s="13">
         <v>0</v>
@@ -14366,7 +14378,7 @@
         <v>14</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H20" s="13">
         <v>0</v>
@@ -14397,7 +14409,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H21" s="13">
         <v>0</v>
@@ -14428,7 +14440,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H22" s="13">
         <v>0</v>
@@ -14546,7 +14558,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="41" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="H26" s="13">
         <v>0</v>
@@ -14574,7 +14586,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H27" s="13">
         <v>0</v>
@@ -14602,7 +14614,7 @@
         <v>11</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H28" s="13">
         <v>0</v>
@@ -15353,31 +15365,31 @@
       <c r="F72" s="30"/>
       <c r="G72" s="30">
         <f>COUNTIFS(G11:G61, "Concluído",D11:D61, "&lt;&gt;"&amp;"")</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="108" t="s">
+      <c r="B73" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="74"/>
-      <c r="H73" s="74"/>
-      <c r="I73" s="75"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="67"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="109" t="s">
+      <c r="B74" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="67"/>
       <c r="H74" s="7" t="s">
         <v>101</v>
       </c>
@@ -15386,15 +15398,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="107" t="str">
+      <c r="B75" s="98" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="67"/>
       <c r="H75" s="33">
         <f>SUMIF($F$11:$F$61,'Dados do Projeto'!$B10,H$11:H$61)</f>
         <v>0</v>
@@ -15405,15 +15417,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="107" t="str">
+      <c r="B76" s="98" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="67"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B11,H$11:H$61)</f>
         <v>0</v>
@@ -15424,15 +15436,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="107" t="str">
+      <c r="B77" s="98" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C77" s="74"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B12,H$11:H$61)</f>
         <v>0</v>
@@ -15443,15 +15455,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="107" t="str">
+      <c r="B78" s="98" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="67"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B14,H$11:H$61)</f>
         <v>0</v>
@@ -15462,15 +15474,15 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="107" t="str">
+      <c r="B79" s="98" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C79" s="74"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="75"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="67"/>
       <c r="H79" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B15,H$11:H$61)</f>
         <v>0</v>
@@ -16494,12 +16506,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B79:G79"/>
     <mergeCell ref="B9:I9"/>
@@ -16508,6 +16514,12 @@
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
     <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C70">
     <cfRule type="expression" dxfId="83" priority="31">
@@ -16645,9 +16657,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16667,85 +16679,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="2">
         <f>Requisitos!C14</f>
         <v>45226</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>45227</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45228</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45229</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45230</v>
@@ -16759,18 +16771,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="77" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -16784,16 +16796,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="57" t="s">
         <v>67</v>
       </c>
@@ -17930,26 +17942,26 @@
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="108" t="s">
+      <c r="B72" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="74"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="75"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="67"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="109" t="s">
+      <c r="B73" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="67"/>
       <c r="H73" s="7" t="s">
         <v>101</v>
       </c>
@@ -17958,15 +17970,15 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="107" t="str">
+      <c r="B74" s="98" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="67"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -17977,15 +17989,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="107" t="str">
+      <c r="B75" s="98" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="67"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -17996,15 +18008,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="107" t="str">
+      <c r="B76" s="98" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="67"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -18015,15 +18027,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="107" t="str">
+      <c r="B77" s="98" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="74"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -18034,15 +18046,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="107" t="str">
+      <c r="B78" s="98" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="67"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -19066,12 +19078,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B9:I9"/>
@@ -19080,6 +19086,12 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F20:F25">
     <cfRule type="expression" dxfId="63" priority="1">
@@ -19265,85 +19277,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="2">
         <f>Requisitos!C15</f>
         <v>45247</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45248</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45249</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45250</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45251</v>
@@ -19356,18 +19368,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="73" t="str">
+      <c r="B7" s="77" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45253</v>
@@ -19380,16 +19392,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="58" t="s">
         <v>67</v>
       </c>
@@ -20350,26 +20362,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="108" t="s">
+      <c r="B63" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="75"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="67"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="109" t="s">
+      <c r="B64" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="74"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="75"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="67"/>
       <c r="H64" s="7" t="s">
         <v>101</v>
       </c>
@@ -20378,15 +20390,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="107" t="str">
+      <c r="B65" s="98" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="74"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="75"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="67"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -20397,15 +20409,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="107" t="str">
+      <c r="B66" s="98" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="66"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="67"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -20416,15 +20428,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="107" t="str">
+      <c r="B67" s="98" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="75"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="66"/>
+      <c r="G67" s="67"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -20435,15 +20447,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="107" t="str">
+      <c r="B68" s="98" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="67"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -20454,15 +20466,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="107" t="str">
+      <c r="B69" s="98" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C69" s="74"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="66"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="67"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -21425,12 +21437,6 @@
   </sheetData>
   <autoFilter ref="B10:J60" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B9:I9"/>
@@ -21439,6 +21445,12 @@
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F17">
     <cfRule type="containsBlanks" dxfId="37" priority="1">

</xml_diff>

<commit_message>
doc: update planejamento_sprints #87
</commit_message>
<xml_diff>
--- a/Artefatos/sprints/Planejamento_sprints.xlsx
+++ b/Artefatos/sprints/Planejamento_sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositorios_github\plf-es-2023-2-ti3-6653100-fabrica-do-saber\Artefatos\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80B27C7-78EB-471A-BE14-D6AC8380A759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C8729F-EAB3-4FB0-95DA-1A6CD6A55225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,7 +896,7 @@
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mmm"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mmm&quot;/&quot;yyyy&quot; &quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1071,6 +1071,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1341,7 +1347,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1538,22 +1544,56 @@
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1563,74 +1603,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1647,6 +1632,15 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1655,6 +1649,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3319,166 +3340,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
     </row>
     <row r="3" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="98"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="99" t="s">
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="90" t="s">
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="106"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="97"/>
-      <c r="F11" s="90" t="s">
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="91"/>
-      <c r="H11" s="92"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="106"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="90" t="s">
+      <c r="C12" s="97"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="91"/>
-      <c r="H12" s="92"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="106"/>
       <c r="K12" s="47"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="90" t="s">
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="106"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="90" t="s">
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="106"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="90" t="s">
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="91"/>
-      <c r="H15" s="92"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="106"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="18"/>
@@ -3580,16 +3601,16 @@
     <row r="99" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="50"/>
-      <c r="B100" s="93"/>
-      <c r="C100" s="85"/>
-      <c r="D100" s="94" t="s">
+      <c r="B100" s="108"/>
+      <c r="C100" s="93"/>
+      <c r="D100" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E100" s="85"/>
-      <c r="F100" s="94" t="s">
+      <c r="E100" s="93"/>
+      <c r="F100" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="G100" s="85"/>
+      <c r="G100" s="93"/>
       <c r="H100" s="51" t="s">
         <v>18</v>
       </c>
@@ -3611,12 +3632,12 @@
     </row>
     <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
-      <c r="B101" s="84"/>
-      <c r="C101" s="85"/>
-      <c r="D101" s="89" t="s">
+      <c r="B101" s="111"/>
+      <c r="C101" s="93"/>
+      <c r="D101" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="85"/>
+      <c r="E101" s="93"/>
       <c r="F101" s="53" t="s">
         <v>24</v>
       </c>
@@ -3649,12 +3670,12 @@
     </row>
     <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
-      <c r="B102" s="84"/>
-      <c r="C102" s="85"/>
-      <c r="D102" s="89" t="s">
+      <c r="B102" s="111"/>
+      <c r="C102" s="93"/>
+      <c r="D102" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E102" s="85"/>
+      <c r="E102" s="93"/>
       <c r="F102" s="53" t="s">
         <v>29</v>
       </c>
@@ -3688,12 +3709,12 @@
     </row>
     <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="50"/>
-      <c r="B103" s="84"/>
-      <c r="C103" s="85"/>
-      <c r="D103" s="89" t="s">
+      <c r="B103" s="111"/>
+      <c r="C103" s="93"/>
+      <c r="D103" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="85"/>
+      <c r="E103" s="93"/>
       <c r="F103" s="53"/>
       <c r="G103" s="54" t="s">
         <v>34</v>
@@ -3725,12 +3746,12 @@
     </row>
     <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="50"/>
-      <c r="B104" s="84"/>
-      <c r="C104" s="85"/>
-      <c r="D104" s="89" t="s">
+      <c r="B104" s="111"/>
+      <c r="C104" s="93"/>
+      <c r="D104" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="85"/>
+      <c r="E104" s="93"/>
       <c r="F104" s="53"/>
       <c r="G104" s="54" t="s">
         <v>36</v>
@@ -3760,12 +3781,12 @@
     </row>
     <row r="105" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="50"/>
-      <c r="B105" s="84"/>
-      <c r="C105" s="85"/>
-      <c r="D105" s="89" t="s">
+      <c r="B105" s="111"/>
+      <c r="C105" s="93"/>
+      <c r="D105" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="E105" s="85"/>
+      <c r="E105" s="93"/>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="s">
         <v>39</v>
@@ -3790,8 +3811,8 @@
     </row>
     <row r="106" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="50"/>
-      <c r="B106" s="84"/>
-      <c r="C106" s="85"/>
+      <c r="B106" s="111"/>
+      <c r="C106" s="93"/>
       <c r="F106" s="53"/>
       <c r="G106" s="54"/>
       <c r="H106" s="53"/>
@@ -3802,8 +3823,8 @@
     </row>
     <row r="107" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="50"/>
-      <c r="B107" s="84"/>
-      <c r="C107" s="85"/>
+      <c r="B107" s="111"/>
+      <c r="C107" s="93"/>
       <c r="D107" s="55"/>
       <c r="E107" s="53"/>
       <c r="F107" s="53"/>
@@ -4771,24 +4792,12 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D105:E105"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B100:C100"/>
     <mergeCell ref="D100:E100"/>
@@ -4800,12 +4809,24 @@
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="F10:F15" xr:uid="{49EDF03A-7EFB-435C-A992-40D98DE85B41}">
@@ -4831,7 +4852,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:G31"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4848,59 +4869,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="98"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -4912,16 +4933,16 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="125" t="str">
+      <c r="B7" s="121" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -4933,15 +4954,15 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
@@ -4953,11 +4974,11 @@
       <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="127" t="s">
+      <c r="E10" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="87"/>
-      <c r="G10" s="88"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="101"/>
       <c r="H10" s="6" t="s">
         <v>45</v>
       </c>
@@ -4972,9 +4993,9 @@
       <c r="D11" s="14">
         <v>45190</v>
       </c>
-      <c r="E11" s="120"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="88"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="101"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4988,9 +5009,9 @@
         <f t="shared" ref="D12" si="0">C12+13</f>
         <v>45204</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5004,9 +5025,9 @@
       <c r="D13" s="14">
         <v>45225</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="88"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="101"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5019,9 +5040,9 @@
       <c r="D14" s="14">
         <v>45246</v>
       </c>
-      <c r="E14" s="121"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5060,13 +5081,13 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
       <c r="H18" s="22" t="s">
         <v>47</v>
       </c>
@@ -5075,11 +5096,11 @@
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="123"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="88"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="101"/>
       <c r="H19" s="25" t="s">
         <v>48</v>
       </c>
@@ -5089,11 +5110,11 @@
       <c r="B20" s="27">
         <v>0</v>
       </c>
-      <c r="C20" s="124"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="88"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="101"/>
       <c r="H20" s="28"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -5110,13 +5131,13 @@
       <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="111"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="120"/>
       <c r="H21" s="61" t="s">
         <v>50</v>
       </c>
@@ -5126,13 +5147,13 @@
       <c r="B22" s="27">
         <v>2</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="111"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="120"/>
       <c r="H22" s="61" t="s">
         <v>50</v>
       </c>
@@ -5141,13 +5162,13 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="111"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="120"/>
       <c r="H23" s="61" t="s">
         <v>50</v>
       </c>
@@ -5156,28 +5177,28 @@
       <c r="B24" s="27">
         <v>4</v>
       </c>
-      <c r="C24" s="114" t="s">
+      <c r="C24" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="115"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="116"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="126"/>
       <c r="H24" s="62" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="108" t="s">
+      <c r="C25" s="127" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="113"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="129"/>
       <c r="H25" s="12" t="s">
         <v>54</v>
       </c>
@@ -5186,13 +5207,13 @@
       <c r="B26" s="27">
         <v>6</v>
       </c>
-      <c r="C26" s="108" t="s">
+      <c r="C26" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="113"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="129"/>
       <c r="H26" s="12" t="s">
         <v>54</v>
       </c>
@@ -5201,13 +5222,13 @@
       <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="111"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="119"/>
+      <c r="F27" s="119"/>
+      <c r="G27" s="120"/>
       <c r="H27" s="61" t="s">
         <v>50</v>
       </c>
@@ -5216,28 +5237,28 @@
       <c r="B28" s="27">
         <v>8</v>
       </c>
-      <c r="C28" s="114" t="s">
+      <c r="C28" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="115"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="116"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="125"/>
+      <c r="G28" s="126"/>
       <c r="H28" s="62" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="109" t="s">
+      <c r="C29" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="111"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
+      <c r="G29" s="120"/>
       <c r="H29" s="61" t="s">
         <v>58</v>
       </c>
@@ -5246,14 +5267,14 @@
       <c r="B30" s="27">
         <v>10</v>
       </c>
-      <c r="C30" s="117" t="s">
+      <c r="C30" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="83" t="s">
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="82" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5261,28 +5282,28 @@
       <c r="B31" s="9">
         <v>11</v>
       </c>
-      <c r="C31" s="114" t="s">
+      <c r="C31" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="82" t="s">
-        <v>54</v>
+      <c r="D31" s="125"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="125"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="62" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="27">
         <v>12</v>
       </c>
-      <c r="C32" s="109" t="s">
+      <c r="C32" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="111"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="119"/>
+      <c r="F32" s="119"/>
+      <c r="G32" s="120"/>
       <c r="H32" s="61" t="s">
         <v>50</v>
       </c>
@@ -5291,11 +5312,11 @@
       <c r="B33" s="9">
         <v>13</v>
       </c>
-      <c r="C33" s="108"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="113"/>
+      <c r="C33" s="127"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="129"/>
       <c r="H33" s="12" t="s">
         <v>54</v>
       </c>
@@ -5304,11 +5325,11 @@
       <c r="B34" s="27">
         <v>14</v>
       </c>
-      <c r="C34" s="108"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="113"/>
+      <c r="C34" s="127"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="12" t="s">
         <v>54</v>
       </c>
@@ -5317,11 +5338,11 @@
       <c r="B35" s="9">
         <v>15</v>
       </c>
-      <c r="C35" s="108"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="113"/>
+      <c r="C35" s="127"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="129"/>
       <c r="H35" s="12" t="s">
         <v>54</v>
       </c>
@@ -5330,11 +5351,11 @@
       <c r="B36" s="27">
         <v>16</v>
       </c>
-      <c r="C36" s="108"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="88"/>
+      <c r="C36" s="127"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="100"/>
+      <c r="F36" s="100"/>
+      <c r="G36" s="101"/>
       <c r="H36" s="12" t="s">
         <v>54</v>
       </c>
@@ -5343,11 +5364,11 @@
       <c r="B37" s="9">
         <v>17</v>
       </c>
-      <c r="C37" s="108"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="88"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
       <c r="H37" s="12" t="s">
         <v>54</v>
       </c>
@@ -5356,11 +5377,11 @@
       <c r="B38" s="27">
         <v>18</v>
       </c>
-      <c r="C38" s="108"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="88"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="100"/>
+      <c r="E38" s="100"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
       <c r="H38" s="12" t="s">
         <v>54</v>
       </c>
@@ -5369,11 +5390,11 @@
       <c r="B39" s="9">
         <v>19</v>
       </c>
-      <c r="C39" s="108"/>
-      <c r="D39" s="87"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="88"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="100"/>
+      <c r="F39" s="100"/>
+      <c r="G39" s="101"/>
       <c r="H39" s="12" t="s">
         <v>54</v>
       </c>
@@ -5382,11 +5403,11 @@
       <c r="B40" s="27">
         <v>20</v>
       </c>
-      <c r="C40" s="108"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="88"/>
+      <c r="C40" s="127"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="101"/>
       <c r="H40" s="12" t="s">
         <v>54</v>
       </c>
@@ -5395,11 +5416,11 @@
       <c r="B41" s="9">
         <v>21</v>
       </c>
-      <c r="C41" s="108"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="88"/>
+      <c r="C41" s="127"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="101"/>
       <c r="H41" s="12" t="s">
         <v>54</v>
       </c>
@@ -5408,11 +5429,11 @@
       <c r="B42" s="27">
         <v>22</v>
       </c>
-      <c r="C42" s="108"/>
-      <c r="D42" s="87"/>
-      <c r="E42" s="87"/>
-      <c r="F42" s="87"/>
-      <c r="G42" s="88"/>
+      <c r="C42" s="127"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="101"/>
       <c r="H42" s="12" t="s">
         <v>54</v>
       </c>
@@ -5421,11 +5442,11 @@
       <c r="B43" s="9">
         <v>23</v>
       </c>
-      <c r="C43" s="108"/>
-      <c r="D43" s="87"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="88"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="101"/>
       <c r="H43" s="12" t="s">
         <v>54</v>
       </c>
@@ -5434,11 +5455,11 @@
       <c r="B44" s="27">
         <v>24</v>
       </c>
-      <c r="C44" s="108"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="87"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="88"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="100"/>
+      <c r="E44" s="100"/>
+      <c r="F44" s="100"/>
+      <c r="G44" s="101"/>
       <c r="H44" s="12" t="s">
         <v>54</v>
       </c>
@@ -5447,11 +5468,11 @@
       <c r="B45" s="9">
         <v>25</v>
       </c>
-      <c r="C45" s="108"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-      <c r="F45" s="87"/>
-      <c r="G45" s="88"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="100"/>
+      <c r="E45" s="100"/>
+      <c r="F45" s="100"/>
+      <c r="G45" s="101"/>
       <c r="H45" s="12" t="s">
         <v>54</v>
       </c>
@@ -5460,11 +5481,11 @@
       <c r="B46" s="27">
         <v>26</v>
       </c>
-      <c r="C46" s="108"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="87"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="88"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="100"/>
+      <c r="E46" s="100"/>
+      <c r="F46" s="100"/>
+      <c r="G46" s="101"/>
       <c r="H46" s="12" t="s">
         <v>54</v>
       </c>
@@ -5473,11 +5494,11 @@
       <c r="B47" s="9">
         <v>27</v>
       </c>
-      <c r="C47" s="108"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="87"/>
-      <c r="G47" s="88"/>
+      <c r="C47" s="127"/>
+      <c r="D47" s="100"/>
+      <c r="E47" s="100"/>
+      <c r="F47" s="100"/>
+      <c r="G47" s="101"/>
       <c r="H47" s="12" t="s">
         <v>54</v>
       </c>
@@ -5486,11 +5507,11 @@
       <c r="B48" s="27">
         <v>28</v>
       </c>
-      <c r="C48" s="108"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="88"/>
+      <c r="C48" s="127"/>
+      <c r="D48" s="100"/>
+      <c r="E48" s="100"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="101"/>
       <c r="H48" s="12" t="s">
         <v>54</v>
       </c>
@@ -5499,11 +5520,11 @@
       <c r="B49" s="9">
         <v>29</v>
       </c>
-      <c r="C49" s="108"/>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="87"/>
-      <c r="G49" s="88"/>
+      <c r="C49" s="127"/>
+      <c r="D49" s="100"/>
+      <c r="E49" s="100"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="101"/>
       <c r="H49" s="12" t="s">
         <v>54</v>
       </c>
@@ -5512,11 +5533,11 @@
       <c r="B50" s="27">
         <v>30</v>
       </c>
-      <c r="C50" s="108"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="87"/>
-      <c r="G50" s="88"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="100"/>
+      <c r="E50" s="100"/>
+      <c r="F50" s="100"/>
+      <c r="G50" s="101"/>
       <c r="H50" s="12" t="s">
         <v>54</v>
       </c>
@@ -5525,11 +5546,11 @@
       <c r="B51" s="9">
         <v>31</v>
       </c>
-      <c r="C51" s="108"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="88"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="100"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="100"/>
+      <c r="G51" s="101"/>
       <c r="H51" s="12" t="s">
         <v>54</v>
       </c>
@@ -5538,11 +5559,11 @@
       <c r="B52" s="27">
         <v>32</v>
       </c>
-      <c r="C52" s="108"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="88"/>
+      <c r="C52" s="127"/>
+      <c r="D52" s="100"/>
+      <c r="E52" s="100"/>
+      <c r="F52" s="100"/>
+      <c r="G52" s="101"/>
       <c r="H52" s="12" t="s">
         <v>54</v>
       </c>
@@ -5551,11 +5572,11 @@
       <c r="B53" s="9">
         <v>33</v>
       </c>
-      <c r="C53" s="108"/>
-      <c r="D53" s="87"/>
-      <c r="E53" s="87"/>
-      <c r="F53" s="87"/>
-      <c r="G53" s="88"/>
+      <c r="C53" s="127"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="100"/>
+      <c r="G53" s="101"/>
       <c r="H53" s="12" t="s">
         <v>54</v>
       </c>
@@ -5564,11 +5585,11 @@
       <c r="B54" s="27">
         <v>34</v>
       </c>
-      <c r="C54" s="108"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="87"/>
-      <c r="F54" s="87"/>
-      <c r="G54" s="88"/>
+      <c r="C54" s="127"/>
+      <c r="D54" s="100"/>
+      <c r="E54" s="100"/>
+      <c r="F54" s="100"/>
+      <c r="G54" s="101"/>
       <c r="H54" s="12" t="s">
         <v>54</v>
       </c>
@@ -5577,11 +5598,11 @@
       <c r="B55" s="9">
         <v>35</v>
       </c>
-      <c r="C55" s="108"/>
-      <c r="D55" s="87"/>
-      <c r="E55" s="87"/>
-      <c r="F55" s="87"/>
-      <c r="G55" s="88"/>
+      <c r="C55" s="127"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="101"/>
       <c r="H55" s="12" t="s">
         <v>54</v>
       </c>
@@ -5590,11 +5611,11 @@
       <c r="B56" s="27">
         <v>36</v>
       </c>
-      <c r="C56" s="108"/>
-      <c r="D56" s="87"/>
-      <c r="E56" s="87"/>
-      <c r="F56" s="87"/>
-      <c r="G56" s="88"/>
+      <c r="C56" s="127"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="100"/>
+      <c r="F56" s="100"/>
+      <c r="G56" s="101"/>
       <c r="H56" s="12" t="s">
         <v>54</v>
       </c>
@@ -5603,11 +5624,11 @@
       <c r="B57" s="9">
         <v>37</v>
       </c>
-      <c r="C57" s="108"/>
-      <c r="D57" s="87"/>
-      <c r="E57" s="87"/>
-      <c r="F57" s="87"/>
-      <c r="G57" s="88"/>
+      <c r="C57" s="127"/>
+      <c r="D57" s="100"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="100"/>
+      <c r="G57" s="101"/>
       <c r="H57" s="12" t="s">
         <v>54</v>
       </c>
@@ -5616,11 +5637,11 @@
       <c r="B58" s="27">
         <v>38</v>
       </c>
-      <c r="C58" s="108"/>
-      <c r="D58" s="87"/>
-      <c r="E58" s="87"/>
-      <c r="F58" s="87"/>
-      <c r="G58" s="88"/>
+      <c r="C58" s="127"/>
+      <c r="D58" s="100"/>
+      <c r="E58" s="100"/>
+      <c r="F58" s="100"/>
+      <c r="G58" s="101"/>
       <c r="H58" s="12" t="s">
         <v>54</v>
       </c>
@@ -5629,11 +5650,11 @@
       <c r="B59" s="9">
         <v>39</v>
       </c>
-      <c r="C59" s="108"/>
-      <c r="D59" s="87"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="87"/>
-      <c r="G59" s="88"/>
+      <c r="C59" s="127"/>
+      <c r="D59" s="100"/>
+      <c r="E59" s="100"/>
+      <c r="F59" s="100"/>
+      <c r="G59" s="101"/>
       <c r="H59" s="12" t="s">
         <v>54</v>
       </c>
@@ -5642,11 +5663,11 @@
       <c r="B60" s="27">
         <v>40</v>
       </c>
-      <c r="C60" s="108"/>
-      <c r="D60" s="87"/>
-      <c r="E60" s="87"/>
-      <c r="F60" s="87"/>
-      <c r="G60" s="88"/>
+      <c r="C60" s="127"/>
+      <c r="D60" s="100"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="100"/>
+      <c r="G60" s="101"/>
       <c r="H60" s="12" t="s">
         <v>54</v>
       </c>
@@ -5655,11 +5676,11 @@
       <c r="B61" s="9">
         <v>41</v>
       </c>
-      <c r="C61" s="108"/>
-      <c r="D61" s="87"/>
-      <c r="E61" s="87"/>
-      <c r="F61" s="87"/>
-      <c r="G61" s="88"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="100"/>
+      <c r="E61" s="100"/>
+      <c r="F61" s="100"/>
+      <c r="G61" s="101"/>
       <c r="H61" s="12" t="s">
         <v>54</v>
       </c>
@@ -5668,11 +5689,11 @@
       <c r="B62" s="27">
         <v>42</v>
       </c>
-      <c r="C62" s="108"/>
-      <c r="D62" s="87"/>
-      <c r="E62" s="87"/>
-      <c r="F62" s="87"/>
-      <c r="G62" s="88"/>
+      <c r="C62" s="127"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="101"/>
       <c r="H62" s="12" t="s">
         <v>54</v>
       </c>
@@ -5681,11 +5702,11 @@
       <c r="B63" s="9">
         <v>43</v>
       </c>
-      <c r="C63" s="108"/>
-      <c r="D63" s="87"/>
-      <c r="E63" s="87"/>
-      <c r="F63" s="87"/>
-      <c r="G63" s="88"/>
+      <c r="C63" s="127"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="101"/>
       <c r="H63" s="12" t="s">
         <v>54</v>
       </c>
@@ -5694,11 +5715,11 @@
       <c r="B64" s="27">
         <v>44</v>
       </c>
-      <c r="C64" s="108"/>
-      <c r="D64" s="87"/>
-      <c r="E64" s="87"/>
-      <c r="F64" s="87"/>
-      <c r="G64" s="88"/>
+      <c r="C64" s="127"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="101"/>
       <c r="H64" s="12" t="s">
         <v>54</v>
       </c>
@@ -5707,11 +5728,11 @@
       <c r="B65" s="9">
         <v>45</v>
       </c>
-      <c r="C65" s="108"/>
-      <c r="D65" s="87"/>
-      <c r="E65" s="87"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="88"/>
+      <c r="C65" s="127"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="101"/>
       <c r="H65" s="12" t="s">
         <v>54</v>
       </c>
@@ -5720,11 +5741,11 @@
       <c r="B66" s="27">
         <v>46</v>
       </c>
-      <c r="C66" s="108"/>
-      <c r="D66" s="87"/>
-      <c r="E66" s="87"/>
-      <c r="F66" s="87"/>
-      <c r="G66" s="88"/>
+      <c r="C66" s="127"/>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="101"/>
       <c r="H66" s="12" t="s">
         <v>54</v>
       </c>
@@ -5733,11 +5754,11 @@
       <c r="B67" s="9">
         <v>47</v>
       </c>
-      <c r="C67" s="108"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="87"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="88"/>
+      <c r="C67" s="127"/>
+      <c r="D67" s="100"/>
+      <c r="E67" s="100"/>
+      <c r="F67" s="100"/>
+      <c r="G67" s="101"/>
       <c r="H67" s="12" t="s">
         <v>54</v>
       </c>
@@ -5746,11 +5767,11 @@
       <c r="B68" s="27">
         <v>48</v>
       </c>
-      <c r="C68" s="108"/>
-      <c r="D68" s="87"/>
-      <c r="E68" s="87"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="88"/>
+      <c r="C68" s="127"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
+      <c r="F68" s="100"/>
+      <c r="G68" s="101"/>
       <c r="H68" s="12" t="s">
         <v>54</v>
       </c>
@@ -5759,11 +5780,11 @@
       <c r="B69" s="9">
         <v>49</v>
       </c>
-      <c r="C69" s="108"/>
-      <c r="D69" s="87"/>
-      <c r="E69" s="87"/>
-      <c r="F69" s="87"/>
-      <c r="G69" s="88"/>
+      <c r="C69" s="127"/>
+      <c r="D69" s="100"/>
+      <c r="E69" s="100"/>
+      <c r="F69" s="100"/>
+      <c r="G69" s="101"/>
       <c r="H69" s="12" t="s">
         <v>54</v>
       </c>
@@ -5772,11 +5793,11 @@
       <c r="B70" s="27">
         <v>50</v>
       </c>
-      <c r="C70" s="108"/>
-      <c r="D70" s="87"/>
-      <c r="E70" s="87"/>
-      <c r="F70" s="87"/>
-      <c r="G70" s="88"/>
+      <c r="C70" s="127"/>
+      <c r="D70" s="100"/>
+      <c r="E70" s="100"/>
+      <c r="F70" s="100"/>
+      <c r="G70" s="101"/>
       <c r="H70" s="12" t="s">
         <v>54</v>
       </c>
@@ -5785,11 +5806,11 @@
       <c r="B71" s="9">
         <v>51</v>
       </c>
-      <c r="C71" s="108"/>
-      <c r="D71" s="87"/>
-      <c r="E71" s="87"/>
-      <c r="F71" s="87"/>
-      <c r="G71" s="88"/>
+      <c r="C71" s="127"/>
+      <c r="D71" s="100"/>
+      <c r="E71" s="100"/>
+      <c r="F71" s="100"/>
+      <c r="G71" s="101"/>
       <c r="H71" s="12" t="s">
         <v>54</v>
       </c>
@@ -5798,11 +5819,11 @@
       <c r="B72" s="27">
         <v>52</v>
       </c>
-      <c r="C72" s="108"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="87"/>
-      <c r="G72" s="88"/>
+      <c r="C72" s="127"/>
+      <c r="D72" s="100"/>
+      <c r="E72" s="100"/>
+      <c r="F72" s="100"/>
+      <c r="G72" s="101"/>
       <c r="H72" s="12" t="s">
         <v>54</v>
       </c>
@@ -5811,11 +5832,11 @@
       <c r="B73" s="9">
         <v>53</v>
       </c>
-      <c r="C73" s="108"/>
-      <c r="D73" s="87"/>
-      <c r="E73" s="87"/>
-      <c r="F73" s="87"/>
-      <c r="G73" s="88"/>
+      <c r="C73" s="127"/>
+      <c r="D73" s="100"/>
+      <c r="E73" s="100"/>
+      <c r="F73" s="100"/>
+      <c r="G73" s="101"/>
       <c r="H73" s="12" t="s">
         <v>54</v>
       </c>
@@ -5824,11 +5845,11 @@
       <c r="B74" s="27">
         <v>54</v>
       </c>
-      <c r="C74" s="108"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="88"/>
+      <c r="C74" s="127"/>
+      <c r="D74" s="100"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="12" t="s">
         <v>54</v>
       </c>
@@ -5837,11 +5858,11 @@
       <c r="B75" s="9">
         <v>55</v>
       </c>
-      <c r="C75" s="108"/>
-      <c r="D75" s="87"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="87"/>
-      <c r="G75" s="88"/>
+      <c r="C75" s="127"/>
+      <c r="D75" s="100"/>
+      <c r="E75" s="100"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="101"/>
       <c r="H75" s="12" t="s">
         <v>54</v>
       </c>
@@ -5850,11 +5871,11 @@
       <c r="B76" s="27">
         <v>56</v>
       </c>
-      <c r="C76" s="108"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="87"/>
-      <c r="G76" s="88"/>
+      <c r="C76" s="127"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="101"/>
       <c r="H76" s="12" t="s">
         <v>54</v>
       </c>
@@ -5863,11 +5884,11 @@
       <c r="B77" s="9">
         <v>57</v>
       </c>
-      <c r="C77" s="108"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="88"/>
+      <c r="C77" s="127"/>
+      <c r="D77" s="100"/>
+      <c r="E77" s="100"/>
+      <c r="F77" s="100"/>
+      <c r="G77" s="101"/>
       <c r="H77" s="12" t="s">
         <v>54</v>
       </c>
@@ -5876,11 +5897,11 @@
       <c r="B78" s="27">
         <v>58</v>
       </c>
-      <c r="C78" s="108"/>
-      <c r="D78" s="87"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="87"/>
-      <c r="G78" s="88"/>
+      <c r="C78" s="127"/>
+      <c r="D78" s="100"/>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
+      <c r="G78" s="101"/>
       <c r="H78" s="12" t="s">
         <v>54</v>
       </c>
@@ -5889,11 +5910,11 @@
       <c r="B79" s="9">
         <v>59</v>
       </c>
-      <c r="C79" s="108"/>
-      <c r="D79" s="87"/>
-      <c r="E79" s="87"/>
-      <c r="F79" s="87"/>
-      <c r="G79" s="88"/>
+      <c r="C79" s="127"/>
+      <c r="D79" s="100"/>
+      <c r="E79" s="100"/>
+      <c r="F79" s="100"/>
+      <c r="G79" s="101"/>
       <c r="H79" s="12" t="s">
         <v>54</v>
       </c>
@@ -5902,11 +5923,11 @@
       <c r="B80" s="27">
         <v>60</v>
       </c>
-      <c r="C80" s="108"/>
-      <c r="D80" s="87"/>
-      <c r="E80" s="87"/>
-      <c r="F80" s="87"/>
-      <c r="G80" s="88"/>
+      <c r="C80" s="127"/>
+      <c r="D80" s="100"/>
+      <c r="E80" s="100"/>
+      <c r="F80" s="100"/>
+      <c r="G80" s="101"/>
       <c r="H80" s="12" t="s">
         <v>54</v>
       </c>
@@ -5915,11 +5936,11 @@
       <c r="B81" s="9">
         <v>61</v>
       </c>
-      <c r="C81" s="108"/>
-      <c r="D81" s="87"/>
-      <c r="E81" s="87"/>
-      <c r="F81" s="87"/>
-      <c r="G81" s="88"/>
+      <c r="C81" s="127"/>
+      <c r="D81" s="100"/>
+      <c r="E81" s="100"/>
+      <c r="F81" s="100"/>
+      <c r="G81" s="101"/>
       <c r="H81" s="12" t="s">
         <v>54</v>
       </c>
@@ -5928,11 +5949,11 @@
       <c r="B82" s="27">
         <v>62</v>
       </c>
-      <c r="C82" s="108"/>
-      <c r="D82" s="87"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="87"/>
-      <c r="G82" s="88"/>
+      <c r="C82" s="127"/>
+      <c r="D82" s="100"/>
+      <c r="E82" s="100"/>
+      <c r="F82" s="100"/>
+      <c r="G82" s="101"/>
       <c r="H82" s="12" t="s">
         <v>54</v>
       </c>
@@ -5941,11 +5962,11 @@
       <c r="B83" s="9">
         <v>63</v>
       </c>
-      <c r="C83" s="108"/>
-      <c r="D83" s="87"/>
-      <c r="E83" s="87"/>
-      <c r="F83" s="87"/>
-      <c r="G83" s="88"/>
+      <c r="C83" s="127"/>
+      <c r="D83" s="100"/>
+      <c r="E83" s="100"/>
+      <c r="F83" s="100"/>
+      <c r="G83" s="101"/>
       <c r="H83" s="12" t="s">
         <v>54</v>
       </c>
@@ -5954,11 +5975,11 @@
       <c r="B84" s="27">
         <v>64</v>
       </c>
-      <c r="C84" s="108"/>
-      <c r="D84" s="87"/>
-      <c r="E84" s="87"/>
-      <c r="F84" s="87"/>
-      <c r="G84" s="88"/>
+      <c r="C84" s="127"/>
+      <c r="D84" s="100"/>
+      <c r="E84" s="100"/>
+      <c r="F84" s="100"/>
+      <c r="G84" s="101"/>
       <c r="H84" s="12" t="s">
         <v>54</v>
       </c>
@@ -5967,11 +5988,11 @@
       <c r="B85" s="9">
         <v>65</v>
       </c>
-      <c r="C85" s="108"/>
-      <c r="D85" s="87"/>
-      <c r="E85" s="87"/>
-      <c r="F85" s="87"/>
-      <c r="G85" s="88"/>
+      <c r="C85" s="127"/>
+      <c r="D85" s="100"/>
+      <c r="E85" s="100"/>
+      <c r="F85" s="100"/>
+      <c r="G85" s="101"/>
       <c r="H85" s="12" t="s">
         <v>54</v>
       </c>
@@ -5980,11 +6001,11 @@
       <c r="B86" s="27">
         <v>66</v>
       </c>
-      <c r="C86" s="108"/>
-      <c r="D86" s="87"/>
-      <c r="E86" s="87"/>
-      <c r="F86" s="87"/>
-      <c r="G86" s="88"/>
+      <c r="C86" s="127"/>
+      <c r="D86" s="100"/>
+      <c r="E86" s="100"/>
+      <c r="F86" s="100"/>
+      <c r="G86" s="101"/>
       <c r="H86" s="12" t="s">
         <v>54</v>
       </c>
@@ -5993,11 +6014,11 @@
       <c r="B87" s="9">
         <v>67</v>
       </c>
-      <c r="C87" s="108"/>
-      <c r="D87" s="87"/>
-      <c r="E87" s="87"/>
-      <c r="F87" s="87"/>
-      <c r="G87" s="88"/>
+      <c r="C87" s="127"/>
+      <c r="D87" s="100"/>
+      <c r="E87" s="100"/>
+      <c r="F87" s="100"/>
+      <c r="G87" s="101"/>
       <c r="H87" s="12" t="s">
         <v>54</v>
       </c>
@@ -6006,11 +6027,11 @@
       <c r="B88" s="27">
         <v>68</v>
       </c>
-      <c r="C88" s="108"/>
-      <c r="D88" s="87"/>
-      <c r="E88" s="87"/>
-      <c r="F88" s="87"/>
-      <c r="G88" s="88"/>
+      <c r="C88" s="127"/>
+      <c r="D88" s="100"/>
+      <c r="E88" s="100"/>
+      <c r="F88" s="100"/>
+      <c r="G88" s="101"/>
       <c r="H88" s="12" t="s">
         <v>54</v>
       </c>
@@ -6019,11 +6040,11 @@
       <c r="B89" s="9">
         <v>69</v>
       </c>
-      <c r="C89" s="108"/>
-      <c r="D89" s="87"/>
-      <c r="E89" s="87"/>
-      <c r="F89" s="87"/>
-      <c r="G89" s="88"/>
+      <c r="C89" s="127"/>
+      <c r="D89" s="100"/>
+      <c r="E89" s="100"/>
+      <c r="F89" s="100"/>
+      <c r="G89" s="101"/>
       <c r="H89" s="12" t="s">
         <v>54</v>
       </c>
@@ -6032,11 +6053,11 @@
       <c r="B90" s="27">
         <v>70</v>
       </c>
-      <c r="C90" s="108"/>
-      <c r="D90" s="87"/>
-      <c r="E90" s="87"/>
-      <c r="F90" s="87"/>
-      <c r="G90" s="88"/>
+      <c r="C90" s="127"/>
+      <c r="D90" s="100"/>
+      <c r="E90" s="100"/>
+      <c r="F90" s="100"/>
+      <c r="G90" s="101"/>
       <c r="H90" s="12" t="s">
         <v>54</v>
       </c>
@@ -6045,11 +6066,11 @@
       <c r="B91" s="9">
         <v>71</v>
       </c>
-      <c r="C91" s="108"/>
-      <c r="D91" s="87"/>
-      <c r="E91" s="87"/>
-      <c r="F91" s="87"/>
-      <c r="G91" s="88"/>
+      <c r="C91" s="127"/>
+      <c r="D91" s="100"/>
+      <c r="E91" s="100"/>
+      <c r="F91" s="100"/>
+      <c r="G91" s="101"/>
       <c r="H91" s="12" t="s">
         <v>54</v>
       </c>
@@ -6058,11 +6079,11 @@
       <c r="B92" s="27">
         <v>72</v>
       </c>
-      <c r="C92" s="108"/>
-      <c r="D92" s="87"/>
-      <c r="E92" s="87"/>
-      <c r="F92" s="87"/>
-      <c r="G92" s="88"/>
+      <c r="C92" s="127"/>
+      <c r="D92" s="100"/>
+      <c r="E92" s="100"/>
+      <c r="F92" s="100"/>
+      <c r="G92" s="101"/>
       <c r="H92" s="12" t="s">
         <v>54</v>
       </c>
@@ -6071,11 +6092,11 @@
       <c r="B93" s="9">
         <v>73</v>
       </c>
-      <c r="C93" s="108"/>
-      <c r="D93" s="87"/>
-      <c r="E93" s="87"/>
-      <c r="F93" s="87"/>
-      <c r="G93" s="88"/>
+      <c r="C93" s="127"/>
+      <c r="D93" s="100"/>
+      <c r="E93" s="100"/>
+      <c r="F93" s="100"/>
+      <c r="G93" s="101"/>
       <c r="H93" s="12" t="s">
         <v>54</v>
       </c>
@@ -6084,11 +6105,11 @@
       <c r="B94" s="27">
         <v>74</v>
       </c>
-      <c r="C94" s="108"/>
-      <c r="D94" s="87"/>
-      <c r="E94" s="87"/>
-      <c r="F94" s="87"/>
-      <c r="G94" s="88"/>
+      <c r="C94" s="127"/>
+      <c r="D94" s="100"/>
+      <c r="E94" s="100"/>
+      <c r="F94" s="100"/>
+      <c r="G94" s="101"/>
       <c r="H94" s="12" t="s">
         <v>54</v>
       </c>
@@ -6097,11 +6118,11 @@
       <c r="B95" s="9">
         <v>75</v>
       </c>
-      <c r="C95" s="108"/>
-      <c r="D95" s="87"/>
-      <c r="E95" s="87"/>
-      <c r="F95" s="87"/>
-      <c r="G95" s="88"/>
+      <c r="C95" s="127"/>
+      <c r="D95" s="100"/>
+      <c r="E95" s="100"/>
+      <c r="F95" s="100"/>
+      <c r="G95" s="101"/>
       <c r="H95" s="12" t="s">
         <v>54</v>
       </c>
@@ -6110,11 +6131,11 @@
       <c r="B96" s="27">
         <v>76</v>
       </c>
-      <c r="C96" s="108"/>
-      <c r="D96" s="87"/>
-      <c r="E96" s="87"/>
-      <c r="F96" s="87"/>
-      <c r="G96" s="88"/>
+      <c r="C96" s="127"/>
+      <c r="D96" s="100"/>
+      <c r="E96" s="100"/>
+      <c r="F96" s="100"/>
+      <c r="G96" s="101"/>
       <c r="H96" s="12" t="s">
         <v>54</v>
       </c>
@@ -6123,11 +6144,11 @@
       <c r="B97" s="9">
         <v>77</v>
       </c>
-      <c r="C97" s="108"/>
-      <c r="D97" s="87"/>
-      <c r="E97" s="87"/>
-      <c r="F97" s="87"/>
-      <c r="G97" s="88"/>
+      <c r="C97" s="127"/>
+      <c r="D97" s="100"/>
+      <c r="E97" s="100"/>
+      <c r="F97" s="100"/>
+      <c r="G97" s="101"/>
       <c r="H97" s="12" t="s">
         <v>54</v>
       </c>
@@ -6136,11 +6157,11 @@
       <c r="B98" s="27">
         <v>78</v>
       </c>
-      <c r="C98" s="108"/>
-      <c r="D98" s="87"/>
-      <c r="E98" s="87"/>
-      <c r="F98" s="87"/>
-      <c r="G98" s="88"/>
+      <c r="C98" s="127"/>
+      <c r="D98" s="100"/>
+      <c r="E98" s="100"/>
+      <c r="F98" s="100"/>
+      <c r="G98" s="101"/>
       <c r="H98" s="12" t="s">
         <v>54</v>
       </c>
@@ -6149,11 +6170,11 @@
       <c r="B99" s="9">
         <v>79</v>
       </c>
-      <c r="C99" s="108"/>
-      <c r="D99" s="87"/>
-      <c r="E99" s="87"/>
-      <c r="F99" s="87"/>
-      <c r="G99" s="88"/>
+      <c r="C99" s="127"/>
+      <c r="D99" s="100"/>
+      <c r="E99" s="100"/>
+      <c r="F99" s="100"/>
+      <c r="G99" s="101"/>
       <c r="H99" s="12" t="s">
         <v>54</v>
       </c>
@@ -6162,11 +6183,11 @@
       <c r="B100" s="27">
         <v>80</v>
       </c>
-      <c r="C100" s="108"/>
-      <c r="D100" s="87"/>
-      <c r="E100" s="87"/>
-      <c r="F100" s="87"/>
-      <c r="G100" s="88"/>
+      <c r="C100" s="127"/>
+      <c r="D100" s="100"/>
+      <c r="E100" s="100"/>
+      <c r="F100" s="100"/>
+      <c r="G100" s="101"/>
       <c r="H100" s="12" t="s">
         <v>54</v>
       </c>
@@ -6175,11 +6196,11 @@
       <c r="B101" s="9">
         <v>81</v>
       </c>
-      <c r="C101" s="108"/>
-      <c r="D101" s="87"/>
-      <c r="E101" s="87"/>
-      <c r="F101" s="87"/>
-      <c r="G101" s="88"/>
+      <c r="C101" s="127"/>
+      <c r="D101" s="100"/>
+      <c r="E101" s="100"/>
+      <c r="F101" s="100"/>
+      <c r="G101" s="101"/>
       <c r="H101" s="12" t="s">
         <v>54</v>
       </c>
@@ -6188,11 +6209,11 @@
       <c r="B102" s="27">
         <v>82</v>
       </c>
-      <c r="C102" s="108"/>
-      <c r="D102" s="87"/>
-      <c r="E102" s="87"/>
-      <c r="F102" s="87"/>
-      <c r="G102" s="88"/>
+      <c r="C102" s="127"/>
+      <c r="D102" s="100"/>
+      <c r="E102" s="100"/>
+      <c r="F102" s="100"/>
+      <c r="G102" s="101"/>
       <c r="H102" s="12" t="s">
         <v>54</v>
       </c>
@@ -6201,11 +6222,11 @@
       <c r="B103" s="9">
         <v>83</v>
       </c>
-      <c r="C103" s="108"/>
-      <c r="D103" s="87"/>
-      <c r="E103" s="87"/>
-      <c r="F103" s="87"/>
-      <c r="G103" s="88"/>
+      <c r="C103" s="127"/>
+      <c r="D103" s="100"/>
+      <c r="E103" s="100"/>
+      <c r="F103" s="100"/>
+      <c r="G103" s="101"/>
       <c r="H103" s="12" t="s">
         <v>54</v>
       </c>
@@ -6214,11 +6235,11 @@
       <c r="B104" s="27">
         <v>84</v>
       </c>
-      <c r="C104" s="108"/>
-      <c r="D104" s="87"/>
-      <c r="E104" s="87"/>
-      <c r="F104" s="87"/>
-      <c r="G104" s="88"/>
+      <c r="C104" s="127"/>
+      <c r="D104" s="100"/>
+      <c r="E104" s="100"/>
+      <c r="F104" s="100"/>
+      <c r="G104" s="101"/>
       <c r="H104" s="12" t="s">
         <v>54</v>
       </c>
@@ -6227,11 +6248,11 @@
       <c r="B105" s="9">
         <v>85</v>
       </c>
-      <c r="C105" s="108"/>
-      <c r="D105" s="87"/>
-      <c r="E105" s="87"/>
-      <c r="F105" s="87"/>
-      <c r="G105" s="88"/>
+      <c r="C105" s="127"/>
+      <c r="D105" s="100"/>
+      <c r="E105" s="100"/>
+      <c r="F105" s="100"/>
+      <c r="G105" s="101"/>
       <c r="H105" s="12" t="s">
         <v>54</v>
       </c>
@@ -6240,11 +6261,11 @@
       <c r="B106" s="27">
         <v>86</v>
       </c>
-      <c r="C106" s="108"/>
-      <c r="D106" s="87"/>
-      <c r="E106" s="87"/>
-      <c r="F106" s="87"/>
-      <c r="G106" s="88"/>
+      <c r="C106" s="127"/>
+      <c r="D106" s="100"/>
+      <c r="E106" s="100"/>
+      <c r="F106" s="100"/>
+      <c r="G106" s="101"/>
       <c r="H106" s="12" t="s">
         <v>54</v>
       </c>
@@ -6253,11 +6274,11 @@
       <c r="B107" s="9">
         <v>87</v>
       </c>
-      <c r="C107" s="108"/>
-      <c r="D107" s="87"/>
-      <c r="E107" s="87"/>
-      <c r="F107" s="87"/>
-      <c r="G107" s="88"/>
+      <c r="C107" s="127"/>
+      <c r="D107" s="100"/>
+      <c r="E107" s="100"/>
+      <c r="F107" s="100"/>
+      <c r="G107" s="101"/>
       <c r="H107" s="12" t="s">
         <v>54</v>
       </c>
@@ -6266,11 +6287,11 @@
       <c r="B108" s="27">
         <v>88</v>
       </c>
-      <c r="C108" s="108"/>
-      <c r="D108" s="87"/>
-      <c r="E108" s="87"/>
-      <c r="F108" s="87"/>
-      <c r="G108" s="88"/>
+      <c r="C108" s="127"/>
+      <c r="D108" s="100"/>
+      <c r="E108" s="100"/>
+      <c r="F108" s="100"/>
+      <c r="G108" s="101"/>
       <c r="H108" s="12" t="s">
         <v>54</v>
       </c>
@@ -6279,11 +6300,11 @@
       <c r="B109" s="9">
         <v>89</v>
       </c>
-      <c r="C109" s="108"/>
-      <c r="D109" s="87"/>
-      <c r="E109" s="87"/>
-      <c r="F109" s="87"/>
-      <c r="G109" s="88"/>
+      <c r="C109" s="127"/>
+      <c r="D109" s="100"/>
+      <c r="E109" s="100"/>
+      <c r="F109" s="100"/>
+      <c r="G109" s="101"/>
       <c r="H109" s="12" t="s">
         <v>54</v>
       </c>
@@ -6292,11 +6313,11 @@
       <c r="B110" s="27">
         <v>90</v>
       </c>
-      <c r="C110" s="108"/>
-      <c r="D110" s="87"/>
-      <c r="E110" s="87"/>
-      <c r="F110" s="87"/>
-      <c r="G110" s="88"/>
+      <c r="C110" s="127"/>
+      <c r="D110" s="100"/>
+      <c r="E110" s="100"/>
+      <c r="F110" s="100"/>
+      <c r="G110" s="101"/>
       <c r="H110" s="12" t="s">
         <v>54</v>
       </c>
@@ -6305,11 +6326,11 @@
       <c r="B111" s="9">
         <v>91</v>
       </c>
-      <c r="C111" s="108"/>
-      <c r="D111" s="87"/>
-      <c r="E111" s="87"/>
-      <c r="F111" s="87"/>
-      <c r="G111" s="88"/>
+      <c r="C111" s="127"/>
+      <c r="D111" s="100"/>
+      <c r="E111" s="100"/>
+      <c r="F111" s="100"/>
+      <c r="G111" s="101"/>
       <c r="H111" s="12" t="s">
         <v>54</v>
       </c>
@@ -6318,11 +6339,11 @@
       <c r="B112" s="27">
         <v>92</v>
       </c>
-      <c r="C112" s="108"/>
-      <c r="D112" s="87"/>
-      <c r="E112" s="87"/>
-      <c r="F112" s="87"/>
-      <c r="G112" s="88"/>
+      <c r="C112" s="127"/>
+      <c r="D112" s="100"/>
+      <c r="E112" s="100"/>
+      <c r="F112" s="100"/>
+      <c r="G112" s="101"/>
       <c r="H112" s="12" t="s">
         <v>54</v>
       </c>
@@ -6331,11 +6352,11 @@
       <c r="B113" s="9">
         <v>93</v>
       </c>
-      <c r="C113" s="108"/>
-      <c r="D113" s="87"/>
-      <c r="E113" s="87"/>
-      <c r="F113" s="87"/>
-      <c r="G113" s="88"/>
+      <c r="C113" s="127"/>
+      <c r="D113" s="100"/>
+      <c r="E113" s="100"/>
+      <c r="F113" s="100"/>
+      <c r="G113" s="101"/>
       <c r="H113" s="12" t="s">
         <v>54</v>
       </c>
@@ -6344,11 +6365,11 @@
       <c r="B114" s="27">
         <v>94</v>
       </c>
-      <c r="C114" s="108"/>
-      <c r="D114" s="87"/>
-      <c r="E114" s="87"/>
-      <c r="F114" s="87"/>
-      <c r="G114" s="88"/>
+      <c r="C114" s="127"/>
+      <c r="D114" s="100"/>
+      <c r="E114" s="100"/>
+      <c r="F114" s="100"/>
+      <c r="G114" s="101"/>
       <c r="H114" s="12" t="s">
         <v>54</v>
       </c>
@@ -6357,11 +6378,11 @@
       <c r="B115" s="9">
         <v>95</v>
       </c>
-      <c r="C115" s="108"/>
-      <c r="D115" s="87"/>
-      <c r="E115" s="87"/>
-      <c r="F115" s="87"/>
-      <c r="G115" s="88"/>
+      <c r="C115" s="127"/>
+      <c r="D115" s="100"/>
+      <c r="E115" s="100"/>
+      <c r="F115" s="100"/>
+      <c r="G115" s="101"/>
       <c r="H115" s="12" t="s">
         <v>54</v>
       </c>
@@ -6370,11 +6391,11 @@
       <c r="B116" s="27">
         <v>96</v>
       </c>
-      <c r="C116" s="108"/>
-      <c r="D116" s="87"/>
-      <c r="E116" s="87"/>
-      <c r="F116" s="87"/>
-      <c r="G116" s="88"/>
+      <c r="C116" s="127"/>
+      <c r="D116" s="100"/>
+      <c r="E116" s="100"/>
+      <c r="F116" s="100"/>
+      <c r="G116" s="101"/>
       <c r="H116" s="12" t="s">
         <v>54</v>
       </c>
@@ -6383,11 +6404,11 @@
       <c r="B117" s="9">
         <v>97</v>
       </c>
-      <c r="C117" s="108"/>
-      <c r="D117" s="87"/>
-      <c r="E117" s="87"/>
-      <c r="F117" s="87"/>
-      <c r="G117" s="88"/>
+      <c r="C117" s="127"/>
+      <c r="D117" s="100"/>
+      <c r="E117" s="100"/>
+      <c r="F117" s="100"/>
+      <c r="G117" s="101"/>
       <c r="H117" s="12" t="s">
         <v>54</v>
       </c>
@@ -6396,11 +6417,11 @@
       <c r="B118" s="27">
         <v>98</v>
       </c>
-      <c r="C118" s="108"/>
-      <c r="D118" s="87"/>
-      <c r="E118" s="87"/>
-      <c r="F118" s="87"/>
-      <c r="G118" s="88"/>
+      <c r="C118" s="127"/>
+      <c r="D118" s="100"/>
+      <c r="E118" s="100"/>
+      <c r="F118" s="100"/>
+      <c r="G118" s="101"/>
       <c r="H118" s="12" t="s">
         <v>54</v>
       </c>
@@ -6409,11 +6430,11 @@
       <c r="B119" s="9">
         <v>99</v>
       </c>
-      <c r="C119" s="108"/>
-      <c r="D119" s="87"/>
-      <c r="E119" s="87"/>
-      <c r="F119" s="87"/>
-      <c r="G119" s="88"/>
+      <c r="C119" s="127"/>
+      <c r="D119" s="100"/>
+      <c r="E119" s="100"/>
+      <c r="F119" s="100"/>
+      <c r="G119" s="101"/>
       <c r="H119" s="12" t="s">
         <v>54</v>
       </c>
@@ -6422,11 +6443,11 @@
       <c r="B120" s="27">
         <v>100</v>
       </c>
-      <c r="C120" s="108"/>
-      <c r="D120" s="87"/>
-      <c r="E120" s="87"/>
-      <c r="F120" s="87"/>
-      <c r="G120" s="88"/>
+      <c r="C120" s="127"/>
+      <c r="D120" s="100"/>
+      <c r="E120" s="100"/>
+      <c r="F120" s="100"/>
+      <c r="G120" s="101"/>
       <c r="H120" s="12" t="s">
         <v>54</v>
       </c>
@@ -8105,50 +8126,53 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="C116:G116"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
@@ -8173,53 +8197,50 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H120" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8269,85 +8290,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="2">
         <f>Requisitos!C11</f>
         <v>45170</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K65" si="0">K1+1</f>
         <v>45171</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45172</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45173</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="105"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45174</v>
@@ -8361,18 +8382,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="str">
+      <c r="B7" s="99" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45176</v>
@@ -8386,16 +8407,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -9766,30 +9787,30 @@
       </c>
     </row>
     <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="129" t="s">
+      <c r="B63" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="87"/>
-      <c r="D63" s="87"/>
-      <c r="E63" s="87"/>
-      <c r="F63" s="87"/>
-      <c r="G63" s="87"/>
-      <c r="H63" s="87"/>
-      <c r="I63" s="88"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="100"/>
+      <c r="H63" s="100"/>
+      <c r="I63" s="101"/>
       <c r="K63" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
       </c>
     </row>
     <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="130" t="s">
+      <c r="B64" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="87"/>
-      <c r="D64" s="87"/>
-      <c r="E64" s="87"/>
-      <c r="F64" s="87"/>
-      <c r="G64" s="88"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="101"/>
       <c r="H64" s="7" t="s">
         <v>99</v>
       </c>
@@ -9802,15 +9823,15 @@
       </c>
     </row>
     <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="128" t="str">
+      <c r="B65" s="133" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="87"/>
-      <c r="D65" s="87"/>
-      <c r="E65" s="87"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="88"/>
+      <c r="C65" s="100"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="101"/>
       <c r="H65" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B10,H$11:H$60)</f>
         <v>0</v>
@@ -9825,15 +9846,15 @@
       </c>
     </row>
     <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="128" t="str">
+      <c r="B66" s="133" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="87"/>
-      <c r="D66" s="87"/>
-      <c r="E66" s="87"/>
-      <c r="F66" s="87"/>
-      <c r="G66" s="88"/>
+      <c r="C66" s="100"/>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="101"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -9848,15 +9869,15 @@
       </c>
     </row>
     <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="128" t="str">
+      <c r="B67" s="133" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="87"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="87"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="88"/>
+      <c r="C67" s="100"/>
+      <c r="D67" s="100"/>
+      <c r="E67" s="100"/>
+      <c r="F67" s="100"/>
+      <c r="G67" s="101"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -9871,15 +9892,15 @@
       </c>
     </row>
     <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="128" t="str">
+      <c r="B68" s="133" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v>Maria Eduarda Amaral</v>
       </c>
-      <c r="C68" s="87"/>
-      <c r="D68" s="87"/>
-      <c r="E68" s="87"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="88"/>
+      <c r="C68" s="100"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
+      <c r="F68" s="100"/>
+      <c r="G68" s="101"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -9894,15 +9915,15 @@
       </c>
     </row>
     <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="128" t="str">
+      <c r="B69" s="133" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C69" s="87"/>
-      <c r="D69" s="87"/>
-      <c r="E69" s="87"/>
-      <c r="F69" s="87"/>
-      <c r="G69" s="88"/>
+      <c r="C69" s="100"/>
+      <c r="D69" s="100"/>
+      <c r="E69" s="100"/>
+      <c r="F69" s="100"/>
+      <c r="G69" s="101"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -9917,15 +9938,15 @@
       </c>
     </row>
     <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="128" t="str">
+      <c r="B70" s="133" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C70" s="87"/>
-      <c r="D70" s="87"/>
-      <c r="E70" s="87"/>
-      <c r="F70" s="87"/>
-      <c r="G70" s="88"/>
+      <c r="C70" s="100"/>
+      <c r="D70" s="100"/>
+      <c r="E70" s="100"/>
+      <c r="F70" s="100"/>
+      <c r="G70" s="101"/>
       <c r="H70" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -11074,85 +11095,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="2">
         <f>Requisitos!C12</f>
         <v>45191</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45192</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45193</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45194</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="105"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45195</v>
@@ -11166,18 +11187,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="str">
+      <c r="B7" s="99" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45197</v>
@@ -11191,16 +11212,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -12566,26 +12587,26 @@
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="129" t="s">
+      <c r="B72" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="87"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="87"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="87"/>
-      <c r="I72" s="88"/>
+      <c r="C72" s="100"/>
+      <c r="D72" s="100"/>
+      <c r="E72" s="100"/>
+      <c r="F72" s="100"/>
+      <c r="G72" s="100"/>
+      <c r="H72" s="100"/>
+      <c r="I72" s="101"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="130" t="s">
+      <c r="B73" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="87"/>
-      <c r="D73" s="87"/>
-      <c r="E73" s="87"/>
-      <c r="F73" s="87"/>
-      <c r="G73" s="88"/>
+      <c r="C73" s="100"/>
+      <c r="D73" s="100"/>
+      <c r="E73" s="100"/>
+      <c r="F73" s="100"/>
+      <c r="G73" s="101"/>
       <c r="H73" s="7" t="s">
         <v>99</v>
       </c>
@@ -12594,15 +12615,15 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="128" t="str">
+      <c r="B74" s="133" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="87"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="88"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="100"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -12613,15 +12634,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="128" t="str">
+      <c r="B75" s="133" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="87"/>
-      <c r="D75" s="87"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="87"/>
-      <c r="G75" s="88"/>
+      <c r="C75" s="100"/>
+      <c r="D75" s="100"/>
+      <c r="E75" s="100"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="101"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -12632,15 +12653,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="128" t="str">
+      <c r="B76" s="133" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="87"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="87"/>
-      <c r="G76" s="88"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="101"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -12651,15 +12672,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="128" t="str">
+      <c r="B77" s="133" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="88"/>
+      <c r="C77" s="100"/>
+      <c r="D77" s="100"/>
+      <c r="E77" s="100"/>
+      <c r="F77" s="100"/>
+      <c r="G77" s="101"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -12670,15 +12691,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="128" t="str">
+      <c r="B78" s="133" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="87"/>
-      <c r="D78" s="87"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="87"/>
-      <c r="G78" s="88"/>
+      <c r="C78" s="100"/>
+      <c r="D78" s="100"/>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
+      <c r="G78" s="101"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -13929,85 +13950,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="2">
         <f>Requisitos!C13</f>
         <v>45205</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K22" si="0">K1+1</f>
         <v>45206</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45207</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45208</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="105"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45209</v>
@@ -14021,18 +14042,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="str">
+      <c r="B7" s="99" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45211</v>
@@ -14046,16 +14067,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -15393,26 +15414,26 @@
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="129" t="s">
+      <c r="B73" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="87"/>
-      <c r="D73" s="87"/>
-      <c r="E73" s="87"/>
-      <c r="F73" s="87"/>
-      <c r="G73" s="87"/>
-      <c r="H73" s="87"/>
-      <c r="I73" s="88"/>
+      <c r="C73" s="100"/>
+      <c r="D73" s="100"/>
+      <c r="E73" s="100"/>
+      <c r="F73" s="100"/>
+      <c r="G73" s="100"/>
+      <c r="H73" s="100"/>
+      <c r="I73" s="101"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="130" t="s">
+      <c r="B74" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="87"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="88"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="100"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="7" t="s">
         <v>99</v>
       </c>
@@ -15421,15 +15442,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="128" t="str">
+      <c r="B75" s="133" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C75" s="87"/>
-      <c r="D75" s="87"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="87"/>
-      <c r="G75" s="88"/>
+      <c r="C75" s="100"/>
+      <c r="D75" s="100"/>
+      <c r="E75" s="100"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="101"/>
       <c r="H75" s="33">
         <f>SUMIF($F$11:$F$61,'Dados do Projeto'!$B10,H$11:H$61)</f>
         <v>0</v>
@@ -15440,15 +15461,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="128" t="str">
+      <c r="B76" s="133" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C76" s="87"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="87"/>
-      <c r="G76" s="88"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="101"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B11,H$11:H$61)</f>
         <v>0</v>
@@ -15459,15 +15480,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="128" t="str">
+      <c r="B77" s="133" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="88"/>
+      <c r="C77" s="100"/>
+      <c r="D77" s="100"/>
+      <c r="E77" s="100"/>
+      <c r="F77" s="100"/>
+      <c r="G77" s="101"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B12,H$11:H$61)</f>
         <v>0</v>
@@ -15478,15 +15499,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="128" t="str">
+      <c r="B78" s="133" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C78" s="87"/>
-      <c r="D78" s="87"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="87"/>
-      <c r="G78" s="88"/>
+      <c r="C78" s="100"/>
+      <c r="D78" s="100"/>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
+      <c r="G78" s="101"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B14,H$11:H$61)</f>
         <v>0</v>
@@ -15497,15 +15518,15 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="128" t="str">
+      <c r="B79" s="133" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C79" s="87"/>
-      <c r="D79" s="87"/>
-      <c r="E79" s="87"/>
-      <c r="F79" s="87"/>
-      <c r="G79" s="88"/>
+      <c r="C79" s="100"/>
+      <c r="D79" s="100"/>
+      <c r="E79" s="100"/>
+      <c r="F79" s="100"/>
+      <c r="G79" s="101"/>
       <c r="H79" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B15,H$11:H$61)</f>
         <v>0</v>
@@ -16529,6 +16550,12 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B79:G79"/>
     <mergeCell ref="B9:I9"/>
@@ -16537,12 +16564,6 @@
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
     <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C70">
     <cfRule type="expression" dxfId="71" priority="31">
@@ -16681,8 +16702,8 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16703,85 +16724,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="2">
         <f>Requisitos!C14</f>
         <v>45226</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>45227</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45228</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45229</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="105"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45230</v>
@@ -16795,18 +16816,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="str">
+      <c r="B7" s="99" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -16820,16 +16841,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="134" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -16889,7 +16910,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H11" s="13">
         <v>0</v>
@@ -16930,7 +16951,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H12" s="13">
         <v>0</v>
@@ -16961,7 +16982,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H13" s="13">
         <v>0</v>
@@ -16992,7 +17013,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H14" s="13">
         <v>0</v>
@@ -17023,7 +17044,7 @@
         <v>8</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H15" s="13">
         <v>0</v>
@@ -17420,31 +17441,31 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="2:11" s="74" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="75">
+      <c r="B29" s="83">
         <v>19</v>
       </c>
-      <c r="C29" s="76">
+      <c r="C29" s="84">
         <v>45246</v>
       </c>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="E29" s="71" t="s">
+      <c r="E29" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="77" t="s">
+      <c r="F29" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="78" t="s">
+      <c r="G29" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="79">
-        <v>0</v>
-      </c>
-      <c r="I29" s="79">
-        <v>0</v>
-      </c>
-      <c r="J29" s="71" t="s">
+      <c r="H29" s="88">
+        <v>0</v>
+      </c>
+      <c r="I29" s="88">
+        <v>0</v>
+      </c>
+      <c r="J29" s="85" t="s">
         <v>162</v>
       </c>
     </row>
@@ -17465,7 +17486,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="78" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H30" s="79">
         <v>0</v>
@@ -18185,31 +18206,31 @@
       <c r="F71" s="30"/>
       <c r="G71" s="30">
         <f>COUNTIFS(G11:G60, "Concluído",D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="129" t="s">
+      <c r="B72" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="87"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="87"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="87"/>
-      <c r="I72" s="88"/>
+      <c r="C72" s="100"/>
+      <c r="D72" s="100"/>
+      <c r="E72" s="100"/>
+      <c r="F72" s="100"/>
+      <c r="G72" s="100"/>
+      <c r="H72" s="100"/>
+      <c r="I72" s="101"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="130" t="s">
+      <c r="B73" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="87"/>
-      <c r="D73" s="87"/>
-      <c r="E73" s="87"/>
-      <c r="F73" s="87"/>
-      <c r="G73" s="88"/>
+      <c r="C73" s="100"/>
+      <c r="D73" s="100"/>
+      <c r="E73" s="100"/>
+      <c r="F73" s="100"/>
+      <c r="G73" s="101"/>
       <c r="H73" s="7" t="s">
         <v>99</v>
       </c>
@@ -18218,15 +18239,15 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="128" t="str">
+      <c r="B74" s="133" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="87"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="88"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="100"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="101"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -18237,15 +18258,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="128" t="str">
+      <c r="B75" s="133" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="87"/>
-      <c r="D75" s="87"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="87"/>
-      <c r="G75" s="88"/>
+      <c r="C75" s="100"/>
+      <c r="D75" s="100"/>
+      <c r="E75" s="100"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="101"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -18256,15 +18277,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="128" t="str">
+      <c r="B76" s="133" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="87"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="87"/>
-      <c r="G76" s="88"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
+      <c r="G76" s="101"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -18275,15 +18296,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="128" t="str">
+      <c r="B77" s="133" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="88"/>
+      <c r="C77" s="100"/>
+      <c r="D77" s="100"/>
+      <c r="E77" s="100"/>
+      <c r="F77" s="100"/>
+      <c r="G77" s="101"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -18294,15 +18315,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="128" t="str">
+      <c r="B78" s="133" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="87"/>
-      <c r="D78" s="87"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="87"/>
-      <c r="G78" s="88"/>
+      <c r="C78" s="100"/>
+      <c r="D78" s="100"/>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
+      <c r="G78" s="101"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -19326,6 +19347,12 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B9:I9"/>
@@ -19334,12 +19361,6 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F33:F69">
     <cfRule type="expression" dxfId="51" priority="25">
@@ -19468,85 +19489,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="2">
         <f>Requisitos!C15</f>
         <v>45247</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="105"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45248</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45249</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45250</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="105"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45251</v>
@@ -19559,18 +19580,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="98" t="str">
+      <c r="B7" s="99" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45253</v>
@@ -19583,16 +19604,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="134" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="58" t="s">
         <v>66</v>
       </c>
@@ -20553,26 +20574,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="129" t="s">
+      <c r="B63" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="87"/>
-      <c r="D63" s="87"/>
-      <c r="E63" s="87"/>
-      <c r="F63" s="87"/>
-      <c r="G63" s="87"/>
-      <c r="H63" s="87"/>
-      <c r="I63" s="88"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="100"/>
+      <c r="H63" s="100"/>
+      <c r="I63" s="101"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="130" t="s">
+      <c r="B64" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="87"/>
-      <c r="D64" s="87"/>
-      <c r="E64" s="87"/>
-      <c r="F64" s="87"/>
-      <c r="G64" s="88"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="101"/>
       <c r="H64" s="7" t="s">
         <v>99</v>
       </c>
@@ -20581,15 +20602,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="128" t="str">
+      <c r="B65" s="133" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="87"/>
-      <c r="D65" s="87"/>
-      <c r="E65" s="87"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="88"/>
+      <c r="C65" s="100"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="101"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -20600,15 +20621,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="128" t="str">
+      <c r="B66" s="133" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="87"/>
-      <c r="D66" s="87"/>
-      <c r="E66" s="87"/>
-      <c r="F66" s="87"/>
-      <c r="G66" s="88"/>
+      <c r="C66" s="100"/>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="101"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -20619,15 +20640,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="128" t="str">
+      <c r="B67" s="133" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="87"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="87"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="88"/>
+      <c r="C67" s="100"/>
+      <c r="D67" s="100"/>
+      <c r="E67" s="100"/>
+      <c r="F67" s="100"/>
+      <c r="G67" s="101"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -20638,15 +20659,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="128" t="str">
+      <c r="B68" s="133" t="str">
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C68" s="87"/>
-      <c r="D68" s="87"/>
-      <c r="E68" s="87"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="88"/>
+      <c r="C68" s="100"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
+      <c r="F68" s="100"/>
+      <c r="G68" s="101"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -20657,15 +20678,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="128" t="str">
+      <c r="B69" s="133" t="str">
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C69" s="87"/>
-      <c r="D69" s="87"/>
-      <c r="E69" s="87"/>
-      <c r="F69" s="87"/>
-      <c r="G69" s="88"/>
+      <c r="C69" s="100"/>
+      <c r="D69" s="100"/>
+      <c r="E69" s="100"/>
+      <c r="F69" s="100"/>
+      <c r="G69" s="101"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -21628,6 +21649,12 @@
   </sheetData>
   <autoFilter ref="B10:J60" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="14">
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B9:I9"/>
@@ -21636,12 +21663,6 @@
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B67:G67"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F17">
     <cfRule type="containsBlanks" dxfId="37" priority="1">

</xml_diff>

<commit_message>
docs: update class diagram
</commit_message>
<xml_diff>
--- a/Artefatos/sprints/Planejamento_sprints.xlsx
+++ b/Artefatos/sprints/Planejamento_sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositorios_github\plf-es-2023-2-ti3-6653100-fabrica-do-saber\Artefatos\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\repositories\plf-es-2023-2-ti3-6653100-fabrica-do-saber\Artefatos\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C8729F-EAB3-4FB0-95DA-1A6CD6A55225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67B99F9-54B1-4788-8900-8B6EFAD99302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Projeto" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="175">
   <si>
     <t>PONTIFÍCIA UNIVERSIDADE CATÓLICA DE MINAS GERAIS</t>
   </si>
@@ -886,6 +886,9 @@
   </si>
   <si>
     <t>8 e 11</t>
+  </si>
+  <si>
+    <t>Diagrama de casos de uso</t>
   </si>
 </sst>
 </file>
@@ -1565,35 +1568,16 @@
     <xf numFmtId="1" fontId="27" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1603,19 +1587,74 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1632,15 +1671,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1649,33 +1679,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1688,22 +1691,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="111">
@@ -2722,7 +2725,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <c:style val="18"/>
   <c:chart>
@@ -3340,166 +3343,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="110"/>
     </row>
     <row r="3" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="110"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="102"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="102"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="93"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102" t="s">
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="100"/>
-      <c r="H9" s="101"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="93"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="104" t="s">
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="105"/>
-      <c r="H10" s="106"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="97"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="104" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="97"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="104" t="s">
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="105"/>
-      <c r="H12" s="106"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="97"/>
       <c r="K12" s="47"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="104" t="s">
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="106"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="97"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="104" t="s">
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="97"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="104" t="s">
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="106"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="97"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="18"/>
@@ -3601,16 +3604,16 @@
     <row r="99" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="50"/>
-      <c r="B100" s="108"/>
-      <c r="C100" s="93"/>
-      <c r="D100" s="109" t="s">
+      <c r="B100" s="98"/>
+      <c r="C100" s="90"/>
+      <c r="D100" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="E100" s="93"/>
-      <c r="F100" s="109" t="s">
+      <c r="E100" s="90"/>
+      <c r="F100" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="G100" s="93"/>
+      <c r="G100" s="90"/>
       <c r="H100" s="51" t="s">
         <v>18</v>
       </c>
@@ -3632,12 +3635,12 @@
     </row>
     <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
-      <c r="B101" s="111"/>
-      <c r="C101" s="93"/>
-      <c r="D101" s="110" t="s">
+      <c r="B101" s="89"/>
+      <c r="C101" s="90"/>
+      <c r="D101" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="93"/>
+      <c r="E101" s="90"/>
       <c r="F101" s="53" t="s">
         <v>24</v>
       </c>
@@ -3670,12 +3673,12 @@
     </row>
     <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
-      <c r="B102" s="111"/>
-      <c r="C102" s="93"/>
-      <c r="D102" s="110" t="s">
+      <c r="B102" s="89"/>
+      <c r="C102" s="90"/>
+      <c r="D102" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="E102" s="93"/>
+      <c r="E102" s="90"/>
       <c r="F102" s="53" t="s">
         <v>29</v>
       </c>
@@ -3709,12 +3712,12 @@
     </row>
     <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="50"/>
-      <c r="B103" s="111"/>
-      <c r="C103" s="93"/>
-      <c r="D103" s="110" t="s">
+      <c r="B103" s="89"/>
+      <c r="C103" s="90"/>
+      <c r="D103" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="93"/>
+      <c r="E103" s="90"/>
       <c r="F103" s="53"/>
       <c r="G103" s="54" t="s">
         <v>34</v>
@@ -3746,12 +3749,12 @@
     </row>
     <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="50"/>
-      <c r="B104" s="111"/>
-      <c r="C104" s="93"/>
-      <c r="D104" s="110" t="s">
+      <c r="B104" s="89"/>
+      <c r="C104" s="90"/>
+      <c r="D104" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="93"/>
+      <c r="E104" s="90"/>
       <c r="F104" s="53"/>
       <c r="G104" s="54" t="s">
         <v>36</v>
@@ -3781,12 +3784,12 @@
     </row>
     <row r="105" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="50"/>
-      <c r="B105" s="111"/>
-      <c r="C105" s="93"/>
-      <c r="D105" s="110" t="s">
+      <c r="B105" s="89"/>
+      <c r="C105" s="90"/>
+      <c r="D105" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="E105" s="93"/>
+      <c r="E105" s="90"/>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="s">
         <v>39</v>
@@ -3811,8 +3814,8 @@
     </row>
     <row r="106" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="50"/>
-      <c r="B106" s="111"/>
-      <c r="C106" s="93"/>
+      <c r="B106" s="89"/>
+      <c r="C106" s="90"/>
       <c r="F106" s="53"/>
       <c r="G106" s="54"/>
       <c r="H106" s="53"/>
@@ -3823,8 +3826,8 @@
     </row>
     <row r="107" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="50"/>
-      <c r="B107" s="111"/>
-      <c r="C107" s="93"/>
+      <c r="B107" s="89"/>
+      <c r="C107" s="90"/>
       <c r="D107" s="55"/>
       <c r="E107" s="53"/>
       <c r="F107" s="53"/>
@@ -4792,12 +4795,24 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B100:C100"/>
     <mergeCell ref="D100:E100"/>
@@ -4809,24 +4824,12 @@
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D105:E105"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="F10:F15" xr:uid="{49EDF03A-7EFB-435C-A992-40D98DE85B41}">
@@ -4851,7 +4854,7 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -4869,59 +4872,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="110"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="110"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="102"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="102"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -4933,16 +4936,16 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="121" t="str">
+      <c r="B7" s="130" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="93"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -4954,15 +4957,15 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="93"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
@@ -4974,11 +4977,11 @@
       <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="123" t="s">
+      <c r="E10" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="93"/>
       <c r="H10" s="6" t="s">
         <v>45</v>
       </c>
@@ -4993,9 +4996,9 @@
       <c r="D11" s="14">
         <v>45190</v>
       </c>
-      <c r="E11" s="113"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="93"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5009,9 +5012,9 @@
         <f t="shared" ref="D12" si="0">C12+13</f>
         <v>45204</v>
       </c>
-      <c r="E12" s="113"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
+      <c r="E12" s="125"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5025,9 +5028,9 @@
       <c r="D13" s="14">
         <v>45225</v>
       </c>
-      <c r="E13" s="113"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="93"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5040,9 +5043,9 @@
       <c r="D14" s="14">
         <v>45246</v>
       </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5081,13 +5084,13 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
       <c r="H18" s="22" t="s">
         <v>47</v>
       </c>
@@ -5096,11 +5099,11 @@
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="116"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="101"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="25" t="s">
         <v>48</v>
       </c>
@@ -5110,11 +5113,11 @@
       <c r="B20" s="27">
         <v>0</v>
       </c>
-      <c r="C20" s="117"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="93"/>
       <c r="H20" s="28"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -5131,13 +5134,13 @@
       <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="119"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="120"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="116"/>
       <c r="H21" s="61" t="s">
         <v>50</v>
       </c>
@@ -5147,13 +5150,13 @@
       <c r="B22" s="27">
         <v>2</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="120"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="116"/>
       <c r="H22" s="61" t="s">
         <v>50</v>
       </c>
@@ -5162,13 +5165,13 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="120"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="116"/>
       <c r="H23" s="61" t="s">
         <v>50</v>
       </c>
@@ -5177,13 +5180,13 @@
       <c r="B24" s="27">
         <v>4</v>
       </c>
-      <c r="C24" s="124" t="s">
+      <c r="C24" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="125"/>
-      <c r="G24" s="126"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="121"/>
       <c r="H24" s="62" t="s">
         <v>58</v>
       </c>
@@ -5192,13 +5195,13 @@
       <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="127" t="s">
+      <c r="C25" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="128"/>
-      <c r="G25" s="129"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="118"/>
       <c r="H25" s="12" t="s">
         <v>54</v>
       </c>
@@ -5207,13 +5210,13 @@
       <c r="B26" s="27">
         <v>6</v>
       </c>
-      <c r="C26" s="127" t="s">
+      <c r="C26" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="129"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="118"/>
       <c r="H26" s="12" t="s">
         <v>54</v>
       </c>
@@ -5222,13 +5225,13 @@
       <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="119"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="120"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="116"/>
       <c r="H27" s="61" t="s">
         <v>50</v>
       </c>
@@ -5237,13 +5240,13 @@
       <c r="B28" s="27">
         <v>8</v>
       </c>
-      <c r="C28" s="124" t="s">
+      <c r="C28" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="126"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="120"/>
+      <c r="F28" s="120"/>
+      <c r="G28" s="121"/>
       <c r="H28" s="62" t="s">
         <v>58</v>
       </c>
@@ -5252,13 +5255,13 @@
       <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="118" t="s">
+      <c r="C29" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="120"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="115"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="116"/>
       <c r="H29" s="61" t="s">
         <v>58</v>
       </c>
@@ -5267,13 +5270,13 @@
       <c r="B30" s="27">
         <v>10</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
-      <c r="F30" s="131"/>
-      <c r="G30" s="132"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="124"/>
       <c r="H30" s="82" t="s">
         <v>54</v>
       </c>
@@ -5282,13 +5285,13 @@
       <c r="B31" s="9">
         <v>11</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="126"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="120"/>
+      <c r="G31" s="121"/>
       <c r="H31" s="62" t="s">
         <v>58</v>
       </c>
@@ -5297,13 +5300,13 @@
       <c r="B32" s="27">
         <v>12</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C32" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="119"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="119"/>
-      <c r="G32" s="120"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="116"/>
       <c r="H32" s="61" t="s">
         <v>50</v>
       </c>
@@ -5312,11 +5315,11 @@
       <c r="B33" s="9">
         <v>13</v>
       </c>
-      <c r="C33" s="127"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="128"/>
-      <c r="F33" s="128"/>
-      <c r="G33" s="129"/>
+      <c r="C33" s="113"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="118"/>
       <c r="H33" s="12" t="s">
         <v>54</v>
       </c>
@@ -5325,11 +5328,11 @@
       <c r="B34" s="27">
         <v>14</v>
       </c>
-      <c r="C34" s="127"/>
-      <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="128"/>
-      <c r="G34" s="129"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="118"/>
       <c r="H34" s="12" t="s">
         <v>54</v>
       </c>
@@ -5338,11 +5341,11 @@
       <c r="B35" s="9">
         <v>15</v>
       </c>
-      <c r="C35" s="127"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="129"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="118"/>
       <c r="H35" s="12" t="s">
         <v>54</v>
       </c>
@@ -5351,11 +5354,11 @@
       <c r="B36" s="27">
         <v>16</v>
       </c>
-      <c r="C36" s="127"/>
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="101"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="93"/>
       <c r="H36" s="12" t="s">
         <v>54</v>
       </c>
@@ -5364,11 +5367,11 @@
       <c r="B37" s="9">
         <v>17</v>
       </c>
-      <c r="C37" s="127"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="101"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="93"/>
       <c r="H37" s="12" t="s">
         <v>54</v>
       </c>
@@ -5377,11 +5380,11 @@
       <c r="B38" s="27">
         <v>18</v>
       </c>
-      <c r="C38" s="127"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="100"/>
-      <c r="G38" s="101"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="92"/>
+      <c r="E38" s="92"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="93"/>
       <c r="H38" s="12" t="s">
         <v>54</v>
       </c>
@@ -5390,11 +5393,11 @@
       <c r="B39" s="9">
         <v>19</v>
       </c>
-      <c r="C39" s="127"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="100"/>
-      <c r="G39" s="101"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="93"/>
       <c r="H39" s="12" t="s">
         <v>54</v>
       </c>
@@ -5403,11 +5406,11 @@
       <c r="B40" s="27">
         <v>20</v>
       </c>
-      <c r="C40" s="127"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="101"/>
+      <c r="C40" s="113"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="93"/>
       <c r="H40" s="12" t="s">
         <v>54</v>
       </c>
@@ -5416,11 +5419,11 @@
       <c r="B41" s="9">
         <v>21</v>
       </c>
-      <c r="C41" s="127"/>
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="101"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="93"/>
       <c r="H41" s="12" t="s">
         <v>54</v>
       </c>
@@ -5429,11 +5432,11 @@
       <c r="B42" s="27">
         <v>22</v>
       </c>
-      <c r="C42" s="127"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="100"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="101"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="93"/>
       <c r="H42" s="12" t="s">
         <v>54</v>
       </c>
@@ -5442,11 +5445,11 @@
       <c r="B43" s="9">
         <v>23</v>
       </c>
-      <c r="C43" s="127"/>
-      <c r="D43" s="100"/>
-      <c r="E43" s="100"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="101"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="93"/>
       <c r="H43" s="12" t="s">
         <v>54</v>
       </c>
@@ -5455,11 +5458,11 @@
       <c r="B44" s="27">
         <v>24</v>
       </c>
-      <c r="C44" s="127"/>
-      <c r="D44" s="100"/>
-      <c r="E44" s="100"/>
-      <c r="F44" s="100"/>
-      <c r="G44" s="101"/>
+      <c r="C44" s="113"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="93"/>
       <c r="H44" s="12" t="s">
         <v>54</v>
       </c>
@@ -5468,11 +5471,11 @@
       <c r="B45" s="9">
         <v>25</v>
       </c>
-      <c r="C45" s="127"/>
-      <c r="D45" s="100"/>
-      <c r="E45" s="100"/>
-      <c r="F45" s="100"/>
-      <c r="G45" s="101"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="93"/>
       <c r="H45" s="12" t="s">
         <v>54</v>
       </c>
@@ -5481,11 +5484,11 @@
       <c r="B46" s="27">
         <v>26</v>
       </c>
-      <c r="C46" s="127"/>
-      <c r="D46" s="100"/>
-      <c r="E46" s="100"/>
-      <c r="F46" s="100"/>
-      <c r="G46" s="101"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="92"/>
+      <c r="E46" s="92"/>
+      <c r="F46" s="92"/>
+      <c r="G46" s="93"/>
       <c r="H46" s="12" t="s">
         <v>54</v>
       </c>
@@ -5494,11 +5497,11 @@
       <c r="B47" s="9">
         <v>27</v>
       </c>
-      <c r="C47" s="127"/>
-      <c r="D47" s="100"/>
-      <c r="E47" s="100"/>
-      <c r="F47" s="100"/>
-      <c r="G47" s="101"/>
+      <c r="C47" s="113"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="92"/>
+      <c r="G47" s="93"/>
       <c r="H47" s="12" t="s">
         <v>54</v>
       </c>
@@ -5507,11 +5510,11 @@
       <c r="B48" s="27">
         <v>28</v>
       </c>
-      <c r="C48" s="127"/>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="101"/>
+      <c r="C48" s="113"/>
+      <c r="D48" s="92"/>
+      <c r="E48" s="92"/>
+      <c r="F48" s="92"/>
+      <c r="G48" s="93"/>
       <c r="H48" s="12" t="s">
         <v>54</v>
       </c>
@@ -5520,11 +5523,11 @@
       <c r="B49" s="9">
         <v>29</v>
       </c>
-      <c r="C49" s="127"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="92"/>
+      <c r="E49" s="92"/>
+      <c r="F49" s="92"/>
+      <c r="G49" s="93"/>
       <c r="H49" s="12" t="s">
         <v>54</v>
       </c>
@@ -5533,11 +5536,11 @@
       <c r="B50" s="27">
         <v>30</v>
       </c>
-      <c r="C50" s="127"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="100"/>
-      <c r="G50" s="101"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="92"/>
+      <c r="E50" s="92"/>
+      <c r="F50" s="92"/>
+      <c r="G50" s="93"/>
       <c r="H50" s="12" t="s">
         <v>54</v>
       </c>
@@ -5546,11 +5549,11 @@
       <c r="B51" s="9">
         <v>31</v>
       </c>
-      <c r="C51" s="127"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="101"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="92"/>
+      <c r="E51" s="92"/>
+      <c r="F51" s="92"/>
+      <c r="G51" s="93"/>
       <c r="H51" s="12" t="s">
         <v>54</v>
       </c>
@@ -5559,11 +5562,11 @@
       <c r="B52" s="27">
         <v>32</v>
       </c>
-      <c r="C52" s="127"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="100"/>
-      <c r="F52" s="100"/>
-      <c r="G52" s="101"/>
+      <c r="C52" s="113"/>
+      <c r="D52" s="92"/>
+      <c r="E52" s="92"/>
+      <c r="F52" s="92"/>
+      <c r="G52" s="93"/>
       <c r="H52" s="12" t="s">
         <v>54</v>
       </c>
@@ -5572,11 +5575,11 @@
       <c r="B53" s="9">
         <v>33</v>
       </c>
-      <c r="C53" s="127"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="100"/>
-      <c r="G53" s="101"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="92"/>
+      <c r="E53" s="92"/>
+      <c r="F53" s="92"/>
+      <c r="G53" s="93"/>
       <c r="H53" s="12" t="s">
         <v>54</v>
       </c>
@@ -5585,11 +5588,11 @@
       <c r="B54" s="27">
         <v>34</v>
       </c>
-      <c r="C54" s="127"/>
-      <c r="D54" s="100"/>
-      <c r="E54" s="100"/>
-      <c r="F54" s="100"/>
-      <c r="G54" s="101"/>
+      <c r="C54" s="113"/>
+      <c r="D54" s="92"/>
+      <c r="E54" s="92"/>
+      <c r="F54" s="92"/>
+      <c r="G54" s="93"/>
       <c r="H54" s="12" t="s">
         <v>54</v>
       </c>
@@ -5598,11 +5601,11 @@
       <c r="B55" s="9">
         <v>35</v>
       </c>
-      <c r="C55" s="127"/>
-      <c r="D55" s="100"/>
-      <c r="E55" s="100"/>
-      <c r="F55" s="100"/>
-      <c r="G55" s="101"/>
+      <c r="C55" s="113"/>
+      <c r="D55" s="92"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="92"/>
+      <c r="G55" s="93"/>
       <c r="H55" s="12" t="s">
         <v>54</v>
       </c>
@@ -5611,11 +5614,11 @@
       <c r="B56" s="27">
         <v>36</v>
       </c>
-      <c r="C56" s="127"/>
-      <c r="D56" s="100"/>
-      <c r="E56" s="100"/>
-      <c r="F56" s="100"/>
-      <c r="G56" s="101"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="92"/>
+      <c r="E56" s="92"/>
+      <c r="F56" s="92"/>
+      <c r="G56" s="93"/>
       <c r="H56" s="12" t="s">
         <v>54</v>
       </c>
@@ -5624,11 +5627,11 @@
       <c r="B57" s="9">
         <v>37</v>
       </c>
-      <c r="C57" s="127"/>
-      <c r="D57" s="100"/>
-      <c r="E57" s="100"/>
-      <c r="F57" s="100"/>
-      <c r="G57" s="101"/>
+      <c r="C57" s="113"/>
+      <c r="D57" s="92"/>
+      <c r="E57" s="92"/>
+      <c r="F57" s="92"/>
+      <c r="G57" s="93"/>
       <c r="H57" s="12" t="s">
         <v>54</v>
       </c>
@@ -5637,11 +5640,11 @@
       <c r="B58" s="27">
         <v>38</v>
       </c>
-      <c r="C58" s="127"/>
-      <c r="D58" s="100"/>
-      <c r="E58" s="100"/>
-      <c r="F58" s="100"/>
-      <c r="G58" s="101"/>
+      <c r="C58" s="113"/>
+      <c r="D58" s="92"/>
+      <c r="E58" s="92"/>
+      <c r="F58" s="92"/>
+      <c r="G58" s="93"/>
       <c r="H58" s="12" t="s">
         <v>54</v>
       </c>
@@ -5650,11 +5653,11 @@
       <c r="B59" s="9">
         <v>39</v>
       </c>
-      <c r="C59" s="127"/>
-      <c r="D59" s="100"/>
-      <c r="E59" s="100"/>
-      <c r="F59" s="100"/>
-      <c r="G59" s="101"/>
+      <c r="C59" s="113"/>
+      <c r="D59" s="92"/>
+      <c r="E59" s="92"/>
+      <c r="F59" s="92"/>
+      <c r="G59" s="93"/>
       <c r="H59" s="12" t="s">
         <v>54</v>
       </c>
@@ -5663,11 +5666,11 @@
       <c r="B60" s="27">
         <v>40</v>
       </c>
-      <c r="C60" s="127"/>
-      <c r="D60" s="100"/>
-      <c r="E60" s="100"/>
-      <c r="F60" s="100"/>
-      <c r="G60" s="101"/>
+      <c r="C60" s="113"/>
+      <c r="D60" s="92"/>
+      <c r="E60" s="92"/>
+      <c r="F60" s="92"/>
+      <c r="G60" s="93"/>
       <c r="H60" s="12" t="s">
         <v>54</v>
       </c>
@@ -5676,11 +5679,11 @@
       <c r="B61" s="9">
         <v>41</v>
       </c>
-      <c r="C61" s="127"/>
-      <c r="D61" s="100"/>
-      <c r="E61" s="100"/>
-      <c r="F61" s="100"/>
-      <c r="G61" s="101"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="92"/>
+      <c r="E61" s="92"/>
+      <c r="F61" s="92"/>
+      <c r="G61" s="93"/>
       <c r="H61" s="12" t="s">
         <v>54</v>
       </c>
@@ -5689,11 +5692,11 @@
       <c r="B62" s="27">
         <v>42</v>
       </c>
-      <c r="C62" s="127"/>
-      <c r="D62" s="100"/>
-      <c r="E62" s="100"/>
-      <c r="F62" s="100"/>
-      <c r="G62" s="101"/>
+      <c r="C62" s="113"/>
+      <c r="D62" s="92"/>
+      <c r="E62" s="92"/>
+      <c r="F62" s="92"/>
+      <c r="G62" s="93"/>
       <c r="H62" s="12" t="s">
         <v>54</v>
       </c>
@@ -5702,11 +5705,11 @@
       <c r="B63" s="9">
         <v>43</v>
       </c>
-      <c r="C63" s="127"/>
-      <c r="D63" s="100"/>
-      <c r="E63" s="100"/>
-      <c r="F63" s="100"/>
-      <c r="G63" s="101"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="93"/>
       <c r="H63" s="12" t="s">
         <v>54</v>
       </c>
@@ -5715,11 +5718,11 @@
       <c r="B64" s="27">
         <v>44</v>
       </c>
-      <c r="C64" s="127"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="101"/>
+      <c r="C64" s="113"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="92"/>
+      <c r="F64" s="92"/>
+      <c r="G64" s="93"/>
       <c r="H64" s="12" t="s">
         <v>54</v>
       </c>
@@ -5728,11 +5731,11 @@
       <c r="B65" s="9">
         <v>45</v>
       </c>
-      <c r="C65" s="127"/>
-      <c r="D65" s="100"/>
-      <c r="E65" s="100"/>
-      <c r="F65" s="100"/>
-      <c r="G65" s="101"/>
+      <c r="C65" s="113"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="92"/>
+      <c r="G65" s="93"/>
       <c r="H65" s="12" t="s">
         <v>54</v>
       </c>
@@ -5741,11 +5744,11 @@
       <c r="B66" s="27">
         <v>46</v>
       </c>
-      <c r="C66" s="127"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="101"/>
+      <c r="C66" s="113"/>
+      <c r="D66" s="92"/>
+      <c r="E66" s="92"/>
+      <c r="F66" s="92"/>
+      <c r="G66" s="93"/>
       <c r="H66" s="12" t="s">
         <v>54</v>
       </c>
@@ -5754,11 +5757,11 @@
       <c r="B67" s="9">
         <v>47</v>
       </c>
-      <c r="C67" s="127"/>
-      <c r="D67" s="100"/>
-      <c r="E67" s="100"/>
-      <c r="F67" s="100"/>
-      <c r="G67" s="101"/>
+      <c r="C67" s="113"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="92"/>
+      <c r="F67" s="92"/>
+      <c r="G67" s="93"/>
       <c r="H67" s="12" t="s">
         <v>54</v>
       </c>
@@ -5767,11 +5770,11 @@
       <c r="B68" s="27">
         <v>48</v>
       </c>
-      <c r="C68" s="127"/>
-      <c r="D68" s="100"/>
-      <c r="E68" s="100"/>
-      <c r="F68" s="100"/>
-      <c r="G68" s="101"/>
+      <c r="C68" s="113"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="93"/>
       <c r="H68" s="12" t="s">
         <v>54</v>
       </c>
@@ -5780,11 +5783,11 @@
       <c r="B69" s="9">
         <v>49</v>
       </c>
-      <c r="C69" s="127"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="100"/>
-      <c r="F69" s="100"/>
-      <c r="G69" s="101"/>
+      <c r="C69" s="113"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="92"/>
+      <c r="F69" s="92"/>
+      <c r="G69" s="93"/>
       <c r="H69" s="12" t="s">
         <v>54</v>
       </c>
@@ -5793,11 +5796,11 @@
       <c r="B70" s="27">
         <v>50</v>
       </c>
-      <c r="C70" s="127"/>
-      <c r="D70" s="100"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="100"/>
-      <c r="G70" s="101"/>
+      <c r="C70" s="113"/>
+      <c r="D70" s="92"/>
+      <c r="E70" s="92"/>
+      <c r="F70" s="92"/>
+      <c r="G70" s="93"/>
       <c r="H70" s="12" t="s">
         <v>54</v>
       </c>
@@ -5806,11 +5809,11 @@
       <c r="B71" s="9">
         <v>51</v>
       </c>
-      <c r="C71" s="127"/>
-      <c r="D71" s="100"/>
-      <c r="E71" s="100"/>
-      <c r="F71" s="100"/>
-      <c r="G71" s="101"/>
+      <c r="C71" s="113"/>
+      <c r="D71" s="92"/>
+      <c r="E71" s="92"/>
+      <c r="F71" s="92"/>
+      <c r="G71" s="93"/>
       <c r="H71" s="12" t="s">
         <v>54</v>
       </c>
@@ -5819,11 +5822,11 @@
       <c r="B72" s="27">
         <v>52</v>
       </c>
-      <c r="C72" s="127"/>
-      <c r="D72" s="100"/>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="101"/>
+      <c r="C72" s="113"/>
+      <c r="D72" s="92"/>
+      <c r="E72" s="92"/>
+      <c r="F72" s="92"/>
+      <c r="G72" s="93"/>
       <c r="H72" s="12" t="s">
         <v>54</v>
       </c>
@@ -5832,11 +5835,11 @@
       <c r="B73" s="9">
         <v>53</v>
       </c>
-      <c r="C73" s="127"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="101"/>
+      <c r="C73" s="113"/>
+      <c r="D73" s="92"/>
+      <c r="E73" s="92"/>
+      <c r="F73" s="92"/>
+      <c r="G73" s="93"/>
       <c r="H73" s="12" t="s">
         <v>54</v>
       </c>
@@ -5845,11 +5848,11 @@
       <c r="B74" s="27">
         <v>54</v>
       </c>
-      <c r="C74" s="127"/>
-      <c r="D74" s="100"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="101"/>
+      <c r="C74" s="113"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="92"/>
+      <c r="F74" s="92"/>
+      <c r="G74" s="93"/>
       <c r="H74" s="12" t="s">
         <v>54</v>
       </c>
@@ -5858,11 +5861,11 @@
       <c r="B75" s="9">
         <v>55</v>
       </c>
-      <c r="C75" s="127"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="101"/>
+      <c r="C75" s="113"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="92"/>
+      <c r="G75" s="93"/>
       <c r="H75" s="12" t="s">
         <v>54</v>
       </c>
@@ -5871,11 +5874,11 @@
       <c r="B76" s="27">
         <v>56</v>
       </c>
-      <c r="C76" s="127"/>
-      <c r="D76" s="100"/>
-      <c r="E76" s="100"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="101"/>
+      <c r="C76" s="113"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="93"/>
       <c r="H76" s="12" t="s">
         <v>54</v>
       </c>
@@ -5884,11 +5887,11 @@
       <c r="B77" s="9">
         <v>57</v>
       </c>
-      <c r="C77" s="127"/>
-      <c r="D77" s="100"/>
-      <c r="E77" s="100"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="101"/>
+      <c r="C77" s="113"/>
+      <c r="D77" s="92"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="92"/>
+      <c r="G77" s="93"/>
       <c r="H77" s="12" t="s">
         <v>54</v>
       </c>
@@ -5897,11 +5900,11 @@
       <c r="B78" s="27">
         <v>58</v>
       </c>
-      <c r="C78" s="127"/>
-      <c r="D78" s="100"/>
-      <c r="E78" s="100"/>
-      <c r="F78" s="100"/>
-      <c r="G78" s="101"/>
+      <c r="C78" s="113"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="92"/>
+      <c r="F78" s="92"/>
+      <c r="G78" s="93"/>
       <c r="H78" s="12" t="s">
         <v>54</v>
       </c>
@@ -5910,11 +5913,11 @@
       <c r="B79" s="9">
         <v>59</v>
       </c>
-      <c r="C79" s="127"/>
-      <c r="D79" s="100"/>
-      <c r="E79" s="100"/>
-      <c r="F79" s="100"/>
-      <c r="G79" s="101"/>
+      <c r="C79" s="113"/>
+      <c r="D79" s="92"/>
+      <c r="E79" s="92"/>
+      <c r="F79" s="92"/>
+      <c r="G79" s="93"/>
       <c r="H79" s="12" t="s">
         <v>54</v>
       </c>
@@ -5923,11 +5926,11 @@
       <c r="B80" s="27">
         <v>60</v>
       </c>
-      <c r="C80" s="127"/>
-      <c r="D80" s="100"/>
-      <c r="E80" s="100"/>
-      <c r="F80" s="100"/>
-      <c r="G80" s="101"/>
+      <c r="C80" s="113"/>
+      <c r="D80" s="92"/>
+      <c r="E80" s="92"/>
+      <c r="F80" s="92"/>
+      <c r="G80" s="93"/>
       <c r="H80" s="12" t="s">
         <v>54</v>
       </c>
@@ -5936,11 +5939,11 @@
       <c r="B81" s="9">
         <v>61</v>
       </c>
-      <c r="C81" s="127"/>
-      <c r="D81" s="100"/>
-      <c r="E81" s="100"/>
-      <c r="F81" s="100"/>
-      <c r="G81" s="101"/>
+      <c r="C81" s="113"/>
+      <c r="D81" s="92"/>
+      <c r="E81" s="92"/>
+      <c r="F81" s="92"/>
+      <c r="G81" s="93"/>
       <c r="H81" s="12" t="s">
         <v>54</v>
       </c>
@@ -5949,11 +5952,11 @@
       <c r="B82" s="27">
         <v>62</v>
       </c>
-      <c r="C82" s="127"/>
-      <c r="D82" s="100"/>
-      <c r="E82" s="100"/>
-      <c r="F82" s="100"/>
-      <c r="G82" s="101"/>
+      <c r="C82" s="113"/>
+      <c r="D82" s="92"/>
+      <c r="E82" s="92"/>
+      <c r="F82" s="92"/>
+      <c r="G82" s="93"/>
       <c r="H82" s="12" t="s">
         <v>54</v>
       </c>
@@ -5962,11 +5965,11 @@
       <c r="B83" s="9">
         <v>63</v>
       </c>
-      <c r="C83" s="127"/>
-      <c r="D83" s="100"/>
-      <c r="E83" s="100"/>
-      <c r="F83" s="100"/>
-      <c r="G83" s="101"/>
+      <c r="C83" s="113"/>
+      <c r="D83" s="92"/>
+      <c r="E83" s="92"/>
+      <c r="F83" s="92"/>
+      <c r="G83" s="93"/>
       <c r="H83" s="12" t="s">
         <v>54</v>
       </c>
@@ -5975,11 +5978,11 @@
       <c r="B84" s="27">
         <v>64</v>
       </c>
-      <c r="C84" s="127"/>
-      <c r="D84" s="100"/>
-      <c r="E84" s="100"/>
-      <c r="F84" s="100"/>
-      <c r="G84" s="101"/>
+      <c r="C84" s="113"/>
+      <c r="D84" s="92"/>
+      <c r="E84" s="92"/>
+      <c r="F84" s="92"/>
+      <c r="G84" s="93"/>
       <c r="H84" s="12" t="s">
         <v>54</v>
       </c>
@@ -5988,11 +5991,11 @@
       <c r="B85" s="9">
         <v>65</v>
       </c>
-      <c r="C85" s="127"/>
-      <c r="D85" s="100"/>
-      <c r="E85" s="100"/>
-      <c r="F85" s="100"/>
-      <c r="G85" s="101"/>
+      <c r="C85" s="113"/>
+      <c r="D85" s="92"/>
+      <c r="E85" s="92"/>
+      <c r="F85" s="92"/>
+      <c r="G85" s="93"/>
       <c r="H85" s="12" t="s">
         <v>54</v>
       </c>
@@ -6001,11 +6004,11 @@
       <c r="B86" s="27">
         <v>66</v>
       </c>
-      <c r="C86" s="127"/>
-      <c r="D86" s="100"/>
-      <c r="E86" s="100"/>
-      <c r="F86" s="100"/>
-      <c r="G86" s="101"/>
+      <c r="C86" s="113"/>
+      <c r="D86" s="92"/>
+      <c r="E86" s="92"/>
+      <c r="F86" s="92"/>
+      <c r="G86" s="93"/>
       <c r="H86" s="12" t="s">
         <v>54</v>
       </c>
@@ -6014,11 +6017,11 @@
       <c r="B87" s="9">
         <v>67</v>
       </c>
-      <c r="C87" s="127"/>
-      <c r="D87" s="100"/>
-      <c r="E87" s="100"/>
-      <c r="F87" s="100"/>
-      <c r="G87" s="101"/>
+      <c r="C87" s="113"/>
+      <c r="D87" s="92"/>
+      <c r="E87" s="92"/>
+      <c r="F87" s="92"/>
+      <c r="G87" s="93"/>
       <c r="H87" s="12" t="s">
         <v>54</v>
       </c>
@@ -6027,11 +6030,11 @@
       <c r="B88" s="27">
         <v>68</v>
       </c>
-      <c r="C88" s="127"/>
-      <c r="D88" s="100"/>
-      <c r="E88" s="100"/>
-      <c r="F88" s="100"/>
-      <c r="G88" s="101"/>
+      <c r="C88" s="113"/>
+      <c r="D88" s="92"/>
+      <c r="E88" s="92"/>
+      <c r="F88" s="92"/>
+      <c r="G88" s="93"/>
       <c r="H88" s="12" t="s">
         <v>54</v>
       </c>
@@ -6040,11 +6043,11 @@
       <c r="B89" s="9">
         <v>69</v>
       </c>
-      <c r="C89" s="127"/>
-      <c r="D89" s="100"/>
-      <c r="E89" s="100"/>
-      <c r="F89" s="100"/>
-      <c r="G89" s="101"/>
+      <c r="C89" s="113"/>
+      <c r="D89" s="92"/>
+      <c r="E89" s="92"/>
+      <c r="F89" s="92"/>
+      <c r="G89" s="93"/>
       <c r="H89" s="12" t="s">
         <v>54</v>
       </c>
@@ -6053,11 +6056,11 @@
       <c r="B90" s="27">
         <v>70</v>
       </c>
-      <c r="C90" s="127"/>
-      <c r="D90" s="100"/>
-      <c r="E90" s="100"/>
-      <c r="F90" s="100"/>
-      <c r="G90" s="101"/>
+      <c r="C90" s="113"/>
+      <c r="D90" s="92"/>
+      <c r="E90" s="92"/>
+      <c r="F90" s="92"/>
+      <c r="G90" s="93"/>
       <c r="H90" s="12" t="s">
         <v>54</v>
       </c>
@@ -6066,11 +6069,11 @@
       <c r="B91" s="9">
         <v>71</v>
       </c>
-      <c r="C91" s="127"/>
-      <c r="D91" s="100"/>
-      <c r="E91" s="100"/>
-      <c r="F91" s="100"/>
-      <c r="G91" s="101"/>
+      <c r="C91" s="113"/>
+      <c r="D91" s="92"/>
+      <c r="E91" s="92"/>
+      <c r="F91" s="92"/>
+      <c r="G91" s="93"/>
       <c r="H91" s="12" t="s">
         <v>54</v>
       </c>
@@ -6079,11 +6082,11 @@
       <c r="B92" s="27">
         <v>72</v>
       </c>
-      <c r="C92" s="127"/>
-      <c r="D92" s="100"/>
-      <c r="E92" s="100"/>
-      <c r="F92" s="100"/>
-      <c r="G92" s="101"/>
+      <c r="C92" s="113"/>
+      <c r="D92" s="92"/>
+      <c r="E92" s="92"/>
+      <c r="F92" s="92"/>
+      <c r="G92" s="93"/>
       <c r="H92" s="12" t="s">
         <v>54</v>
       </c>
@@ -6092,11 +6095,11 @@
       <c r="B93" s="9">
         <v>73</v>
       </c>
-      <c r="C93" s="127"/>
-      <c r="D93" s="100"/>
-      <c r="E93" s="100"/>
-      <c r="F93" s="100"/>
-      <c r="G93" s="101"/>
+      <c r="C93" s="113"/>
+      <c r="D93" s="92"/>
+      <c r="E93" s="92"/>
+      <c r="F93" s="92"/>
+      <c r="G93" s="93"/>
       <c r="H93" s="12" t="s">
         <v>54</v>
       </c>
@@ -6105,11 +6108,11 @@
       <c r="B94" s="27">
         <v>74</v>
       </c>
-      <c r="C94" s="127"/>
-      <c r="D94" s="100"/>
-      <c r="E94" s="100"/>
-      <c r="F94" s="100"/>
-      <c r="G94" s="101"/>
+      <c r="C94" s="113"/>
+      <c r="D94" s="92"/>
+      <c r="E94" s="92"/>
+      <c r="F94" s="92"/>
+      <c r="G94" s="93"/>
       <c r="H94" s="12" t="s">
         <v>54</v>
       </c>
@@ -6118,11 +6121,11 @@
       <c r="B95" s="9">
         <v>75</v>
       </c>
-      <c r="C95" s="127"/>
-      <c r="D95" s="100"/>
-      <c r="E95" s="100"/>
-      <c r="F95" s="100"/>
-      <c r="G95" s="101"/>
+      <c r="C95" s="113"/>
+      <c r="D95" s="92"/>
+      <c r="E95" s="92"/>
+      <c r="F95" s="92"/>
+      <c r="G95" s="93"/>
       <c r="H95" s="12" t="s">
         <v>54</v>
       </c>
@@ -6131,11 +6134,11 @@
       <c r="B96" s="27">
         <v>76</v>
       </c>
-      <c r="C96" s="127"/>
-      <c r="D96" s="100"/>
-      <c r="E96" s="100"/>
-      <c r="F96" s="100"/>
-      <c r="G96" s="101"/>
+      <c r="C96" s="113"/>
+      <c r="D96" s="92"/>
+      <c r="E96" s="92"/>
+      <c r="F96" s="92"/>
+      <c r="G96" s="93"/>
       <c r="H96" s="12" t="s">
         <v>54</v>
       </c>
@@ -6144,11 +6147,11 @@
       <c r="B97" s="9">
         <v>77</v>
       </c>
-      <c r="C97" s="127"/>
-      <c r="D97" s="100"/>
-      <c r="E97" s="100"/>
-      <c r="F97" s="100"/>
-      <c r="G97" s="101"/>
+      <c r="C97" s="113"/>
+      <c r="D97" s="92"/>
+      <c r="E97" s="92"/>
+      <c r="F97" s="92"/>
+      <c r="G97" s="93"/>
       <c r="H97" s="12" t="s">
         <v>54</v>
       </c>
@@ -6157,11 +6160,11 @@
       <c r="B98" s="27">
         <v>78</v>
       </c>
-      <c r="C98" s="127"/>
-      <c r="D98" s="100"/>
-      <c r="E98" s="100"/>
-      <c r="F98" s="100"/>
-      <c r="G98" s="101"/>
+      <c r="C98" s="113"/>
+      <c r="D98" s="92"/>
+      <c r="E98" s="92"/>
+      <c r="F98" s="92"/>
+      <c r="G98" s="93"/>
       <c r="H98" s="12" t="s">
         <v>54</v>
       </c>
@@ -6170,11 +6173,11 @@
       <c r="B99" s="9">
         <v>79</v>
       </c>
-      <c r="C99" s="127"/>
-      <c r="D99" s="100"/>
-      <c r="E99" s="100"/>
-      <c r="F99" s="100"/>
-      <c r="G99" s="101"/>
+      <c r="C99" s="113"/>
+      <c r="D99" s="92"/>
+      <c r="E99" s="92"/>
+      <c r="F99" s="92"/>
+      <c r="G99" s="93"/>
       <c r="H99" s="12" t="s">
         <v>54</v>
       </c>
@@ -6183,11 +6186,11 @@
       <c r="B100" s="27">
         <v>80</v>
       </c>
-      <c r="C100" s="127"/>
-      <c r="D100" s="100"/>
-      <c r="E100" s="100"/>
-      <c r="F100" s="100"/>
-      <c r="G100" s="101"/>
+      <c r="C100" s="113"/>
+      <c r="D100" s="92"/>
+      <c r="E100" s="92"/>
+      <c r="F100" s="92"/>
+      <c r="G100" s="93"/>
       <c r="H100" s="12" t="s">
         <v>54</v>
       </c>
@@ -6196,11 +6199,11 @@
       <c r="B101" s="9">
         <v>81</v>
       </c>
-      <c r="C101" s="127"/>
-      <c r="D101" s="100"/>
-      <c r="E101" s="100"/>
-      <c r="F101" s="100"/>
-      <c r="G101" s="101"/>
+      <c r="C101" s="113"/>
+      <c r="D101" s="92"/>
+      <c r="E101" s="92"/>
+      <c r="F101" s="92"/>
+      <c r="G101" s="93"/>
       <c r="H101" s="12" t="s">
         <v>54</v>
       </c>
@@ -6209,11 +6212,11 @@
       <c r="B102" s="27">
         <v>82</v>
       </c>
-      <c r="C102" s="127"/>
-      <c r="D102" s="100"/>
-      <c r="E102" s="100"/>
-      <c r="F102" s="100"/>
-      <c r="G102" s="101"/>
+      <c r="C102" s="113"/>
+      <c r="D102" s="92"/>
+      <c r="E102" s="92"/>
+      <c r="F102" s="92"/>
+      <c r="G102" s="93"/>
       <c r="H102" s="12" t="s">
         <v>54</v>
       </c>
@@ -6222,11 +6225,11 @@
       <c r="B103" s="9">
         <v>83</v>
       </c>
-      <c r="C103" s="127"/>
-      <c r="D103" s="100"/>
-      <c r="E103" s="100"/>
-      <c r="F103" s="100"/>
-      <c r="G103" s="101"/>
+      <c r="C103" s="113"/>
+      <c r="D103" s="92"/>
+      <c r="E103" s="92"/>
+      <c r="F103" s="92"/>
+      <c r="G103" s="93"/>
       <c r="H103" s="12" t="s">
         <v>54</v>
       </c>
@@ -6235,11 +6238,11 @@
       <c r="B104" s="27">
         <v>84</v>
       </c>
-      <c r="C104" s="127"/>
-      <c r="D104" s="100"/>
-      <c r="E104" s="100"/>
-      <c r="F104" s="100"/>
-      <c r="G104" s="101"/>
+      <c r="C104" s="113"/>
+      <c r="D104" s="92"/>
+      <c r="E104" s="92"/>
+      <c r="F104" s="92"/>
+      <c r="G104" s="93"/>
       <c r="H104" s="12" t="s">
         <v>54</v>
       </c>
@@ -6248,11 +6251,11 @@
       <c r="B105" s="9">
         <v>85</v>
       </c>
-      <c r="C105" s="127"/>
-      <c r="D105" s="100"/>
-      <c r="E105" s="100"/>
-      <c r="F105" s="100"/>
-      <c r="G105" s="101"/>
+      <c r="C105" s="113"/>
+      <c r="D105" s="92"/>
+      <c r="E105" s="92"/>
+      <c r="F105" s="92"/>
+      <c r="G105" s="93"/>
       <c r="H105" s="12" t="s">
         <v>54</v>
       </c>
@@ -6261,11 +6264,11 @@
       <c r="B106" s="27">
         <v>86</v>
       </c>
-      <c r="C106" s="127"/>
-      <c r="D106" s="100"/>
-      <c r="E106" s="100"/>
-      <c r="F106" s="100"/>
-      <c r="G106" s="101"/>
+      <c r="C106" s="113"/>
+      <c r="D106" s="92"/>
+      <c r="E106" s="92"/>
+      <c r="F106" s="92"/>
+      <c r="G106" s="93"/>
       <c r="H106" s="12" t="s">
         <v>54</v>
       </c>
@@ -6274,11 +6277,11 @@
       <c r="B107" s="9">
         <v>87</v>
       </c>
-      <c r="C107" s="127"/>
-      <c r="D107" s="100"/>
-      <c r="E107" s="100"/>
-      <c r="F107" s="100"/>
-      <c r="G107" s="101"/>
+      <c r="C107" s="113"/>
+      <c r="D107" s="92"/>
+      <c r="E107" s="92"/>
+      <c r="F107" s="92"/>
+      <c r="G107" s="93"/>
       <c r="H107" s="12" t="s">
         <v>54</v>
       </c>
@@ -6287,11 +6290,11 @@
       <c r="B108" s="27">
         <v>88</v>
       </c>
-      <c r="C108" s="127"/>
-      <c r="D108" s="100"/>
-      <c r="E108" s="100"/>
-      <c r="F108" s="100"/>
-      <c r="G108" s="101"/>
+      <c r="C108" s="113"/>
+      <c r="D108" s="92"/>
+      <c r="E108" s="92"/>
+      <c r="F108" s="92"/>
+      <c r="G108" s="93"/>
       <c r="H108" s="12" t="s">
         <v>54</v>
       </c>
@@ -6300,11 +6303,11 @@
       <c r="B109" s="9">
         <v>89</v>
       </c>
-      <c r="C109" s="127"/>
-      <c r="D109" s="100"/>
-      <c r="E109" s="100"/>
-      <c r="F109" s="100"/>
-      <c r="G109" s="101"/>
+      <c r="C109" s="113"/>
+      <c r="D109" s="92"/>
+      <c r="E109" s="92"/>
+      <c r="F109" s="92"/>
+      <c r="G109" s="93"/>
       <c r="H109" s="12" t="s">
         <v>54</v>
       </c>
@@ -6313,11 +6316,11 @@
       <c r="B110" s="27">
         <v>90</v>
       </c>
-      <c r="C110" s="127"/>
-      <c r="D110" s="100"/>
-      <c r="E110" s="100"/>
-      <c r="F110" s="100"/>
-      <c r="G110" s="101"/>
+      <c r="C110" s="113"/>
+      <c r="D110" s="92"/>
+      <c r="E110" s="92"/>
+      <c r="F110" s="92"/>
+      <c r="G110" s="93"/>
       <c r="H110" s="12" t="s">
         <v>54</v>
       </c>
@@ -6326,11 +6329,11 @@
       <c r="B111" s="9">
         <v>91</v>
       </c>
-      <c r="C111" s="127"/>
-      <c r="D111" s="100"/>
-      <c r="E111" s="100"/>
-      <c r="F111" s="100"/>
-      <c r="G111" s="101"/>
+      <c r="C111" s="113"/>
+      <c r="D111" s="92"/>
+      <c r="E111" s="92"/>
+      <c r="F111" s="92"/>
+      <c r="G111" s="93"/>
       <c r="H111" s="12" t="s">
         <v>54</v>
       </c>
@@ -6339,11 +6342,11 @@
       <c r="B112" s="27">
         <v>92</v>
       </c>
-      <c r="C112" s="127"/>
-      <c r="D112" s="100"/>
-      <c r="E112" s="100"/>
-      <c r="F112" s="100"/>
-      <c r="G112" s="101"/>
+      <c r="C112" s="113"/>
+      <c r="D112" s="92"/>
+      <c r="E112" s="92"/>
+      <c r="F112" s="92"/>
+      <c r="G112" s="93"/>
       <c r="H112" s="12" t="s">
         <v>54</v>
       </c>
@@ -6352,11 +6355,11 @@
       <c r="B113" s="9">
         <v>93</v>
       </c>
-      <c r="C113" s="127"/>
-      <c r="D113" s="100"/>
-      <c r="E113" s="100"/>
-      <c r="F113" s="100"/>
-      <c r="G113" s="101"/>
+      <c r="C113" s="113"/>
+      <c r="D113" s="92"/>
+      <c r="E113" s="92"/>
+      <c r="F113" s="92"/>
+      <c r="G113" s="93"/>
       <c r="H113" s="12" t="s">
         <v>54</v>
       </c>
@@ -6365,11 +6368,11 @@
       <c r="B114" s="27">
         <v>94</v>
       </c>
-      <c r="C114" s="127"/>
-      <c r="D114" s="100"/>
-      <c r="E114" s="100"/>
-      <c r="F114" s="100"/>
-      <c r="G114" s="101"/>
+      <c r="C114" s="113"/>
+      <c r="D114" s="92"/>
+      <c r="E114" s="92"/>
+      <c r="F114" s="92"/>
+      <c r="G114" s="93"/>
       <c r="H114" s="12" t="s">
         <v>54</v>
       </c>
@@ -6378,11 +6381,11 @@
       <c r="B115" s="9">
         <v>95</v>
       </c>
-      <c r="C115" s="127"/>
-      <c r="D115" s="100"/>
-      <c r="E115" s="100"/>
-      <c r="F115" s="100"/>
-      <c r="G115" s="101"/>
+      <c r="C115" s="113"/>
+      <c r="D115" s="92"/>
+      <c r="E115" s="92"/>
+      <c r="F115" s="92"/>
+      <c r="G115" s="93"/>
       <c r="H115" s="12" t="s">
         <v>54</v>
       </c>
@@ -6391,11 +6394,11 @@
       <c r="B116" s="27">
         <v>96</v>
       </c>
-      <c r="C116" s="127"/>
-      <c r="D116" s="100"/>
-      <c r="E116" s="100"/>
-      <c r="F116" s="100"/>
-      <c r="G116" s="101"/>
+      <c r="C116" s="113"/>
+      <c r="D116" s="92"/>
+      <c r="E116" s="92"/>
+      <c r="F116" s="92"/>
+      <c r="G116" s="93"/>
       <c r="H116" s="12" t="s">
         <v>54</v>
       </c>
@@ -6404,11 +6407,11 @@
       <c r="B117" s="9">
         <v>97</v>
       </c>
-      <c r="C117" s="127"/>
-      <c r="D117" s="100"/>
-      <c r="E117" s="100"/>
-      <c r="F117" s="100"/>
-      <c r="G117" s="101"/>
+      <c r="C117" s="113"/>
+      <c r="D117" s="92"/>
+      <c r="E117" s="92"/>
+      <c r="F117" s="92"/>
+      <c r="G117" s="93"/>
       <c r="H117" s="12" t="s">
         <v>54</v>
       </c>
@@ -6417,11 +6420,11 @@
       <c r="B118" s="27">
         <v>98</v>
       </c>
-      <c r="C118" s="127"/>
-      <c r="D118" s="100"/>
-      <c r="E118" s="100"/>
-      <c r="F118" s="100"/>
-      <c r="G118" s="101"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="92"/>
+      <c r="E118" s="92"/>
+      <c r="F118" s="92"/>
+      <c r="G118" s="93"/>
       <c r="H118" s="12" t="s">
         <v>54</v>
       </c>
@@ -6430,11 +6433,11 @@
       <c r="B119" s="9">
         <v>99</v>
       </c>
-      <c r="C119" s="127"/>
-      <c r="D119" s="100"/>
-      <c r="E119" s="100"/>
-      <c r="F119" s="100"/>
-      <c r="G119" s="101"/>
+      <c r="C119" s="113"/>
+      <c r="D119" s="92"/>
+      <c r="E119" s="92"/>
+      <c r="F119" s="92"/>
+      <c r="G119" s="93"/>
       <c r="H119" s="12" t="s">
         <v>54</v>
       </c>
@@ -6443,11 +6446,11 @@
       <c r="B120" s="27">
         <v>100</v>
       </c>
-      <c r="C120" s="127"/>
-      <c r="D120" s="100"/>
-      <c r="E120" s="100"/>
-      <c r="F120" s="100"/>
-      <c r="G120" s="101"/>
+      <c r="C120" s="113"/>
+      <c r="D120" s="92"/>
+      <c r="E120" s="92"/>
+      <c r="F120" s="92"/>
+      <c r="G120" s="93"/>
       <c r="H120" s="12" t="s">
         <v>54</v>
       </c>
@@ -8126,53 +8129,50 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
@@ -8197,50 +8197,53 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C95:G95"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H120" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8290,85 +8293,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
       <c r="K1" s="2">
         <f>Requisitos!C11</f>
         <v>45170</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="110"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K65" si="0">K1+1</f>
         <v>45171</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45172</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45173</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45174</v>
@@ -8382,18 +8385,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="str">
+      <c r="B7" s="103" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45176</v>
@@ -8410,13 +8413,13 @@
       <c r="B9" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -9790,13 +9793,13 @@
       <c r="B63" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="100"/>
-      <c r="D63" s="100"/>
-      <c r="E63" s="100"/>
-      <c r="F63" s="100"/>
-      <c r="G63" s="100"/>
-      <c r="H63" s="100"/>
-      <c r="I63" s="101"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="92"/>
+      <c r="H63" s="92"/>
+      <c r="I63" s="93"/>
       <c r="K63" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -9806,11 +9809,11 @@
       <c r="B64" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="100"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="101"/>
+      <c r="C64" s="92"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="92"/>
+      <c r="F64" s="92"/>
+      <c r="G64" s="93"/>
       <c r="H64" s="7" t="s">
         <v>99</v>
       </c>
@@ -9827,11 +9830,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="100"/>
-      <c r="D65" s="100"/>
-      <c r="E65" s="100"/>
-      <c r="F65" s="100"/>
-      <c r="G65" s="101"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="92"/>
+      <c r="G65" s="93"/>
       <c r="H65" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B10,H$11:H$60)</f>
         <v>0</v>
@@ -9850,11 +9853,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="101"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="92"/>
+      <c r="E66" s="92"/>
+      <c r="F66" s="92"/>
+      <c r="G66" s="93"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -9873,11 +9876,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="100"/>
-      <c r="D67" s="100"/>
-      <c r="E67" s="100"/>
-      <c r="F67" s="100"/>
-      <c r="G67" s="101"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="92"/>
+      <c r="F67" s="92"/>
+      <c r="G67" s="93"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -9896,11 +9899,11 @@
         <f>'Dados do Projeto'!B13</f>
         <v>Maria Eduarda Amaral</v>
       </c>
-      <c r="C68" s="100"/>
-      <c r="D68" s="100"/>
-      <c r="E68" s="100"/>
-      <c r="F68" s="100"/>
-      <c r="G68" s="101"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="93"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -9919,11 +9922,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C69" s="100"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="100"/>
-      <c r="F69" s="100"/>
-      <c r="G69" s="101"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="92"/>
+      <c r="F69" s="92"/>
+      <c r="G69" s="93"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -9942,11 +9945,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C70" s="100"/>
-      <c r="D70" s="100"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="100"/>
-      <c r="G70" s="101"/>
+      <c r="C70" s="92"/>
+      <c r="D70" s="92"/>
+      <c r="E70" s="92"/>
+      <c r="F70" s="92"/>
+      <c r="G70" s="93"/>
       <c r="H70" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -11095,85 +11098,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
       <c r="K1" s="2">
         <f>Requisitos!C12</f>
         <v>45191</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="110"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45192</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45193</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45194</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45195</v>
@@ -11187,18 +11190,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="str">
+      <c r="B7" s="103" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45197</v>
@@ -11215,13 +11218,13 @@
       <c r="B9" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -12590,23 +12593,23 @@
       <c r="B72" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="100"/>
-      <c r="D72" s="100"/>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="100"/>
-      <c r="H72" s="100"/>
-      <c r="I72" s="101"/>
+      <c r="C72" s="92"/>
+      <c r="D72" s="92"/>
+      <c r="E72" s="92"/>
+      <c r="F72" s="92"/>
+      <c r="G72" s="92"/>
+      <c r="H72" s="92"/>
+      <c r="I72" s="93"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="100"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="101"/>
+      <c r="C73" s="92"/>
+      <c r="D73" s="92"/>
+      <c r="E73" s="92"/>
+      <c r="F73" s="92"/>
+      <c r="G73" s="93"/>
       <c r="H73" s="7" t="s">
         <v>99</v>
       </c>
@@ -12619,11 +12622,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="100"/>
-      <c r="D74" s="100"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="101"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="92"/>
+      <c r="F74" s="92"/>
+      <c r="G74" s="93"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -12638,11 +12641,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="100"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="101"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="92"/>
+      <c r="G75" s="93"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -12657,11 +12660,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="100"/>
-      <c r="D76" s="100"/>
-      <c r="E76" s="100"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="101"/>
+      <c r="C76" s="92"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="93"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -12676,11 +12679,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="100"/>
-      <c r="D77" s="100"/>
-      <c r="E77" s="100"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="101"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="92"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="92"/>
+      <c r="G77" s="93"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -12695,11 +12698,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="100"/>
-      <c r="D78" s="100"/>
-      <c r="E78" s="100"/>
-      <c r="F78" s="100"/>
-      <c r="G78" s="101"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="92"/>
+      <c r="F78" s="92"/>
+      <c r="G78" s="93"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -13950,85 +13953,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
       <c r="K1" s="2">
         <f>Requisitos!C13</f>
         <v>45205</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="110"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K22" si="0">K1+1</f>
         <v>45206</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45207</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45208</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45209</v>
@@ -14042,18 +14045,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="str">
+      <c r="B7" s="103" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45211</v>
@@ -14070,13 +14073,13 @@
       <c r="B9" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -15417,23 +15420,23 @@
       <c r="B73" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="100"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="100"/>
-      <c r="H73" s="100"/>
-      <c r="I73" s="101"/>
+      <c r="C73" s="92"/>
+      <c r="D73" s="92"/>
+      <c r="E73" s="92"/>
+      <c r="F73" s="92"/>
+      <c r="G73" s="92"/>
+      <c r="H73" s="92"/>
+      <c r="I73" s="93"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="100"/>
-      <c r="D74" s="100"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="101"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="92"/>
+      <c r="F74" s="92"/>
+      <c r="G74" s="93"/>
       <c r="H74" s="7" t="s">
         <v>99</v>
       </c>
@@ -15446,11 +15449,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C75" s="100"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="101"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="92"/>
+      <c r="G75" s="93"/>
       <c r="H75" s="33">
         <f>SUMIF($F$11:$F$61,'Dados do Projeto'!$B10,H$11:H$61)</f>
         <v>0</v>
@@ -15465,11 +15468,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C76" s="100"/>
-      <c r="D76" s="100"/>
-      <c r="E76" s="100"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="101"/>
+      <c r="C76" s="92"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="93"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B11,H$11:H$61)</f>
         <v>0</v>
@@ -15484,11 +15487,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C77" s="100"/>
-      <c r="D77" s="100"/>
-      <c r="E77" s="100"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="101"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="92"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="92"/>
+      <c r="G77" s="93"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B12,H$11:H$61)</f>
         <v>0</v>
@@ -15503,11 +15506,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C78" s="100"/>
-      <c r="D78" s="100"/>
-      <c r="E78" s="100"/>
-      <c r="F78" s="100"/>
-      <c r="G78" s="101"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="92"/>
+      <c r="F78" s="92"/>
+      <c r="G78" s="93"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B14,H$11:H$61)</f>
         <v>0</v>
@@ -15522,11 +15525,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C79" s="100"/>
-      <c r="D79" s="100"/>
-      <c r="E79" s="100"/>
-      <c r="F79" s="100"/>
-      <c r="G79" s="101"/>
+      <c r="C79" s="92"/>
+      <c r="D79" s="92"/>
+      <c r="E79" s="92"/>
+      <c r="F79" s="92"/>
+      <c r="G79" s="93"/>
       <c r="H79" s="33">
         <f>SUMIF(F$11:F$61,'Dados do Projeto'!B15,H$11:H$61)</f>
         <v>0</v>
@@ -16550,12 +16553,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B79:G79"/>
     <mergeCell ref="B9:I9"/>
@@ -16564,6 +16561,12 @@
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
     <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C70">
     <cfRule type="expression" dxfId="71" priority="31">
@@ -16701,9 +16704,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16724,85 +16727,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
       <c r="K1" s="2">
         <f>Requisitos!C14</f>
         <v>45226</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="110"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>45227</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45228</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45229</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45230</v>
@@ -16816,18 +16819,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="str">
+      <c r="B7" s="103" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45232</v>
@@ -16844,13 +16847,13 @@
       <c r="B9" s="134" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="57" t="s">
         <v>66</v>
       </c>
@@ -16942,7 +16945,7 @@
         <v>45239</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>172</v>
@@ -16979,7 +16982,7 @@
         <v>133</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>37</v>
@@ -17010,7 +17013,7 @@
         <v>172</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="41" t="s">
         <v>37</v>
@@ -18214,23 +18217,23 @@
       <c r="B72" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="100"/>
-      <c r="D72" s="100"/>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="100"/>
-      <c r="H72" s="100"/>
-      <c r="I72" s="101"/>
+      <c r="C72" s="92"/>
+      <c r="D72" s="92"/>
+      <c r="E72" s="92"/>
+      <c r="F72" s="92"/>
+      <c r="G72" s="92"/>
+      <c r="H72" s="92"/>
+      <c r="I72" s="93"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="100"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="101"/>
+      <c r="C73" s="92"/>
+      <c r="D73" s="92"/>
+      <c r="E73" s="92"/>
+      <c r="F73" s="92"/>
+      <c r="G73" s="93"/>
       <c r="H73" s="7" t="s">
         <v>99</v>
       </c>
@@ -18243,11 +18246,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C74" s="100"/>
-      <c r="D74" s="100"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="101"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="92"/>
+      <c r="F74" s="92"/>
+      <c r="G74" s="93"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -18262,11 +18265,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C75" s="100"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="101"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="92"/>
+      <c r="G75" s="93"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -18281,11 +18284,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C76" s="100"/>
-      <c r="D76" s="100"/>
-      <c r="E76" s="100"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="101"/>
+      <c r="C76" s="92"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="93"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -18300,11 +18303,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C77" s="100"/>
-      <c r="D77" s="100"/>
-      <c r="E77" s="100"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="101"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="92"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="92"/>
+      <c r="G77" s="93"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -18319,11 +18322,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C78" s="100"/>
-      <c r="D78" s="100"/>
-      <c r="E78" s="100"/>
-      <c r="F78" s="100"/>
-      <c r="G78" s="101"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="92"/>
+      <c r="F78" s="92"/>
+      <c r="G78" s="93"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -19347,12 +19350,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B9:I9"/>
@@ -19361,6 +19358,12 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F33:F69">
     <cfRule type="expression" dxfId="51" priority="25">
@@ -19489,85 +19492,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
       <c r="K1" s="2">
         <f>Requisitos!C15</f>
         <v>45247</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="110"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>45248</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>45249</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>45250</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>45251</v>
@@ -19580,18 +19583,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="99" t="str">
+      <c r="B7" s="103" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Fábrica do Saber</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45253</v>
@@ -19607,13 +19610,13 @@
       <c r="B9" s="134" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="58" t="s">
         <v>66</v>
       </c>
@@ -20577,23 +20580,23 @@
       <c r="B63" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="100"/>
-      <c r="D63" s="100"/>
-      <c r="E63" s="100"/>
-      <c r="F63" s="100"/>
-      <c r="G63" s="100"/>
-      <c r="H63" s="100"/>
-      <c r="I63" s="101"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="92"/>
+      <c r="H63" s="92"/>
+      <c r="I63" s="93"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="100"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="101"/>
+      <c r="C64" s="92"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="92"/>
+      <c r="F64" s="92"/>
+      <c r="G64" s="93"/>
       <c r="H64" s="7" t="s">
         <v>99</v>
       </c>
@@ -20606,11 +20609,11 @@
         <f>'Dados do Projeto'!B10</f>
         <v>Guilherme Lage</v>
       </c>
-      <c r="C65" s="100"/>
-      <c r="D65" s="100"/>
-      <c r="E65" s="100"/>
-      <c r="F65" s="100"/>
-      <c r="G65" s="101"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="92"/>
+      <c r="G65" s="93"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -20625,11 +20628,11 @@
         <f>'Dados do Projeto'!B11</f>
         <v>João Gabriel Perez</v>
       </c>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="101"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="92"/>
+      <c r="E66" s="92"/>
+      <c r="F66" s="92"/>
+      <c r="G66" s="93"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -20644,11 +20647,11 @@
         <f>'Dados do Projeto'!B12</f>
         <v>Lucas Soares</v>
       </c>
-      <c r="C67" s="100"/>
-      <c r="D67" s="100"/>
-      <c r="E67" s="100"/>
-      <c r="F67" s="100"/>
-      <c r="G67" s="101"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="92"/>
+      <c r="F67" s="92"/>
+      <c r="G67" s="93"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -20663,11 +20666,11 @@
         <f>'Dados do Projeto'!B14</f>
         <v>Marlene Moraes</v>
       </c>
-      <c r="C68" s="100"/>
-      <c r="D68" s="100"/>
-      <c r="E68" s="100"/>
-      <c r="F68" s="100"/>
-      <c r="G68" s="101"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="93"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -20682,11 +20685,11 @@
         <f>'Dados do Projeto'!B15</f>
         <v>Vitor Stahlberg</v>
       </c>
-      <c r="C69" s="100"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="100"/>
-      <c r="F69" s="100"/>
-      <c r="G69" s="101"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="92"/>
+      <c r="F69" s="92"/>
+      <c r="G69" s="93"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B15,H$11:H$60)</f>
         <v>0</v>
@@ -21649,12 +21652,6 @@
   </sheetData>
   <autoFilter ref="B10:J60" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B9:I9"/>
@@ -21663,6 +21660,12 @@
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F17">
     <cfRule type="containsBlanks" dxfId="37" priority="1">

</xml_diff>